<commit_message>
Correción de error en el tiempo de tareas y mejora visual de la organizaciñon de la Semana 1
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -534,7 +534,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,6 +544,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,29 +617,11 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -620,15 +632,193 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel ET3" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -904,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,724 +1115,1263 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="2"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:11" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9">
         <v>30</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>1</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" s="8"/>
+      <c r="H4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="10">
         <v>1</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="8">
+        <f>SUMIF(E4:E28,1,D4:D28)</f>
         <v>270</v>
       </c>
+      <c r="K4">
+        <f>SUMIF(E4:E28,1,F4:F28)</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9">
         <v>20</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>3</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="H5" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="11">
         <v>2</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="8">
+        <f>SUMIF(E4:E28,2,D4:D28)</f>
         <v>270</v>
       </c>
+      <c r="K5">
+        <f>SUMIF(E4:E28,2,F4:F28)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
         <v>20</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="H6" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="12">
         <v>3</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="8">
+        <f>SUMIF(E4:E28,3,D4:D28)</f>
         <v>270</v>
       </c>
+      <c r="K6">
+        <f>SUMIF(E4:E28,3,F4:F28)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9">
         <v>20</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>4</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="H7" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="13">
         <v>4</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="8">
+        <f>SUMIF(E4:E28,4,D4:D28)</f>
         <v>270</v>
       </c>
+      <c r="K7">
+        <f>SUMIF(E4:E28,4,F4:F28)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9">
+        <v>30</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="14">
+        <v>5</v>
+      </c>
+      <c r="J8" s="8">
+        <f>SUMIF(E4:E28,5,D4:D28)</f>
+        <v>270</v>
+      </c>
+      <c r="K8">
+        <f>SUMIF(E4:E28,5,F4:F28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="10">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9">
+        <v>90</v>
+      </c>
+      <c r="E9" s="9">
+        <v>5</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9">
+        <v>90</v>
+      </c>
+      <c r="E10" s="9">
+        <v>4</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>8</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9">
+        <v>90</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>9</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9">
+        <v>90</v>
+      </c>
+      <c r="E12" s="9">
+        <v>3</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>10</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9">
+        <v>60</v>
+      </c>
+      <c r="E13" s="9">
         <v>2</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="H8" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="I8" s="1">
+      <c r="B14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9">
+        <v>60</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>12</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9">
+        <v>30</v>
+      </c>
+      <c r="E15" s="9">
+        <v>3</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>13</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9">
+        <v>30</v>
+      </c>
+      <c r="E16" s="9">
         <v>5</v>
       </c>
-      <c r="J8" s="1">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>6</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="F16" s="9"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>14</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9">
+        <v>30</v>
+      </c>
+      <c r="E17" s="9">
+        <v>4</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>15</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9">
+        <v>30</v>
+      </c>
+      <c r="E18" s="9">
+        <v>5</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>16</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9">
+        <v>30</v>
+      </c>
+      <c r="E19" s="9">
+        <v>4</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>17</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9">
+        <v>100</v>
+      </c>
+      <c r="E20" s="9">
+        <v>5</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>18</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9">
+        <v>120</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>19</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9">
+        <v>90</v>
+      </c>
+      <c r="E22" s="9">
+        <v>3</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10">
-        <v>90</v>
-      </c>
-      <c r="E9" s="10">
+      <c r="B23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9">
+        <v>30</v>
+      </c>
+      <c r="E23" s="9">
+        <v>2</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>21</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9">
+        <v>40</v>
+      </c>
+      <c r="E24" s="9">
+        <v>3</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>22</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9">
+        <v>20</v>
+      </c>
+      <c r="E25" s="9">
         <v>5</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>7</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10">
-        <v>90</v>
-      </c>
-      <c r="E10" s="10">
+      <c r="F25" s="9"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>23</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9">
+        <v>100</v>
+      </c>
+      <c r="E26" s="9">
         <v>4</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>8</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10">
-        <v>90</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="F26" s="9"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>24</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9">
+        <v>70</v>
+      </c>
+      <c r="E27" s="9">
+        <v>2</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>25</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9">
+        <v>30</v>
+      </c>
+      <c r="E28" s="9">
         <v>1</v>
       </c>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>9</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10">
-        <v>90</v>
-      </c>
-      <c r="E12" s="10">
-        <v>3</v>
-      </c>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>10</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10">
-        <v>60</v>
-      </c>
-      <c r="E13" s="10">
-        <v>2</v>
-      </c>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>11</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10">
-        <v>60</v>
-      </c>
-      <c r="E14" s="10">
-        <v>2</v>
-      </c>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>12</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10">
-        <v>30</v>
-      </c>
-      <c r="E15" s="10">
-        <v>3</v>
-      </c>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>13</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10">
-        <v>30</v>
-      </c>
-      <c r="E16" s="10">
-        <v>5</v>
-      </c>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>14</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10">
-        <v>30</v>
-      </c>
-      <c r="E17" s="10">
-        <v>4</v>
-      </c>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>15</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10">
-        <v>30</v>
-      </c>
-      <c r="E18" s="10">
-        <v>5</v>
-      </c>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>16</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10">
-        <v>30</v>
-      </c>
-      <c r="E19" s="10">
-        <v>4</v>
-      </c>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>17</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10">
-        <v>100</v>
-      </c>
-      <c r="E20" s="10">
-        <v>5</v>
-      </c>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10">
-        <v>120</v>
-      </c>
-      <c r="E21" s="10">
-        <v>1</v>
-      </c>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>19</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10">
-        <v>90</v>
-      </c>
-      <c r="E22" s="10">
-        <v>3</v>
-      </c>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>20</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10">
-        <v>30</v>
-      </c>
-      <c r="E23" s="10">
-        <v>2</v>
-      </c>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
-        <v>21</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10">
-        <v>40</v>
-      </c>
-      <c r="E24" s="10">
-        <v>3</v>
-      </c>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
-        <v>22</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10">
-        <v>20</v>
-      </c>
-      <c r="E25" s="10">
-        <v>5</v>
-      </c>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>23</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10">
-        <v>100</v>
-      </c>
-      <c r="E26" s="10">
-        <v>4</v>
-      </c>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>24</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10">
-        <v>70</v>
-      </c>
-      <c r="E27" s="10">
-        <v>2</v>
-      </c>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
-        <v>25</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10">
-        <v>30</v>
-      </c>
-      <c r="E28" s="10">
-        <v>1</v>
-      </c>
       <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="3" t="s">
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="8" t="s">
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C36" s="9"/>
-      <c r="D36" s="12">
+      <c r="D36" s="9">
         <v>120</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="8" t="s">
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="9"/>
-      <c r="D37" s="12">
+      <c r="D37" s="9">
         <v>30</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="8" t="s">
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="9"/>
-      <c r="D38" s="12">
+      <c r="D38" s="9">
         <v>30</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="8" t="s">
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="16" t="s">
         <v>43</v>
       </c>
       <c r="C39" s="9"/>
-      <c r="D39" s="12">
+      <c r="D39" s="9">
         <v>30</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="8" t="s">
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="9"/>
-      <c r="D40" s="10">
+      <c r="D40" s="9">
         <v>100</v>
       </c>
-      <c r="E40" s="10"/>
+      <c r="E40" s="9"/>
       <c r="F40" s="9"/>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="B41" s="8" t="s">
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="9"/>
-      <c r="D41" s="10">
+      <c r="D41" s="9">
         <v>120</v>
       </c>
-      <c r="E41" s="10"/>
+      <c r="E41" s="9"/>
       <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="8" t="s">
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+    </row>
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
+      <c r="J66" s="8"/>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8"/>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="8"/>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="8"/>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8"/>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8"/>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="8"/>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8"/>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:F2"/>
   </mergeCells>
+  <conditionalFormatting sqref="E4:E28">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:I8">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Retoque de borrador para controlador grupo
Base de controlador grupo
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ET3_GIT\EXCEL TAREAS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
@@ -19,7 +14,7 @@
     <definedName name="Estados">Hoja2!$A$1:$A$6</definedName>
     <definedName name="EstadosVálidos">Hoja2!$A$1:$A$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -554,7 +549,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -840,7 +835,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -875,7 +870,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1052,7 +1047,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1062,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1205,7 +1200,9 @@
       <c r="F5" s="7">
         <v>3</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="7">
+        <v>20</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="9" t="s">
         <v>7</v>
@@ -1263,7 +1260,7 @@
       </c>
       <c r="L6" s="15">
         <f>SUMIF(F4:F28,3,G4:G28)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M6" s="15">
         <f t="shared" si="0"/>
@@ -1271,7 +1268,7 @@
       </c>
       <c r="N6" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
@@ -1393,7 +1390,7 @@
       </c>
       <c r="L9" s="16">
         <f>SUM(L4:L8)</f>
-        <v>215</v>
+        <v>255</v>
       </c>
       <c r="M9" s="16">
         <f>SUM(M4:M8)</f>
@@ -1401,7 +1398,7 @@
       </c>
       <c r="N9" s="16">
         <f>SUM(N4:N8)</f>
-        <v>4637.5</v>
+        <v>5637.5</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>59</v>
@@ -1472,7 +1469,9 @@
       <c r="F12" s="7">
         <v>3</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7">
+        <v>20</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>

</xml_diff>

<commit_message>
He añadido una tarea de la sección extra a mi trabajo semanal
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -744,16 +744,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -761,7 +761,322 @@
     <cellStyle name="Excel ET3" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="51">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1082,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,24 +1418,24 @@
   <sheetData>
     <row r="1" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:15" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1165,7 +1480,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="19">
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -1209,7 +1524,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="19">
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -1253,7 +1568,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+      <c r="A6" s="19">
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -1297,7 +1612,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="19">
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -1343,7 +1658,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21">
+      <c r="A8" s="19">
         <v>5</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -1389,7 +1704,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21">
+      <c r="A9" s="19">
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -1421,7 +1736,7 @@
         <f>SUM(M4:M8)</f>
         <v>337.5</v>
       </c>
-      <c r="N9" s="20">
+      <c r="N9" s="18">
         <f>SUM(N4:N8)</f>
         <v>0</v>
       </c>
@@ -1430,7 +1745,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="19">
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -1455,7 +1770,7 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:15" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="19">
         <v>8</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -1482,7 +1797,7 @@
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="19">
         <v>9</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -1507,7 +1822,7 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+      <c r="A13" s="19">
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -1534,7 +1849,7 @@
       <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="19">
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1561,7 +1876,7 @@
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15" s="19">
         <v>12</v>
       </c>
       <c r="B15" s="13" t="s">
@@ -1584,7 +1899,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+      <c r="A16" s="19">
         <v>13</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -1607,7 +1922,7 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="19">
         <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -1630,7 +1945,7 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="19">
         <v>15</v>
       </c>
       <c r="B18" s="13" t="s">
@@ -1653,7 +1968,7 @@
       <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="19">
         <v>16</v>
       </c>
       <c r="B19" s="13" t="s">
@@ -1676,7 +1991,7 @@
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="19">
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -1699,7 +2014,7 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="19">
         <v>18</v>
       </c>
       <c r="B21" s="13" t="s">
@@ -1726,7 +2041,7 @@
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="21">
+      <c r="A22" s="19">
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
@@ -1749,7 +2064,7 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+      <c r="A23" s="19">
         <v>20</v>
       </c>
       <c r="B23" s="13" t="s">
@@ -1772,7 +2087,7 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="21">
+      <c r="A24" s="19">
         <v>21</v>
       </c>
       <c r="B24" s="13" t="s">
@@ -1795,7 +2110,7 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="21">
+      <c r="A25" s="19">
         <v>22</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -1818,7 +2133,7 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="21">
+      <c r="A26" s="19">
         <v>23</v>
       </c>
       <c r="B26" s="13" t="s">
@@ -1843,7 +2158,7 @@
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="21">
+      <c r="A27" s="19">
         <v>24</v>
       </c>
       <c r="B27" s="13" t="s">
@@ -1870,7 +2185,7 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="21">
+      <c r="A28" s="19">
         <v>25</v>
       </c>
       <c r="B28" s="12" t="s">
@@ -2007,7 +2322,9 @@
       <c r="E36" s="6">
         <v>120</v>
       </c>
-      <c r="F36" s="6"/>
+      <c r="F36" s="6">
+        <v>1</v>
+      </c>
       <c r="G36" s="6"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -2598,24 +2915,41 @@
     <mergeCell ref="B1:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F28">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:J8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36:F42">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Creado el controlador ACCIONES_CONTROLLER.php dónde falta controlar la accion de borrar ya que afecta otras tablas. Actualizado el excel dónde figura esta tarea con un estado paralizado hasta resolver el problema comentado anteriormente
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -1398,7 +1398,7 @@
   <dimension ref="A1:O80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,7 +2325,9 @@
       <c r="F36" s="6">
         <v>1</v>
       </c>
-      <c r="G36" s="6"/>
+      <c r="G36" s="6">
+        <v>30</v>
+      </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>

</xml_diff>

<commit_message>
Creados los controladores de FUNCIONALIDADES Y FUNCIONALIDAD_ACCION, esta tarea está paralizada hasta que abordemos una solución al borrado de tuplas de una tabla respecto a otras. Modificación de la tarea en el excel
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
   <si>
     <t>Tareas principales</t>
   </si>
@@ -558,6 +558,9 @@
   </si>
   <si>
     <t>Falta solucionar como se trataría el borrado de un acción</t>
+  </si>
+  <si>
+    <t>Falta solucionar como se trataría el borrado de una funcionalidad y de funcionalidad_accion</t>
   </si>
 </sst>
 </file>
@@ -764,35 +767,7 @@
     <cellStyle name="Excel ET3" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -825,258 +800,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1400,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1238,7 @@
       </c>
       <c r="L4" s="14">
         <f>SUMIF(F4:F42,1,G4:G42)</f>
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="M4" s="14">
         <f>K4/60*15</f>
@@ -1523,7 +1246,7 @@
       </c>
       <c r="N4" s="15" t="str">
         <f>FIXED(L4/60*25,2)</f>
-        <v>64,58</v>
+        <v>83,33</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1733,7 +1456,7 @@
       </c>
       <c r="L9" s="15">
         <f>SUM(L4:L8)</f>
-        <v>380</v>
+        <v>425</v>
       </c>
       <c r="M9" s="15">
         <f>SUM(M4:M8)</f>
@@ -2414,22 +2137,26 @@
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
     </row>
-    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="E41" s="6">
         <v>120</v>
       </c>
       <c r="F41" s="6">
         <v>1</v>
       </c>
-      <c r="G41" s="6"/>
+      <c r="G41" s="6">
+        <v>45</v>
+      </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
@@ -2924,41 +2651,41 @@
     <mergeCell ref="B1:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F28">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:J8">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36:F42">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Añadidas nuevas tareas extra. Mejora de la tabla de seguimiento del proyecyo
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
   <si>
     <t>Tareas principales</t>
   </si>
@@ -459,15 +459,6 @@
     </r>
   </si>
   <si>
-    <t>Revisión de la tarea 25</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 26</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 35</t>
-  </si>
-  <si>
     <t>nº Tarea</t>
   </si>
   <si>
@@ -506,9 +497,6 @@
     <t>Coste por hora planificado</t>
   </si>
   <si>
-    <t>Coste por hora empleado</t>
-  </si>
-  <si>
     <t>Semana 1(Del 20/10/2017 hasta 26/10/2017)</t>
   </si>
   <si>
@@ -561,6 +549,137 @@
   </si>
   <si>
     <t>Falta solucionar como se trataría el borrado de una funcionalidad y de funcionalidad_accion</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 23</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 24</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 36</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 40</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 41</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 42</t>
+  </si>
+  <si>
+    <t>Implementar el control sobre los usuarios que pertenecen a uno o varios grupos y tienen unos ciertos permisos.</t>
+  </si>
+  <si>
+    <t>Finalizada/Corregida</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tratamiento del borrado entre las tablas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> USUARIO, USUARIO_GRUPO y GRUPO.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tratamiento del borrado entre las tablas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> PERMISO y GRUPO.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tratamiento del borrado entre las tabla</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s: PERMISO y FUNCIONALIDAD_ACCION</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tratamiento del borrado entre las tablas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION.</t>
+    </r>
+  </si>
+  <si>
+    <t>Coste por hora planificado utilizado</t>
+  </si>
+  <si>
+    <t>Beneficio real</t>
+  </si>
+  <si>
+    <t>Beneficio planificado</t>
+  </si>
+  <si>
+    <t>Ingresos reales</t>
+  </si>
+  <si>
+    <t>Ingresos planificados</t>
   </si>
 </sst>
 </file>
@@ -683,9 +802,7 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color theme="8" tint="-0.24994659260841701"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -699,7 +816,7 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -739,18 +856,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -762,6 +873,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel ET3" xfId="1"/>
@@ -771,7 +885,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -785,21 +913,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1121,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O80"/>
+  <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,34 +1252,36 @@
     <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="32.28515625" customWidth="1"/>
     <col min="12" max="12" width="29.5703125" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="13" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" customWidth="1"/>
+    <col min="17" max="17" width="21.28515625" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
-      <c r="B1" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-    </row>
-    <row r="3" spans="1:15" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:19" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -1174,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
@@ -1193,27 +1309,39 @@
         <v>5</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+        <v>80</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6">
@@ -1244,20 +1372,36 @@
         <f>K4/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N4" s="15" t="str">
-        <f>FIXED(L4/60*25,2)</f>
-        <v>83,33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
+      <c r="N4" s="14">
+        <f>K4/60*25</f>
+        <v>112.5</v>
+      </c>
+      <c r="O4" s="14">
+        <f>N4-M4</f>
+        <v>45</v>
+      </c>
+      <c r="P4" s="14">
+        <f>L4/60*15</f>
+        <v>50</v>
+      </c>
+      <c r="Q4" s="14">
+        <f>L4/60*25</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="R4" s="14">
+        <f>Q4-P4</f>
+        <v>33.333333333333343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6">
@@ -1285,23 +1429,39 @@
         <v>120</v>
       </c>
       <c r="M5" s="14">
-        <f t="shared" ref="M5:M8" si="0">K5/60*15</f>
+        <f>K5/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N5" s="15" t="str">
-        <f t="shared" ref="N5:N8" si="1">FIXED(L5/60*25,2)</f>
-        <v>50,00</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="N5" s="14">
+        <f>K5/60*25</f>
+        <v>112.5</v>
+      </c>
+      <c r="O5" s="14">
+        <f t="shared" ref="O5:O8" si="0">N5-M5</f>
+        <v>45</v>
+      </c>
+      <c r="P5" s="14">
+        <f t="shared" ref="P5:P8" si="1">L5/60*15</f>
+        <v>30</v>
+      </c>
+      <c r="Q5" s="14">
+        <f>L5/60*25</f>
+        <v>50</v>
+      </c>
+      <c r="R5" s="14">
+        <f t="shared" ref="R5:R8" si="2">Q5-P5</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6">
@@ -1329,26 +1489,42 @@
         <v>40</v>
       </c>
       <c r="M6" s="14">
+        <f>K6/60*15</f>
+        <v>67.5</v>
+      </c>
+      <c r="N6" s="14">
+        <f>K6/60*25</f>
+        <v>112.5</v>
+      </c>
+      <c r="O6" s="14">
         <f t="shared" si="0"/>
-        <v>67.5</v>
-      </c>
-      <c r="N6" s="15" t="str">
+        <v>45</v>
+      </c>
+      <c r="P6" s="14">
         <f t="shared" si="1"/>
-        <v>16,67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="14">
+        <f>L6/60*25</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="R6" s="14">
+        <f t="shared" si="2"/>
+        <v>6.6666666666666643</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E7" s="6">
         <v>20</v>
@@ -1370,31 +1546,47 @@
         <f>SUMIF(F4:F28,4,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="14">
         <f>SUMIF(F4:F42,4,G4:G42)</f>
         <v>65</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="14">
+        <f>K7/60*15</f>
+        <v>67.5</v>
+      </c>
+      <c r="N7" s="14">
+        <f>K7/60*25</f>
+        <v>112.5</v>
+      </c>
+      <c r="O7" s="14">
         <f t="shared" si="0"/>
-        <v>67.5</v>
-      </c>
-      <c r="N7" s="15" t="str">
+        <v>45</v>
+      </c>
+      <c r="P7" s="14">
         <f t="shared" si="1"/>
-        <v>27,08</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+        <v>16.25</v>
+      </c>
+      <c r="Q7" s="14">
+        <f>L7/60*25</f>
+        <v>27.083333333333332</v>
+      </c>
+      <c r="R7" s="14">
+        <f t="shared" si="2"/>
+        <v>10.833333333333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
         <v>5</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E8" s="6">
         <v>30</v>
@@ -1412,32 +1604,48 @@
       <c r="J8" s="11">
         <v>5</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="15">
         <f>SUMIF(F4:F28,5,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <f>SUMIF(F4:F42,5,G4:G42)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="16">
+        <f>K8/60*15</f>
+        <v>67.5</v>
+      </c>
+      <c r="N8" s="14">
+        <f>K8/60*25</f>
+        <v>112.5</v>
+      </c>
+      <c r="O8" s="14">
         <f t="shared" si="0"/>
-        <v>67.5</v>
-      </c>
-      <c r="N8" s="15" t="str">
+        <v>45</v>
+      </c>
+      <c r="P8" s="14">
         <f t="shared" si="1"/>
-        <v>0,00</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
+        <f>L8/60*25</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6">
@@ -1454,31 +1662,47 @@
         <f>SUM(K4:K8)</f>
         <v>1350</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="14">
         <f>SUM(L4:L8)</f>
         <v>425</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="14">
         <f>SUM(M4:M8)</f>
         <v>337.5</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="20">
         <f>SUM(N4:N8)</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+        <v>562.5</v>
+      </c>
+      <c r="O9" s="20">
+        <f>SUM(O4:O8)</f>
+        <v>225</v>
+      </c>
+      <c r="P9" s="20">
+        <f>SUM(P4:P8)</f>
+        <v>106.25</v>
+      </c>
+      <c r="Q9" s="20" t="str">
+        <f>FIXED(SUM(Q5:Q8))</f>
+        <v>93,75</v>
+      </c>
+      <c r="R9" s="20" t="str">
+        <f>FIXED(SUM(R5:R8))</f>
+        <v>37,50</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6">
@@ -1495,8 +1719,8 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:15" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+    <row r="11" spans="1:19" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
         <v>8</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -1506,7 +1730,7 @@
         <v>54</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E11" s="6">
         <v>90</v>
@@ -1522,15 +1746,15 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
         <v>9</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6">
@@ -1547,18 +1771,18 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+    <row r="13" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="E13" s="6">
         <v>60</v>
@@ -1574,18 +1798,18 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+    <row r="14" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="E14" s="6">
         <v>60</v>
@@ -1601,15 +1825,15 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
         <v>12</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
@@ -1624,15 +1848,15 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
         <v>13</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6">
@@ -1648,14 +1872,14 @@
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
+      <c r="A17" s="17">
         <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6">
@@ -1671,14 +1895,14 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="17">
         <v>15</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6">
@@ -1694,14 +1918,14 @@
       <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="17">
         <v>16</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6">
@@ -1717,14 +1941,14 @@
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+      <c r="A20" s="17">
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6">
@@ -1740,7 +1964,7 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
+      <c r="A21" s="17">
         <v>18</v>
       </c>
       <c r="B21" s="13" t="s">
@@ -1750,7 +1974,7 @@
         <v>54</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E21" s="6">
         <v>120</v>
@@ -1767,14 +1991,14 @@
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
+      <c r="A22" s="17">
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6">
@@ -1790,14 +2014,14 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
+      <c r="A23" s="17">
         <v>20</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6">
@@ -1813,14 +2037,14 @@
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
+      <c r="A24" s="17">
         <v>21</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6">
@@ -1836,14 +2060,14 @@
       <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="19">
+      <c r="A25" s="17">
         <v>22</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6">
@@ -1859,14 +2083,14 @@
       <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
+      <c r="A26" s="17">
         <v>23</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6">
@@ -1884,17 +2108,17 @@
       <c r="K26" s="5"/>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="19">
+      <c r="A27" s="17">
         <v>24</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E27" s="6">
         <v>70</v>
@@ -1911,14 +2135,14 @@
       <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="17">
         <v>25</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6">
@@ -2020,7 +2244,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>13</v>
@@ -2042,10 +2266,10 @@
         <v>38</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E36" s="6">
         <v>120</v>
@@ -2064,10 +2288,10 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="13" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6">
@@ -2083,10 +2307,10 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="13" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6">
@@ -2102,10 +2326,10 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="13" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6">
@@ -2124,7 +2348,7 @@
         <v>33</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6">
@@ -2143,10 +2367,10 @@
         <v>32</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E41" s="6">
         <v>120</v>
@@ -2168,7 +2392,7 @@
         <v>31</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6">
@@ -2183,10 +2407,16 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
+      <c r="B43" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="E43" s="6">
+        <v>30</v>
+      </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="5"/>
@@ -2196,10 +2426,16 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
+      <c r="B44" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="E44" s="6">
+        <v>30</v>
+      </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="5"/>
@@ -2209,10 +2445,16 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
+      <c r="B45" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
+      <c r="E45" s="6">
+        <v>30</v>
+      </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="5"/>
@@ -2222,10 +2464,16 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
+      <c r="B46" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+      <c r="E46" s="6">
+        <v>90</v>
+      </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="5"/>
@@ -2235,10 +2483,16 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
+      <c r="B47" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+      <c r="E47" s="6">
+        <v>90</v>
+      </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="5"/>
@@ -2248,10 +2502,16 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
+      <c r="B48" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="E48" s="6">
+        <v>90</v>
+      </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="5"/>
@@ -2261,10 +2521,16 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
+      <c r="B49" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
+      <c r="E49" s="6">
+        <v>90</v>
+      </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="5"/>
@@ -2272,12 +2538,18 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
+      <c r="B50" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="E50" s="6">
+        <v>120</v>
+      </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="5"/>
@@ -2673,24 +2945,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36:F42">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>1</formula>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>2</formula>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>4</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>4</formula>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>5</formula>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C28 C36:C42">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C28 C36:C50">
       <formula1>Estados</formula1>
     </dataValidation>
   </dataValidations>
@@ -2704,7 +2976,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:A6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2714,32 +2986,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel actualizado otra vez por Brais Santos
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
   <si>
     <t>Semana 1(Del 20/10/2017 hasta 26/10/2017)</t>
   </si>
@@ -81,26 +81,7 @@
     <t>Beneficio real</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Organizar y asignar tareas:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> Semana 1</t>
-    </r>
+    <t>Organizar y asignar tareas: Semana 1</t>
   </si>
   <si>
     <t>Finalizada</t>
@@ -109,26 +90,7 @@
     <t>Miguel Ferreiro Díaz</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestión de usuarios</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>:  Modificar controladores para adaptarlo al nuevo modelo de datos</t>
-    </r>
+    <t>Gestión de usuarios:  Modificar controladores para adaptarlo al nuevo modelo de datos</t>
   </si>
   <si>
     <t>Sin empezar</t>
@@ -137,26 +99,7 @@
     <t>Alejandro Vila Cid</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestión de usuario</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>s:  Modificar modelos para adaptarlo al nuevo modelo de datos</t>
-    </r>
+    <t>Gestión de usuarios:  Modificar modelos para adaptarlo al nuevo modelo de datos</t>
   </si>
   <si>
     <t>Pendiente de correción</t>
@@ -168,26 +111,7 @@
     <t>Jonatan Couto Riádigos</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestión de usuarios</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>:  Modificar vistas para adapartalo al nuevo modelo de datos</t>
-    </r>
+    <t>Gestión de usuarios:  Modificar vistas para adapartalo al nuevo modelo de datos</t>
   </si>
   <si>
     <t>Paralizada</t>
@@ -208,148 +132,34 @@
     <t>Brais Rodríguez Martínez</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestion de grupos de usuario: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear modelo de datos para  la tabla USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-    </r>
+    <t>Gestion de grupos de usuario: Crear modelo de datos para  la tabla USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestion de grupos de usuario: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear modelo de datos para  la tabla GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-    </r>
+    <t>Gestion de grupos de usuario: Crear modelo de datos para  la tabla GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
     <t>Nombre del modelo:GRUPO_MODEL</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestión de grupos de usuario: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear controlador para manejar las acciones asociadas a la gestión de los USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-    </r>
+    <t>Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de los USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
     <t>Creado el controladro: USUARIOS_GRUPO_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de USUARIO_GRUPO no se puede editar al ser claves.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestión de grupos de usuario: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear controlador para manejar las acciones asociadas a la gestión de GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestión de grupos de usuario: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear vistas  las posibles acciones sobre la tabla USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-    </r>
+    <t>Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t>Gestión de grupos de usuario: Crear vistas  las posibles acciones sobre la tabla USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
     <t>Creadas las vistas de acuerdo a los atributos actuales</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestión de grupos de usuario:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> Crear vistas para las posibles acciones sobre la tabla GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-    </r>
+    <t>Gestión de grupos de usuario: Crear vistas para las posibles acciones sobre la tabla GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
     <t>Revisión de la tarea 9</t>
@@ -367,73 +177,16 @@
     <t>Revisión de la tarea 13</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestion de permisos de usuario: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear modelo de datos para la tabla PERMISOS. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestion de permisos de usuario:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear controlador de datos para la tabla PERMISOS.  (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-    </r>
+    <t>Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t>Gestion de permisos de usuario:  Crear controlador de datos para la tabla PERMISOS.  (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
     <t>Creado el controladro: PERMISOS_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de  PERMISOS no se puede editar al ser claves.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestion de permisos de usuario: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> Crear vistas para las posibles acciones sobre la tabla PERMISOS.   (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-    </r>
+    <t>Gestion de permisos de usuario:  Crear vistas para las posibles acciones sobre la tabla PERMISOS.   (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
     <t>Revisión de la tarea 19</t>
@@ -445,104 +198,25 @@
     <t>Revisión de la tarea 21</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestión de acciones:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear modelo de datos para ACCIONES</t>
-    </r>
+    <t>Gestión de acciones:  Crear modelo de datos para ACCIONES</t>
   </si>
   <si>
     <t>Nombre del modelo:ACCIONES_MODEL</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestión de acciones: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear vistas para ACCIONES</t>
-    </r>
+    <t>Gestión de acciones: Crear vistas para ACCIONES</t>
   </si>
   <si>
     <t>Estructura provisional de las vistas para acciones</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Organizar y asignar tareas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>: Semana 1</t>
-    </r>
-  </si>
-  <si>
     <t>Tareas extra</t>
   </si>
   <si>
     <t>Recursos asociado</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestión de acciones: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear controlador de datos para ACCIONES</t>
-    </r>
+    <t>Gestión de acciones: Crear controlador de datos para ACCIONES</t>
   </si>
   <si>
     <t>Falta solucionar como se trataría el borrado de un acción</t>
@@ -557,73 +231,16 @@
     <t>Revisión de la tarea 36</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestion de funcionalidades: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear modelo de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestion de funcionalidades: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear controlador de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
-    </r>
+    <t>Gestion de funcionalidades: Crear modelo de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t>Gestion de funcionalidades: Crear controlador de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
   </si>
   <si>
     <t>Falta solucionar como se trataría el borrado de una funcionalidad y de funcionalidad_accion</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Gestion de funcionalidades: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Crear vistas para las posibles acciones sobre las tablas FUNCIONALIDADES Y FUNCIONALIDAD_ACCION</t>
-    </r>
+    <t>Gestion de funcionalidades: Crear vistas para las posibles acciones sobre las tablas FUNCIONALIDADES Y FUNCIONALIDAD_ACCION</t>
   </si>
   <si>
     <t>Revisión de la tarea 40</t>
@@ -635,92 +252,16 @@
     <t>Revisión de la tarea 42</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Tratamiento del borrado entre las tablas:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> USUARIO, USUARIO_GRUPO y GRUPO.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Tratamiento del borrado entre las tablas:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> PERMISO y GRUPO.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Tratamiento del borrado entre las tabla</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>s: PERMISO y FUNCIONALIDAD_ACCION</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Tratamiento del borrado entre las tablas:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION.</t>
-    </r>
+    <t>Tratamiento del borrado entre las tablas: USUARIO, USUARIO_GRUPO y GRUPO.</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: PERMISO y GRUPO.</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION.</t>
   </si>
   <si>
     <t>Implementar el control sobre los usuarios que pertenecen a uno o varios grupos y tienen unos ciertos permisos.</t>
@@ -766,14 +307,14 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="22"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="22"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -903,11 +444,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -916,15 +457,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -932,7 +473,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -940,7 +481,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -948,15 +489,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -972,11 +505,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -988,10 +521,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1000,7 +529,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel ET3" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1151,28 +680,28 @@
   </sheetPr>
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="90.7142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1260,52 +789,52 @@
       <c r="C4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="n">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F4" s="10" t="n">
+      <c r="F4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="10" t="n">
+      <c r="G4" s="7" t="n">
         <v>50</v>
       </c>
       <c r="H4" s="5"/>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="11" t="n">
+      <c r="J4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="5" t="n">
         <f aca="false">SUMIF(F4:F28,1,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L4" s="12" t="n">
+      <c r="L4" s="5" t="n">
         <f aca="false">SUMIF(F4:F42,1,G4:G42)</f>
         <v>200</v>
       </c>
-      <c r="M4" s="12" t="n">
+      <c r="M4" s="5" t="n">
         <f aca="false">K4/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N4" s="12" t="n">
+      <c r="N4" s="5" t="n">
         <f aca="false">K4/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O4" s="12" t="n">
+      <c r="O4" s="5" t="n">
         <f aca="false">N4-M4</f>
         <v>45</v>
       </c>
-      <c r="P4" s="12" t="n">
+      <c r="P4" s="5" t="n">
         <f aca="false">L4/60*15</f>
         <v>50</v>
       </c>
-      <c r="Q4" s="12" t="n">
+      <c r="Q4" s="5" t="n">
         <f aca="false">L4/60*25</f>
         <v>83.3333333333333</v>
       </c>
-      <c r="R4" s="12" t="n">
+      <c r="R4" s="5" t="n">
         <f aca="false">Q4-P4</f>
         <v>33.3333333333333</v>
       </c>
@@ -1320,52 +849,52 @@
       <c r="C5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="n">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="10" t="n">
+      <c r="G5" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="13" t="n">
+      <c r="J5" s="11" t="n">
         <v>2</v>
       </c>
       <c r="K5" s="5" t="n">
         <f aca="false">SUMIF(F4:F28,2,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L5" s="12" t="n">
+      <c r="L5" s="5" t="n">
         <f aca="false">SUMIF(F4:F42,2,G4:G42)</f>
         <v>120</v>
       </c>
-      <c r="M5" s="12" t="n">
+      <c r="M5" s="5" t="n">
         <f aca="false">K5/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N5" s="12" t="n">
+      <c r="N5" s="5" t="n">
         <f aca="false">K5/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O5" s="12" t="n">
+      <c r="O5" s="5" t="n">
         <f aca="false">N5-M5</f>
         <v>45</v>
       </c>
-      <c r="P5" s="12" t="n">
+      <c r="P5" s="5" t="n">
         <f aca="false">L5/60*15</f>
         <v>30</v>
       </c>
-      <c r="Q5" s="12" t="n">
+      <c r="Q5" s="5" t="n">
         <f aca="false">L5/60*25</f>
         <v>50</v>
       </c>
-      <c r="R5" s="12" t="n">
+      <c r="R5" s="5" t="n">
         <f aca="false">Q5-P5</f>
         <v>20</v>
       </c>
@@ -1380,52 +909,54 @@
       <c r="C6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10" t="n">
+      <c r="E6" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="G6" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="14" t="n">
+      <c r="J6" s="12" t="n">
         <v>3</v>
       </c>
       <c r="K6" s="5" t="n">
         <f aca="false">SUMIF(F4:F28,3,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L6" s="12" t="n">
+      <c r="L6" s="5" t="n">
         <f aca="false">SUMIF(F4:F42,3,G4:G42)</f>
         <v>40</v>
       </c>
-      <c r="M6" s="12" t="n">
+      <c r="M6" s="5" t="n">
         <f aca="false">K6/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N6" s="12" t="n">
+      <c r="N6" s="5" t="n">
         <f aca="false">K6/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O6" s="12" t="n">
+      <c r="O6" s="5" t="n">
         <f aca="false">N6-M6</f>
         <v>45</v>
       </c>
-      <c r="P6" s="12" t="n">
+      <c r="P6" s="5" t="n">
         <f aca="false">L6/60*15</f>
         <v>10</v>
       </c>
-      <c r="Q6" s="12" t="n">
+      <c r="Q6" s="5" t="n">
         <f aca="false">L6/60*25</f>
         <v>16.6666666666667</v>
       </c>
-      <c r="R6" s="12" t="n">
+      <c r="R6" s="5" t="n">
         <f aca="false">Q6-P6</f>
         <v>6.66666666666666</v>
       </c>
@@ -1440,54 +971,54 @@
       <c r="C7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="10" t="n">
+      <c r="E7" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F7" s="10" t="n">
+      <c r="F7" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="10" t="n">
+      <c r="G7" s="7" t="n">
         <v>15</v>
       </c>
       <c r="H7" s="5"/>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="15" t="n">
+      <c r="J7" s="13" t="n">
         <v>4</v>
       </c>
       <c r="K7" s="5" t="n">
         <f aca="false">SUMIF(F4:F28,4,E4:E28)</f>
-        <v>250</v>
-      </c>
-      <c r="L7" s="12" t="n">
+        <v>270</v>
+      </c>
+      <c r="L7" s="5" t="n">
         <f aca="false">SUMIF(F4:F42,4,G4:G42)</f>
         <v>65</v>
       </c>
-      <c r="M7" s="12" t="n">
+      <c r="M7" s="5" t="n">
         <f aca="false">K7/60*15</f>
-        <v>62.5</v>
-      </c>
-      <c r="N7" s="12" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="N7" s="5" t="n">
         <f aca="false">K7/60*25</f>
-        <v>104.166666666667</v>
-      </c>
-      <c r="O7" s="12" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="O7" s="5" t="n">
         <f aca="false">N7-M7</f>
-        <v>41.6666666666667</v>
-      </c>
-      <c r="P7" s="12" t="n">
+        <v>45</v>
+      </c>
+      <c r="P7" s="5" t="n">
         <f aca="false">L7/60*15</f>
         <v>16.25</v>
       </c>
-      <c r="Q7" s="12" t="n">
+      <c r="Q7" s="5" t="n">
         <f aca="false">L7/60*25</f>
         <v>27.0833333333333</v>
       </c>
-      <c r="R7" s="12" t="n">
+      <c r="R7" s="5" t="n">
         <f aca="false">Q7-P7</f>
         <v>10.8333333333333</v>
       </c>
@@ -1496,60 +1027,60 @@
       <c r="A8" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="10" t="n">
+      <c r="E8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="F8" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="10" t="n">
+      <c r="G8" s="7" t="n">
         <v>30</v>
       </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="16" t="n">
+      <c r="J8" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="K8" s="17" t="n">
+      <c r="K8" s="16" t="n">
         <f aca="false">SUMIF(F4:F28,5,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L8" s="18" t="n">
+      <c r="L8" s="16" t="n">
         <f aca="false">SUMIF(F4:F42,5,G4:G42)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="18" t="n">
+      <c r="M8" s="16" t="n">
         <f aca="false">K8/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N8" s="12" t="n">
+      <c r="N8" s="5" t="n">
         <f aca="false">K8/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O8" s="12" t="n">
+      <c r="O8" s="5" t="n">
         <f aca="false">N8-M8</f>
         <v>45</v>
       </c>
-      <c r="P8" s="12" t="n">
+      <c r="P8" s="5" t="n">
         <f aca="false">L8/60*15</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="12" t="n">
+      <c r="Q8" s="5" t="n">
         <f aca="false">L8/60*25</f>
         <v>0</v>
       </c>
-      <c r="R8" s="12" t="n">
+      <c r="R8" s="5" t="n">
         <f aca="false">Q8-P8</f>
         <v>0</v>
       </c>
@@ -1564,46 +1095,46 @@
       <c r="C9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="n">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F9" s="10" t="n">
+      <c r="F9" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="n">
         <f aca="false">SUM(K4:K8)</f>
-        <v>1330</v>
-      </c>
-      <c r="L9" s="12" t="n">
+        <v>1350</v>
+      </c>
+      <c r="L9" s="5" t="n">
         <f aca="false">SUM(L4:L8)</f>
         <v>425</v>
       </c>
-      <c r="M9" s="12" t="n">
+      <c r="M9" s="5" t="n">
         <f aca="false">SUM(M4:M8)</f>
-        <v>332.5</v>
-      </c>
-      <c r="N9" s="19" t="n">
+        <v>337.5</v>
+      </c>
+      <c r="N9" s="17" t="n">
         <f aca="false">SUM(N4:N8)</f>
-        <v>554.166666666667</v>
-      </c>
-      <c r="O9" s="19" t="n">
+        <v>562.5</v>
+      </c>
+      <c r="O9" s="17" t="n">
         <f aca="false">SUM(O4:O8)</f>
-        <v>221.666666666667</v>
-      </c>
-      <c r="P9" s="19" t="n">
+        <v>225</v>
+      </c>
+      <c r="P9" s="17" t="n">
         <f aca="false">SUM(P4:P8)</f>
         <v>106.25</v>
       </c>
-      <c r="Q9" s="19" t="str">
+      <c r="Q9" s="17" t="str">
         <f aca="false">FIXED(SUM(Q5:Q8))</f>
         <v>93,75</v>
       </c>
-      <c r="R9" s="19" t="str">
+      <c r="R9" s="17" t="str">
         <f aca="false">FIXED(SUM(R5:R8))</f>
         <v>37,50</v>
       </c>
@@ -1621,16 +1152,16 @@
       <c r="C10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="10" t="n">
+      <c r="E10" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F10" s="10" t="n">
+      <c r="F10" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G10" s="10" t="n">
+      <c r="G10" s="7" t="n">
         <v>25</v>
       </c>
       <c r="H10" s="5"/>
@@ -1648,16 +1179,16 @@
       <c r="C11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="10" t="n">
+      <c r="E11" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F11" s="10" t="n">
+      <c r="F11" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="10" t="n">
+      <c r="G11" s="7" t="n">
         <v>35</v>
       </c>
       <c r="H11" s="5"/>
@@ -1675,14 +1206,14 @@
       <c r="C12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10" t="n">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F12" s="10" t="n">
+      <c r="F12" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="10" t="n">
+      <c r="G12" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H12" s="5"/>
@@ -1700,16 +1231,16 @@
       <c r="C13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="10" t="n">
+      <c r="E13" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F13" s="10" t="n">
+      <c r="F13" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="10" t="n">
+      <c r="G13" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H13" s="5"/>
@@ -1727,16 +1258,16 @@
       <c r="C14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="10" t="n">
+      <c r="E14" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F14" s="10" t="n">
+      <c r="F14" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="10" t="n">
+      <c r="G14" s="7" t="n">
         <v>15</v>
       </c>
       <c r="H14" s="5"/>
@@ -1748,20 +1279,20 @@
       <c r="A15" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10" t="n">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F15" s="10" t="n">
+      <c r="F15" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="10"/>
+      <c r="G15" s="7"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1771,20 +1302,20 @@
       <c r="A16" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10" t="n">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F16" s="10" t="n">
+      <c r="F16" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G16" s="10"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -1794,20 +1325,20 @@
       <c r="A17" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10" t="n">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F17" s="10" t="n">
+      <c r="F17" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1817,20 +1348,20 @@
       <c r="A18" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10" t="n">
+      <c r="D18" s="7"/>
+      <c r="E18" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F18" s="10" t="n">
+      <c r="F18" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G18" s="10"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1840,20 +1371,20 @@
       <c r="A19" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10" t="n">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F19" s="10" t="n">
+      <c r="F19" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1869,14 +1400,14 @@
       <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10" t="n">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F20" s="10" t="n">
+      <c r="F20" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G20" s="10"/>
+      <c r="G20" s="7"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -1892,16 +1423,16 @@
       <c r="C21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="10" t="n">
+      <c r="E21" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="F21" s="10" t="n">
+      <c r="F21" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="10" t="n">
+      <c r="G21" s="7" t="n">
         <v>40</v>
       </c>
       <c r="H21" s="5"/>
@@ -1919,14 +1450,14 @@
       <c r="C22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10" t="n">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F22" s="10" t="n">
+      <c r="F22" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="10"/>
+      <c r="G22" s="7"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -1936,20 +1467,20 @@
       <c r="A23" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10" t="n">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F23" s="10" t="n">
+      <c r="F23" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G23" s="10"/>
+      <c r="G23" s="7"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -1959,20 +1490,20 @@
       <c r="A24" s="7" t="n">
         <v>21</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10" t="n">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="F24" s="10" t="n">
+      <c r="F24" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G24" s="10"/>
+      <c r="G24" s="7"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -1982,20 +1513,20 @@
       <c r="A25" s="7" t="n">
         <v>22</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="14" t="s">
         <v>56</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10" t="n">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F25" s="10" t="n">
+      <c r="F25" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G25" s="10"/>
+      <c r="G25" s="7"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -2011,16 +1542,16 @@
       <c r="C26" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="10" t="n">
+      <c r="E26" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F26" s="10" t="n">
+      <c r="F26" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G26" s="10" t="n">
+      <c r="G26" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H26" s="5"/>
@@ -2038,16 +1569,16 @@
       <c r="C27" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="10" t="n">
+      <c r="E27" s="7" t="n">
         <v>70</v>
       </c>
-      <c r="F27" s="10" t="n">
+      <c r="F27" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G27" s="10" t="n">
+      <c r="G27" s="7" t="n">
         <v>40</v>
       </c>
       <c r="H27" s="5"/>
@@ -2060,19 +1591,19 @@
         <v>25</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10" t="n">
+      <c r="D28" s="7"/>
+      <c r="E28" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F28" s="10" t="n">
+      <c r="F28" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G28" s="10"/>
+      <c r="G28" s="7"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -2080,12 +1611,12 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -2093,12 +1624,12 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -2106,12 +1637,12 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -2119,12 +1650,12 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -2132,12 +1663,12 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -2145,12 +1676,12 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -2159,7 +1690,7 @@
     <row r="35" customFormat="false" ht="29.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
       <c r="B35" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>3</v>
@@ -2171,7 +1702,7 @@
         <v>5</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>7</v>
@@ -2184,21 +1715,21 @@
     <row r="36" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
       <c r="B36" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="10" t="n">
+      <c r="D36" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="F36" s="10" t="n">
+      <c r="F36" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="n">
+      <c r="G36" s="7" t="n">
         <v>30</v>
       </c>
       <c r="H36" s="5"/>
@@ -2208,18 +1739,18 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1"/>
-      <c r="B37" s="8" t="s">
-        <v>66</v>
+      <c r="B37" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10" t="n">
+      <c r="D37" s="7"/>
+      <c r="E37" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
@@ -2227,18 +1758,18 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1"/>
-      <c r="B38" s="8" t="s">
-        <v>67</v>
+      <c r="B38" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10" t="n">
+      <c r="D38" s="7"/>
+      <c r="E38" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
@@ -2246,18 +1777,18 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
-      <c r="B39" s="8" t="s">
-        <v>68</v>
+      <c r="B39" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10" t="n">
+      <c r="D39" s="7"/>
+      <c r="E39" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -2266,17 +1797,17 @@
     <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>
       <c r="B40" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10" t="n">
+      <c r="D40" s="7"/>
+      <c r="E40" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
@@ -2285,21 +1816,21 @@
     <row r="41" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
       <c r="B41" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="10" t="n">
+      <c r="D41" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="F41" s="10" t="n">
+      <c r="F41" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G41" s="10" t="n">
+      <c r="G41" s="7" t="n">
         <v>45</v>
       </c>
       <c r="H41" s="5"/>
@@ -2310,17 +1841,17 @@
     <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
       <c r="B42" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10" t="n">
+      <c r="D42" s="7"/>
+      <c r="E42" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
@@ -2328,18 +1859,18 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
-      <c r="B43" s="8" t="s">
-        <v>73</v>
+      <c r="B43" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10" t="n">
+      <c r="D43" s="7"/>
+      <c r="E43" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
@@ -2347,18 +1878,18 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1"/>
-      <c r="B44" s="8" t="s">
-        <v>74</v>
+      <c r="B44" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10" t="n">
+      <c r="D44" s="7"/>
+      <c r="E44" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
@@ -2366,18 +1897,18 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
-      <c r="B45" s="8" t="s">
-        <v>75</v>
+      <c r="B45" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10" t="n">
+      <c r="D45" s="7"/>
+      <c r="E45" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
@@ -2386,17 +1917,17 @@
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1"/>
       <c r="B46" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10" t="n">
+      <c r="D46" s="7"/>
+      <c r="E46" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
@@ -2405,17 +1936,17 @@
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1"/>
       <c r="B47" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10" t="n">
+      <c r="D47" s="7"/>
+      <c r="E47" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
@@ -2424,17 +1955,17 @@
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1"/>
       <c r="B48" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10" t="n">
+      <c r="D48" s="7"/>
+      <c r="E48" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
@@ -2443,17 +1974,17 @@
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1"/>
       <c r="B49" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10" t="n">
+      <c r="D49" s="7"/>
+      <c r="E49" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
@@ -2461,18 +1992,18 @@
     </row>
     <row r="50" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
-      <c r="B50" s="20" t="s">
-        <v>80</v>
+      <c r="B50" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10" t="n">
+      <c r="D50" s="7"/>
+      <c r="E50" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
@@ -2550,18 +2081,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,7 +2107,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Correción del excel ya que las tareas a corregir se habían descolocado de fila
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maite\Desktop\ET3\et3\EXCEL TAREAS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="Estados" vbProcedure="false">Hoja2!$A$1:$A$6</definedName>
-    <definedName function="false" hidden="false" name="EstadosVálidos" vbProcedure="false">Hoja2!$A$1:$A$5</definedName>
+    <definedName name="Estados">Hoja2!$A$1:$A$6</definedName>
+    <definedName name="EstadosVálidos">Hoja2!$A$1:$A$5</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
   <si>
     <t>Semana 1(Del 20/10/2017 hasta 26/10/2017)</t>
   </si>
@@ -171,12 +175,6 @@
     <t>Revisión de la tarea 11</t>
   </si>
   <si>
-    <t>Revisión de la tarea 12</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 13</t>
-  </si>
-  <si>
     <t>Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
@@ -192,12 +190,6 @@
     <t>Revisión de la tarea 19</t>
   </si>
   <si>
-    <t>Revisión de la tarea 20</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 21</t>
-  </si>
-  <si>
     <t>Gestión de acciones:  Crear modelo de datos para ACCIONES</t>
   </si>
   <si>
@@ -274,37 +266,34 @@
   </si>
   <si>
     <t>Aplazada</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 6</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 17</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 8</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 7</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="22"/>
@@ -321,12 +310,19 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -374,14 +370,14 @@
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF2F5597"/>
       </left>
@@ -396,7 +392,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -405,137 +401,107 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyProtection="0">
+      <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB4C7E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -549,7 +515,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
+          <bgColor rgb="FFDBDBDB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
         </patternFill>
       </fill>
     </dxf>
@@ -563,21 +543,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
+          <bgColor rgb="FFC5E0B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -591,25 +557,12 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
+          <bgColor rgb="FFD9D9D9"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -668,64 +621,338 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF2F5597"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:S50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="90.7142857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.3928571428571"/>
+    <col min="1" max="1" width="10.42578125"/>
+    <col min="2" max="2" width="90.7109375"/>
+    <col min="3" max="4" width="23.140625"/>
+    <col min="5" max="5" width="19.42578125"/>
+    <col min="6" max="6" width="22.42578125"/>
+    <col min="7" max="7" width="19"/>
+    <col min="8" max="8" width="10.42578125"/>
+    <col min="9" max="9" width="22.7109375"/>
+    <col min="10" max="10" width="16.5703125"/>
+    <col min="11" max="11" width="31.42578125"/>
+    <col min="12" max="12" width="28.7109375"/>
+    <col min="13" max="15" width="17.42578125"/>
+    <col min="16" max="16" width="19.140625"/>
+    <col min="17" max="17" width="20.7109375"/>
+    <col min="18" max="18" width="14"/>
+    <col min="19" max="1025" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -779,8 +1006,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -790,57 +1017,57 @@
         <v>19</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="7">
         <v>30</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="G4" s="7" t="n">
+      <c r="G4" s="7">
         <v>50</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="10" t="n">
+      <c r="J4" s="10">
         <v>1</v>
       </c>
-      <c r="K4" s="5" t="n">
-        <f aca="false">SUMIF(F4:F28,1,E4:E28)</f>
+      <c r="K4" s="5">
+        <f>SUMIF(F4:F28,1,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L4" s="5" t="n">
-        <f aca="false">SUMIF(F4:F42,1,G4:G42)</f>
+      <c r="L4" s="5">
+        <f>SUMIF(F4:F42,1,G4:G42)</f>
         <v>200</v>
       </c>
-      <c r="M4" s="5" t="n">
-        <f aca="false">K4/60*15</f>
+      <c r="M4" s="5">
+        <f>K4/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N4" s="5" t="n">
-        <f aca="false">K4/60*25</f>
+      <c r="N4" s="5">
+        <f>K4/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O4" s="5" t="n">
-        <f aca="false">N4-M4</f>
+      <c r="O4" s="5">
+        <f>N4-M4</f>
         <v>45</v>
       </c>
-      <c r="P4" s="5" t="n">
-        <f aca="false">L4/60*15</f>
+      <c r="P4" s="5">
+        <f>L4/60*15</f>
         <v>50</v>
       </c>
-      <c r="Q4" s="5" t="n">
-        <f aca="false">L4/60*25</f>
-        <v>83.3333333333333</v>
-      </c>
-      <c r="R4" s="5" t="n">
-        <f aca="false">Q4-P4</f>
-        <v>33.3333333333333</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="Q4" s="5">
+        <f>L4/60*25</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="R4" s="5">
+        <f>Q4-P4</f>
+        <v>33.333333333333343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -850,57 +1077,57 @@
         <v>22</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="7">
         <v>20</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="7">
         <v>3</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="7">
         <v>20</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="11" t="n">
+      <c r="J5" s="11">
         <v>2</v>
       </c>
-      <c r="K5" s="5" t="n">
-        <f aca="false">SUMIF(F4:F28,2,E4:E28)</f>
+      <c r="K5" s="5">
+        <f>SUMIF(F4:F28,2,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L5" s="5" t="n">
-        <f aca="false">SUMIF(F4:F42,2,G4:G42)</f>
+      <c r="L5" s="5">
+        <f>SUMIF(F4:F42,2,G4:G42)</f>
         <v>120</v>
       </c>
-      <c r="M5" s="5" t="n">
-        <f aca="false">K5/60*15</f>
+      <c r="M5" s="5">
+        <f>K5/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N5" s="5" t="n">
-        <f aca="false">K5/60*25</f>
+      <c r="N5" s="5">
+        <f>K5/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O5" s="5" t="n">
-        <f aca="false">N5-M5</f>
+      <c r="O5" s="5">
+        <f>N5-M5</f>
         <v>45</v>
       </c>
-      <c r="P5" s="5" t="n">
-        <f aca="false">L5/60*15</f>
+      <c r="P5" s="5">
+        <f>L5/60*15</f>
         <v>30</v>
       </c>
-      <c r="Q5" s="5" t="n">
-        <f aca="false">L5/60*25</f>
+      <c r="Q5" s="5">
+        <f>L5/60*25</f>
         <v>50</v>
       </c>
-      <c r="R5" s="5" t="n">
-        <f aca="false">Q5-P5</f>
+      <c r="R5" s="5">
+        <f>Q5-P5</f>
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -912,57 +1139,57 @@
       <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="7">
         <v>20</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="7">
         <v>4</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="7">
         <v>20</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="12" t="n">
+      <c r="J6" s="12">
         <v>3</v>
       </c>
-      <c r="K6" s="5" t="n">
-        <f aca="false">SUMIF(F4:F28,3,E4:E28)</f>
+      <c r="K6" s="5">
+        <f>SUMIF(F4:F28,3,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L6" s="5" t="n">
-        <f aca="false">SUMIF(F4:F42,3,G4:G42)</f>
+      <c r="L6" s="5">
+        <f>SUMIF(F4:F42,3,G4:G42)</f>
         <v>40</v>
       </c>
-      <c r="M6" s="5" t="n">
-        <f aca="false">K6/60*15</f>
+      <c r="M6" s="5">
+        <f>K6/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N6" s="5" t="n">
-        <f aca="false">K6/60*25</f>
+      <c r="N6" s="5">
+        <f>K6/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O6" s="5" t="n">
-        <f aca="false">N6-M6</f>
+      <c r="O6" s="5">
+        <f>N6-M6</f>
         <v>45</v>
       </c>
-      <c r="P6" s="5" t="n">
-        <f aca="false">L6/60*15</f>
+      <c r="P6" s="5">
+        <f>L6/60*15</f>
         <v>10</v>
       </c>
-      <c r="Q6" s="5" t="n">
-        <f aca="false">L6/60*25</f>
-        <v>16.6666666666667</v>
-      </c>
-      <c r="R6" s="5" t="n">
-        <f aca="false">Q6-P6</f>
-        <v>6.66666666666666</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+      <c r="Q6" s="5">
+        <f>L6/60*25</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="R6" s="5">
+        <f>Q6-P6</f>
+        <v>6.6666666666666643</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -974,57 +1201,57 @@
       <c r="D7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="7">
         <v>20</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="7">
         <v>2</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="G7" s="7">
         <v>15</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="13" t="n">
+      <c r="J7" s="13">
         <v>4</v>
       </c>
-      <c r="K7" s="5" t="n">
-        <f aca="false">SUMIF(F4:F28,4,E4:E28)</f>
+      <c r="K7" s="5">
+        <f>SUMIF(F4:F28,4,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="5" t="n">
-        <f aca="false">SUMIF(F4:F42,4,G4:G42)</f>
+      <c r="L7" s="5">
+        <f>SUMIF(F4:F42,4,G4:G42)</f>
         <v>65</v>
       </c>
-      <c r="M7" s="5" t="n">
-        <f aca="false">K7/60*15</f>
+      <c r="M7" s="5">
+        <f>K7/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N7" s="5" t="n">
-        <f aca="false">K7/60*25</f>
+      <c r="N7" s="5">
+        <f>K7/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O7" s="5" t="n">
-        <f aca="false">N7-M7</f>
+      <c r="O7" s="5">
+        <f>N7-M7</f>
         <v>45</v>
       </c>
-      <c r="P7" s="5" t="n">
-        <f aca="false">L7/60*15</f>
+      <c r="P7" s="5">
+        <f>L7/60*15</f>
         <v>16.25</v>
       </c>
-      <c r="Q7" s="5" t="n">
-        <f aca="false">L7/60*25</f>
-        <v>27.0833333333333</v>
-      </c>
-      <c r="R7" s="5" t="n">
-        <f aca="false">Q7-P7</f>
-        <v>10.8333333333333</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+      <c r="Q7" s="5">
+        <f>L7/60*25</f>
+        <v>27.083333333333332</v>
+      </c>
+      <c r="R7" s="5">
+        <f>Q7-P7</f>
+        <v>10.833333333333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
@@ -1036,57 +1263,57 @@
       <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="7">
         <v>30</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="7">
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="7">
         <v>30</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="15" t="n">
+      <c r="J8" s="15">
         <v>5</v>
       </c>
-      <c r="K8" s="16" t="n">
-        <f aca="false">SUMIF(F4:F28,5,E4:E28)</f>
+      <c r="K8" s="16">
+        <f>SUMIF(F4:F28,5,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L8" s="16" t="n">
-        <f aca="false">SUMIF(F4:F42,5,G4:G42)</f>
+      <c r="L8" s="16">
+        <f>SUMIF(F4:F42,5,G4:G42)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="16" t="n">
-        <f aca="false">K8/60*15</f>
+      <c r="M8" s="16">
+        <f>K8/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N8" s="5" t="n">
-        <f aca="false">K8/60*25</f>
+      <c r="N8" s="5">
+        <f>K8/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O8" s="5" t="n">
-        <f aca="false">N8-M8</f>
+      <c r="O8" s="5">
+        <f>N8-M8</f>
         <v>45</v>
       </c>
-      <c r="P8" s="5" t="n">
-        <f aca="false">L8/60*15</f>
+      <c r="P8" s="5">
+        <f>L8/60*15</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="5" t="n">
-        <f aca="false">L8/60*25</f>
+      <c r="Q8" s="5">
+        <f>L8/60*25</f>
         <v>0</v>
       </c>
-      <c r="R8" s="5" t="n">
-        <f aca="false">Q8-P8</f>
+      <c r="R8" s="5">
+        <f>Q8-P8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
+    <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1096,54 +1323,54 @@
         <v>22</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="7">
         <v>90</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F9" s="7">
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="5" t="n">
-        <f aca="false">SUM(K4:K8)</f>
+      <c r="K9" s="5">
+        <f t="shared" ref="K9:P9" si="0">SUM(K4:K8)</f>
         <v>1350</v>
       </c>
-      <c r="L9" s="5" t="n">
-        <f aca="false">SUM(L4:L8)</f>
+      <c r="L9" s="5">
+        <f t="shared" si="0"/>
         <v>425</v>
       </c>
-      <c r="M9" s="5" t="n">
-        <f aca="false">SUM(M4:M8)</f>
+      <c r="M9" s="5">
+        <f t="shared" si="0"/>
         <v>337.5</v>
       </c>
-      <c r="N9" s="17" t="n">
-        <f aca="false">SUM(N4:N8)</f>
+      <c r="N9" s="17">
+        <f t="shared" si="0"/>
         <v>562.5</v>
       </c>
-      <c r="O9" s="17" t="n">
-        <f aca="false">SUM(O4:O8)</f>
+      <c r="O9" s="17">
+        <f t="shared" si="0"/>
         <v>225</v>
       </c>
-      <c r="P9" s="17" t="n">
-        <f aca="false">SUM(P4:P8)</f>
+      <c r="P9" s="17">
+        <f t="shared" si="0"/>
         <v>106.25</v>
       </c>
       <c r="Q9" s="17" t="str">
-        <f aca="false">FIXED(SUM(Q5:Q8))</f>
+        <f>FIXED(SUM(Q5:Q8))</f>
         <v>93,75</v>
       </c>
       <c r="R9" s="17" t="str">
-        <f aca="false">FIXED(SUM(R5:R8))</f>
+        <f>FIXED(SUM(R5:R8))</f>
         <v>37,50</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1155,13 +1382,13 @@
       <c r="D10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="7">
         <v>90</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F10" s="7">
         <v>4</v>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="G10" s="7">
         <v>25</v>
       </c>
       <c r="H10" s="5"/>
@@ -1169,8 +1396,8 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
+    <row r="11" spans="1:19" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1182,13 +1409,13 @@
       <c r="D11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="7">
         <v>90</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="F11" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="7" t="n">
+      <c r="G11" s="7">
         <v>35</v>
       </c>
       <c r="H11" s="5"/>
@@ -1196,8 +1423,8 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
+    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1207,13 +1434,13 @@
         <v>22</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="7" t="n">
+      <c r="E12" s="7">
         <v>90</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="7">
         <v>3</v>
       </c>
-      <c r="G12" s="7" t="n">
+      <c r="G12" s="7">
         <v>20</v>
       </c>
       <c r="H12" s="5"/>
@@ -1221,8 +1448,8 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+    <row r="13" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1234,13 +1461,13 @@
       <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="E13" s="7">
         <v>60</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="7">
         <v>2</v>
       </c>
-      <c r="G13" s="7" t="n">
+      <c r="G13" s="7">
         <v>20</v>
       </c>
       <c r="H13" s="5"/>
@@ -1248,8 +1475,8 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+    <row r="14" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1261,13 +1488,13 @@
       <c r="D14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="7" t="n">
+      <c r="E14" s="7">
         <v>60</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="7">
         <v>2</v>
       </c>
-      <c r="G14" s="7" t="n">
+      <c r="G14" s="7">
         <v>15</v>
       </c>
       <c r="H14" s="5"/>
@@ -1275,21 +1502,21 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>12</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="7" t="n">
+      <c r="E15" s="7">
         <v>30</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="7">
         <v>3</v>
       </c>
       <c r="G15" s="7"/>
@@ -1298,21 +1525,21 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>13</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="7" t="n">
+      <c r="E16" s="7">
         <v>30</v>
       </c>
-      <c r="F16" s="7" t="n">
+      <c r="F16" s="7">
         <v>5</v>
       </c>
       <c r="G16" s="7"/>
@@ -1321,21 +1548,21 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="n">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>14</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="7" t="n">
+      <c r="E17" s="7">
         <v>30</v>
       </c>
-      <c r="F17" s="7" t="n">
+      <c r="F17" s="7">
         <v>4</v>
       </c>
       <c r="G17" s="7"/>
@@ -1344,21 +1571,21 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>15</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="7" t="n">
+      <c r="E18" s="7">
         <v>30</v>
       </c>
-      <c r="F18" s="7" t="n">
+      <c r="F18" s="7">
         <v>5</v>
       </c>
       <c r="G18" s="7"/>
@@ -1367,21 +1594,21 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="n">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>16</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="7" t="n">
+      <c r="E19" s="7">
         <v>30</v>
       </c>
-      <c r="F19" s="7" t="n">
+      <c r="F19" s="7">
         <v>4</v>
       </c>
       <c r="G19" s="7"/>
@@ -1390,21 +1617,21 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="n">
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>17</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="7" t="n">
+      <c r="E20" s="7">
         <v>100</v>
       </c>
-      <c r="F20" s="7" t="n">
+      <c r="F20" s="7">
         <v>5</v>
       </c>
       <c r="G20" s="7"/>
@@ -1413,26 +1640,26 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="n">
+    <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="E21" s="7">
         <v>120</v>
       </c>
-      <c r="F21" s="7" t="n">
+      <c r="F21" s="7">
         <v>1</v>
       </c>
-      <c r="G21" s="7" t="n">
+      <c r="G21" s="7">
         <v>40</v>
       </c>
       <c r="H21" s="5"/>
@@ -1440,21 +1667,21 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="n">
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>19</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="7" t="n">
+      <c r="E22" s="7">
         <v>90</v>
       </c>
-      <c r="F22" s="7" t="n">
+      <c r="F22" s="7">
         <v>3</v>
       </c>
       <c r="G22" s="7"/>
@@ -1463,21 +1690,21 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="n">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
         <v>20</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="7"/>
-      <c r="E23" s="7" t="n">
+      <c r="E23" s="7">
         <v>30</v>
       </c>
-      <c r="F23" s="7" t="n">
+      <c r="F23" s="7">
         <v>2</v>
       </c>
       <c r="G23" s="7"/>
@@ -1486,21 +1713,21 @@
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="n">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
         <v>21</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="7" t="n">
+      <c r="E24" s="7">
         <v>40</v>
       </c>
-      <c r="F24" s="7" t="n">
+      <c r="F24" s="7">
         <v>3</v>
       </c>
       <c r="G24" s="7"/>
@@ -1509,21 +1736,21 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="n">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>22</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="7"/>
-      <c r="E25" s="7" t="n">
+      <c r="E25" s="7">
         <v>20</v>
       </c>
-      <c r="F25" s="7" t="n">
+      <c r="F25" s="7">
         <v>5</v>
       </c>
       <c r="G25" s="7"/>
@@ -1532,26 +1759,26 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="n">
+    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <v>23</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="7" t="n">
+        <v>54</v>
+      </c>
+      <c r="E26" s="7">
         <v>100</v>
       </c>
-      <c r="F26" s="7" t="n">
+      <c r="F26" s="7">
         <v>4</v>
       </c>
-      <c r="G26" s="7" t="n">
+      <c r="G26" s="7">
         <v>20</v>
       </c>
       <c r="H26" s="5"/>
@@ -1559,26 +1786,26 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="n">
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>24</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="7" t="n">
+        <v>56</v>
+      </c>
+      <c r="E27" s="7">
         <v>70</v>
       </c>
-      <c r="F27" s="7" t="n">
+      <c r="F27" s="7">
         <v>2</v>
       </c>
-      <c r="G27" s="7" t="n">
+      <c r="G27" s="7">
         <v>40</v>
       </c>
       <c r="H27" s="5"/>
@@ -1586,8 +1813,8 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="n">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>25</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -1597,10 +1824,10 @@
         <v>22</v>
       </c>
       <c r="D28" s="7"/>
-      <c r="E28" s="7" t="n">
+      <c r="E28" s="7">
         <v>30</v>
       </c>
-      <c r="F28" s="7" t="n">
+      <c r="F28" s="7">
         <v>1</v>
       </c>
       <c r="G28" s="7"/>
@@ -1609,8 +1836,8 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1622,8 +1849,8 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1"/>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1635,8 +1862,8 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1648,8 +1875,8 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1"/>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1661,8 +1888,8 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1"/>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1674,8 +1901,8 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1"/>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1687,10 +1914,10 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" customFormat="false" ht="29.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1"/>
+    <row r="35" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
       <c r="B35" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>3</v>
@@ -1702,7 +1929,7 @@
         <v>5</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>7</v>
@@ -1712,24 +1939,24 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1"/>
+    <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
       <c r="B36" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="7" t="n">
+        <v>60</v>
+      </c>
+      <c r="E36" s="7">
         <v>120</v>
       </c>
-      <c r="F36" s="7" t="n">
+      <c r="F36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="7" t="n">
+      <c r="G36" s="7">
         <v>30</v>
       </c>
       <c r="H36" s="5"/>
@@ -1737,16 +1964,16 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1"/>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
       <c r="B37" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="7" t="n">
+      <c r="E37" s="7">
         <v>30</v>
       </c>
       <c r="F37" s="7"/>
@@ -1756,16 +1983,16 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1"/>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
       <c r="B38" s="14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D38" s="7"/>
-      <c r="E38" s="7" t="n">
+      <c r="E38" s="7">
         <v>30</v>
       </c>
       <c r="F38" s="7"/>
@@ -1775,16 +2002,16 @@
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
       <c r="B39" s="14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="7" t="n">
+      <c r="E39" s="7">
         <v>30</v>
       </c>
       <c r="F39" s="7"/>
@@ -1794,16 +2021,16 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
+    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
       <c r="B40" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D40" s="7"/>
-      <c r="E40" s="7" t="n">
+      <c r="E40" s="7">
         <v>100</v>
       </c>
       <c r="F40" s="7"/>
@@ -1813,24 +2040,24 @@
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
     </row>
-    <row r="41" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1"/>
+    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
       <c r="B41" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E41" s="7" t="n">
+        <v>66</v>
+      </c>
+      <c r="E41" s="7">
         <v>120</v>
       </c>
-      <c r="F41" s="7" t="n">
+      <c r="F41" s="7">
         <v>1</v>
       </c>
-      <c r="G41" s="7" t="n">
+      <c r="G41" s="7">
         <v>45</v>
       </c>
       <c r="H41" s="5"/>
@@ -1838,16 +2065,16 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1"/>
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
       <c r="B42" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D42" s="7"/>
-      <c r="E42" s="7" t="n">
+      <c r="E42" s="7">
         <v>90</v>
       </c>
       <c r="F42" s="7"/>
@@ -1857,16 +2084,16 @@
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1"/>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
       <c r="B43" s="14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D43" s="7"/>
-      <c r="E43" s="7" t="n">
+      <c r="E43" s="7">
         <v>30</v>
       </c>
       <c r="F43" s="7"/>
@@ -1876,16 +2103,16 @@
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1"/>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
       <c r="B44" s="14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D44" s="7"/>
-      <c r="E44" s="7" t="n">
+      <c r="E44" s="7">
         <v>30</v>
       </c>
       <c r="F44" s="7"/>
@@ -1895,16 +2122,16 @@
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1"/>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
       <c r="B45" s="14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="7" t="n">
+      <c r="E45" s="7">
         <v>30</v>
       </c>
       <c r="F45" s="7"/>
@@ -1914,16 +2141,16 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1"/>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
       <c r="B46" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D46" s="7"/>
-      <c r="E46" s="7" t="n">
+      <c r="E46" s="7">
         <v>90</v>
       </c>
       <c r="F46" s="7"/>
@@ -1933,16 +2160,16 @@
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1"/>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
       <c r="B47" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D47" s="7"/>
-      <c r="E47" s="7" t="n">
+      <c r="E47" s="7">
         <v>90</v>
       </c>
       <c r="F47" s="7"/>
@@ -1952,16 +2179,16 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1"/>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
       <c r="B48" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D48" s="7"/>
-      <c r="E48" s="7" t="n">
+      <c r="E48" s="7">
         <v>90</v>
       </c>
       <c r="F48" s="7"/>
@@ -1971,16 +2198,16 @@
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1"/>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
       <c r="B49" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D49" s="7"/>
-      <c r="E49" s="7" t="n">
+      <c r="E49" s="7">
         <v>90</v>
       </c>
       <c r="F49" s="7"/>
@@ -1990,16 +2217,16 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
     </row>
-    <row r="50" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1"/>
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
       <c r="B50" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D50" s="7"/>
-      <c r="E50" s="7" t="n">
+      <c r="E50" s="7">
         <v>120</v>
       </c>
       <c r="F50" s="7"/>
@@ -2009,119 +2236,117 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
     </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" s="7">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F28">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:J8">
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36:F42">
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C28 C36:C50" type="list">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C28 C36:C51">
       <formula1>Estados</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3928571428571"/>
+    <col min="1" max="1" width="22.140625"/>
+    <col min="2" max="1025" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revisada la tarea 8 no me deja cambiar de estado por Brais Santos
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maite\Desktop\ET3\et3\EXCEL TAREAS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Estados">Hoja2!$A$1:$A$6</definedName>
-    <definedName name="EstadosVálidos">Hoja2!$A$1:$A$5</definedName>
+    <definedName function="false" hidden="false" name="Estados" vbProcedure="false">Hoja2!$A$1:$A$6</definedName>
+    <definedName function="false" hidden="false" name="EstadosVálidos" vbProcedure="false">Hoja2!$A$1:$A$5</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="85">
   <si>
     <t>Semana 1(Del 20/10/2017 hasta 26/10/2017)</t>
   </si>
@@ -151,7 +147,7 @@
     <t>Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de los USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
-    <t>Creado el controladro: USUARIOS_GRUPO_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de USUARIO_GRUPO no se puede editar al ser claves.</t>
+    <t>Creado el controladro: USUARIOS_GRUPO_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de USUARIO_GRUPO no se puede editar al ser claves.                              </t>
   </si>
   <si>
     <t>Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
@@ -166,99 +162,117 @@
     <t>Gestión de grupos de usuario: Crear vistas para las posibles acciones sobre la tabla GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
+    <t>Revisión de la tarea 6</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 7</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 8</t>
+  </si>
+  <si>
+    <t>En la correción en la línea 28 se cambio idgrupo por grupo porque estaba mal puesto,en lalínea 41 se cambio USUARIOS_GRUPO_ADD por USUARIOS_ADD y en la línea 61 USUARIOS_DELETE por USUARIOS_GRUPO_DELETE. En la línea 60 se cambió USUARIOS_GRUPO por USUARIOS_GRUPO_Model</t>
+  </si>
+  <si>
     <t>Revisión de la tarea 9</t>
   </si>
   <si>
     <t>Revisión de la tarea 10</t>
   </si>
   <si>
+    <t>Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t>Gestion de permisos de usuario:  Crear controlador de datos para la tabla PERMISOS.  (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t>Creado el controladro: PERMISOS_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de  PERMISOS no se puede editar al ser claves.</t>
+  </si>
+  <si>
+    <t>Gestion de permisos de usuario:  Crear vistas para las posibles acciones sobre la tabla PERMISOS.   (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 17</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 18</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 19</t>
+  </si>
+  <si>
+    <t>Gestión de acciones:  Crear modelo de datos para ACCIONES</t>
+  </si>
+  <si>
+    <t>Nombre del modelo:ACCIONES_MODEL</t>
+  </si>
+  <si>
+    <t>Gestión de acciones: Crear vistas para ACCIONES</t>
+  </si>
+  <si>
+    <t>Estructura provisional de las vistas para acciones</t>
+  </si>
+  <si>
+    <t>Tareas extra</t>
+  </si>
+  <si>
+    <t>Recursos asociado</t>
+  </si>
+  <si>
+    <t>Gestión de acciones: Crear controlador de datos para ACCIONES</t>
+  </si>
+  <si>
+    <t>Falta solucionar como se trataría el borrado de un acción</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 23</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 24</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 36</t>
+  </si>
+  <si>
+    <t>Gestion de funcionalidades: Crear modelo de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t>Gestion de funcionalidades: Crear controlador de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t>Falta solucionar como se trataría el borrado de una funcionalidad y de funcionalidad_accion</t>
+  </si>
+  <si>
+    <t>Gestion de funcionalidades: Crear vistas para las posibles acciones sobre las tablas FUNCIONALIDADES Y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 40</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 41</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 42</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: USUARIO, USUARIO_GRUPO y GRUPO.</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: PERMISO y GRUPO.</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION.</t>
+  </si>
+  <si>
+    <t>Implementar el control sobre los usuarios que pertenecen a uno o varios grupos y tienen unos ciertos permisos.</t>
+  </si>
+  <si>
     <t>Revisión de la tarea 11</t>
   </si>
   <si>
-    <t>Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Gestion de permisos de usuario:  Crear controlador de datos para la tabla PERMISOS.  (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Creado el controladro: PERMISOS_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de  PERMISOS no se puede editar al ser claves.</t>
-  </si>
-  <si>
-    <t>Gestion de permisos de usuario:  Crear vistas para las posibles acciones sobre la tabla PERMISOS.   (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 19</t>
-  </si>
-  <si>
-    <t>Gestión de acciones:  Crear modelo de datos para ACCIONES</t>
-  </si>
-  <si>
-    <t>Nombre del modelo:ACCIONES_MODEL</t>
-  </si>
-  <si>
-    <t>Gestión de acciones: Crear vistas para ACCIONES</t>
-  </si>
-  <si>
-    <t>Estructura provisional de las vistas para acciones</t>
-  </si>
-  <si>
-    <t>Tareas extra</t>
-  </si>
-  <si>
-    <t>Recursos asociado</t>
-  </si>
-  <si>
-    <t>Gestión de acciones: Crear controlador de datos para ACCIONES</t>
-  </si>
-  <si>
-    <t>Falta solucionar como se trataría el borrado de un acción</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 23</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 24</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 36</t>
-  </si>
-  <si>
-    <t>Gestion de funcionalidades: Crear modelo de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t>Gestion de funcionalidades: Crear controlador de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t>Falta solucionar como se trataría el borrado de una funcionalidad y de funcionalidad_accion</t>
-  </si>
-  <si>
-    <t>Gestion de funcionalidades: Crear vistas para las posibles acciones sobre las tablas FUNCIONALIDADES Y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 40</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 41</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 42</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: USUARIO, USUARIO_GRUPO y GRUPO.</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: PERMISO y GRUPO.</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION.</t>
-  </si>
-  <si>
-    <t>Implementar el control sobre los usuarios que pertenecen a uno o varios grupos y tienen unos ciertos permisos.</t>
-  </si>
-  <si>
     <t>Finalizada/Corregida</t>
   </si>
   <si>
@@ -266,34 +280,37 @@
   </si>
   <si>
     <t>Aplazada</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 6</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 17</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 8</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 7</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="22"/>
@@ -310,7 +327,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -318,7 +335,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -370,14 +386,14 @@
     </fill>
   </fills>
   <borders count="5">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
         <color rgb="FF2F5597"/>
       </left>
@@ -392,7 +408,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -401,93 +417,159 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyProtection="0">
-      <alignment wrapText="1"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+  <cellXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
+  <cellStyles count="7">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFE699"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -501,7 +583,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBDBDB"/>
         </patternFill>
       </fill>
     </dxf>
@@ -515,21 +611,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
+          <bgColor rgb="FFC5E0B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -543,26 +625,11 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFFFE699"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -621,338 +688,64 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF2F5597"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125"/>
-    <col min="2" max="2" width="90.7109375"/>
-    <col min="3" max="4" width="23.140625"/>
-    <col min="5" max="5" width="19.42578125"/>
-    <col min="6" max="6" width="22.42578125"/>
-    <col min="7" max="7" width="19"/>
-    <col min="8" max="8" width="10.42578125"/>
-    <col min="9" max="9" width="22.7109375"/>
-    <col min="10" max="10" width="16.5703125"/>
-    <col min="11" max="11" width="31.42578125"/>
-    <col min="12" max="12" width="28.7109375"/>
-    <col min="13" max="15" width="17.42578125"/>
-    <col min="16" max="16" width="19.140625"/>
-    <col min="17" max="17" width="20.7109375"/>
-    <col min="18" max="18" width="14"/>
-    <col min="19" max="1025" width="10.42578125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="89.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1006,8 +799,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1017,57 +810,57 @@
         <v>19</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="7">
+      <c r="E4" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="7" t="n">
         <v>50</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="K4" s="5">
-        <f>SUMIF(F4:F28,1,E4:E28)</f>
+      <c r="K4" s="5" t="n">
+        <f aca="false">SUMIF(F4:F28,1,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L4" s="5">
-        <f>SUMIF(F4:F42,1,G4:G42)</f>
+      <c r="L4" s="5" t="n">
+        <f aca="false">SUMIF(F4:F42,1,G4:G42)</f>
         <v>200</v>
       </c>
-      <c r="M4" s="5">
-        <f>K4/60*15</f>
+      <c r="M4" s="5" t="n">
+        <f aca="false">K4/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N4" s="5">
-        <f>K4/60*25</f>
+      <c r="N4" s="5" t="n">
+        <f aca="false">K4/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O4" s="5">
-        <f>N4-M4</f>
+      <c r="O4" s="5" t="n">
+        <f aca="false">N4-M4</f>
         <v>45</v>
       </c>
-      <c r="P4" s="5">
-        <f>L4/60*15</f>
+      <c r="P4" s="5" t="n">
+        <f aca="false">L4/60*15</f>
         <v>50</v>
       </c>
-      <c r="Q4" s="5">
-        <f>L4/60*25</f>
-        <v>83.333333333333343</v>
-      </c>
-      <c r="R4" s="5">
-        <f>Q4-P4</f>
-        <v>33.333333333333343</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="Q4" s="5" t="n">
+        <f aca="false">L4/60*25</f>
+        <v>83.3333333333333</v>
+      </c>
+      <c r="R4" s="5" t="n">
+        <f aca="false">Q4-P4</f>
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1077,57 +870,57 @@
         <v>22</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="7">
+      <c r="E5" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K5" s="5">
-        <f>SUMIF(F4:F28,2,E4:E28)</f>
+      <c r="K5" s="5" t="n">
+        <f aca="false">SUMIF(F4:F28,2,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L5" s="5">
-        <f>SUMIF(F4:F42,2,G4:G42)</f>
+      <c r="L5" s="5" t="n">
+        <f aca="false">SUMIF(F4:F42,2,G4:G42)</f>
         <v>120</v>
       </c>
-      <c r="M5" s="5">
-        <f>K5/60*15</f>
+      <c r="M5" s="5" t="n">
+        <f aca="false">K5/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N5" s="5">
-        <f>K5/60*25</f>
+      <c r="N5" s="5" t="n">
+        <f aca="false">K5/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O5" s="5">
-        <f>N5-M5</f>
+      <c r="O5" s="5" t="n">
+        <f aca="false">N5-M5</f>
         <v>45</v>
       </c>
-      <c r="P5" s="5">
-        <f>L5/60*15</f>
+      <c r="P5" s="5" t="n">
+        <f aca="false">L5/60*15</f>
         <v>30</v>
       </c>
-      <c r="Q5" s="5">
-        <f>L5/60*25</f>
+      <c r="Q5" s="5" t="n">
+        <f aca="false">L5/60*25</f>
         <v>50</v>
       </c>
-      <c r="R5" s="5">
-        <f>Q5-P5</f>
+      <c r="R5" s="5" t="n">
+        <f aca="false">Q5-P5</f>
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+    <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1139,57 +932,57 @@
       <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="K6" s="5">
-        <f>SUMIF(F4:F28,3,E4:E28)</f>
+      <c r="K6" s="5" t="n">
+        <f aca="false">SUMIF(F4:F28,3,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L6" s="5">
-        <f>SUMIF(F4:F42,3,G4:G42)</f>
+      <c r="L6" s="5" t="n">
+        <f aca="false">SUMIF(F4:F42,3,G4:G42)</f>
         <v>40</v>
       </c>
-      <c r="M6" s="5">
-        <f>K6/60*15</f>
+      <c r="M6" s="5" t="n">
+        <f aca="false">K6/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N6" s="5">
-        <f>K6/60*25</f>
+      <c r="N6" s="5" t="n">
+        <f aca="false">K6/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O6" s="5">
-        <f>N6-M6</f>
+      <c r="O6" s="5" t="n">
+        <f aca="false">N6-M6</f>
         <v>45</v>
       </c>
-      <c r="P6" s="5">
-        <f>L6/60*15</f>
+      <c r="P6" s="5" t="n">
+        <f aca="false">L6/60*15</f>
         <v>10</v>
       </c>
-      <c r="Q6" s="5">
-        <f>L6/60*25</f>
-        <v>16.666666666666664</v>
-      </c>
-      <c r="R6" s="5">
-        <f>Q6-P6</f>
-        <v>6.6666666666666643</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="Q6" s="5" t="n">
+        <f aca="false">L6/60*25</f>
+        <v>16.6666666666667</v>
+      </c>
+      <c r="R6" s="5" t="n">
+        <f aca="false">Q6-P6</f>
+        <v>6.66666666666666</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1201,57 +994,57 @@
       <c r="D7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="7" t="n">
         <v>15</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="K7" s="5">
-        <f>SUMIF(F4:F28,4,E4:E28)</f>
+      <c r="K7" s="5" t="n">
+        <f aca="false">SUMIF(F4:F28,4,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="5">
-        <f>SUMIF(F4:F42,4,G4:G42)</f>
+      <c r="L7" s="5" t="n">
+        <f aca="false">SUMIF(F4:F42,4,G4:G42)</f>
         <v>65</v>
       </c>
-      <c r="M7" s="5">
-        <f>K7/60*15</f>
+      <c r="M7" s="5" t="n">
+        <f aca="false">K7/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N7" s="5">
-        <f>K7/60*25</f>
+      <c r="N7" s="5" t="n">
+        <f aca="false">K7/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O7" s="5">
-        <f>N7-M7</f>
+      <c r="O7" s="5" t="n">
+        <f aca="false">N7-M7</f>
         <v>45</v>
       </c>
-      <c r="P7" s="5">
-        <f>L7/60*15</f>
+      <c r="P7" s="5" t="n">
+        <f aca="false">L7/60*15</f>
         <v>16.25</v>
       </c>
-      <c r="Q7" s="5">
-        <f>L7/60*25</f>
-        <v>27.083333333333332</v>
-      </c>
-      <c r="R7" s="5">
-        <f>Q7-P7</f>
-        <v>10.833333333333332</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="Q7" s="5" t="n">
+        <f aca="false">L7/60*25</f>
+        <v>27.0833333333333</v>
+      </c>
+      <c r="R7" s="5" t="n">
+        <f aca="false">Q7-P7</f>
+        <v>10.8333333333333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
@@ -1263,57 +1056,57 @@
       <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="7" t="n">
         <v>30</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="K8" s="16">
-        <f>SUMIF(F4:F28,5,E4:E28)</f>
+      <c r="K8" s="16" t="n">
+        <f aca="false">SUMIF(F4:F28,5,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L8" s="16">
-        <f>SUMIF(F4:F42,5,G4:G42)</f>
+      <c r="L8" s="16" t="n">
+        <f aca="false">SUMIF(F4:F42,5,G4:G42)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="16">
-        <f>K8/60*15</f>
+      <c r="M8" s="16" t="n">
+        <f aca="false">K8/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N8" s="5">
-        <f>K8/60*25</f>
+      <c r="N8" s="5" t="n">
+        <f aca="false">K8/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O8" s="5">
-        <f>N8-M8</f>
+      <c r="O8" s="5" t="n">
+        <f aca="false">N8-M8</f>
         <v>45</v>
       </c>
-      <c r="P8" s="5">
-        <f>L8/60*15</f>
+      <c r="P8" s="5" t="n">
+        <f aca="false">L8/60*15</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="5">
-        <f>L8/60*25</f>
+      <c r="Q8" s="5" t="n">
+        <f aca="false">L8/60*25</f>
         <v>0</v>
       </c>
-      <c r="R8" s="5">
-        <f>Q8-P8</f>
+      <c r="R8" s="5" t="n">
+        <f aca="false">Q8-P8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1323,54 +1116,54 @@
         <v>22</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="7">
+      <c r="E9" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="7" t="n">
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="5">
-        <f t="shared" ref="K9:P9" si="0">SUM(K4:K8)</f>
+      <c r="K9" s="5" t="n">
+        <f aca="false">SUM(K4:K8)</f>
         <v>1350</v>
       </c>
-      <c r="L9" s="5">
-        <f t="shared" si="0"/>
+      <c r="L9" s="5" t="n">
+        <f aca="false">SUM(L4:L8)</f>
         <v>425</v>
       </c>
-      <c r="M9" s="5">
-        <f t="shared" si="0"/>
+      <c r="M9" s="5" t="n">
+        <f aca="false">SUM(M4:M8)</f>
         <v>337.5</v>
       </c>
-      <c r="N9" s="17">
-        <f t="shared" si="0"/>
+      <c r="N9" s="17" t="n">
+        <f aca="false">SUM(N4:N8)</f>
         <v>562.5</v>
       </c>
-      <c r="O9" s="17">
-        <f t="shared" si="0"/>
+      <c r="O9" s="17" t="n">
+        <f aca="false">SUM(O4:O8)</f>
         <v>225</v>
       </c>
-      <c r="P9" s="17">
-        <f t="shared" si="0"/>
+      <c r="P9" s="17" t="n">
+        <f aca="false">SUM(P4:P8)</f>
         <v>106.25</v>
       </c>
       <c r="Q9" s="17" t="str">
-        <f>FIXED(SUM(Q5:Q8))</f>
+        <f aca="false">FIXED(SUM(Q5:Q8))</f>
         <v>93,75</v>
       </c>
       <c r="R9" s="17" t="str">
-        <f>FIXED(SUM(R5:R8))</f>
+        <f aca="false">FIXED(SUM(R5:R8))</f>
         <v>37,50</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1382,13 +1175,13 @@
       <c r="D10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="7" t="n">
         <v>25</v>
       </c>
       <c r="H10" s="5"/>
@@ -1396,8 +1189,8 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:19" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+    <row r="11" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1409,13 +1202,13 @@
       <c r="D11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="7" t="n">
         <v>35</v>
       </c>
       <c r="H11" s="5"/>
@@ -1423,8 +1216,8 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1434,13 +1227,13 @@
         <v>22</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="7">
+      <c r="E12" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H12" s="5"/>
@@ -1448,8 +1241,8 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1461,13 +1254,13 @@
       <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H13" s="5"/>
@@ -1475,8 +1268,8 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+    <row r="14" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
         <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1488,13 +1281,13 @@
       <c r="D14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="7" t="n">
         <v>15</v>
       </c>
       <c r="H14" s="5"/>
@@ -1502,21 +1295,21 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="n">
         <v>12</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="7">
+      <c r="E15" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="7" t="n">
         <v>3</v>
       </c>
       <c r="G15" s="7"/>
@@ -1525,21 +1318,21 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="n">
         <v>13</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="7">
+      <c r="E16" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="7" t="n">
         <v>5</v>
       </c>
       <c r="G16" s="7"/>
@@ -1548,21 +1341,23 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+    <row r="17" customFormat="false" ht="202.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="n">
         <v>14</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7">
+      <c r="D17" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="7" t="n">
         <v>4</v>
       </c>
       <c r="G17" s="7"/>
@@ -1571,21 +1366,21 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="n">
         <v>15</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="7">
+      <c r="E18" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="7" t="n">
         <v>5</v>
       </c>
       <c r="G18" s="7"/>
@@ -1594,21 +1389,21 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="n">
         <v>16</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="7">
+      <c r="E19" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="7" t="n">
         <v>4</v>
       </c>
       <c r="G19" s="7"/>
@@ -1617,21 +1412,21 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="n">
         <v>17</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="7">
+      <c r="E20" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="7" t="n">
         <v>5</v>
       </c>
       <c r="G20" s="7"/>
@@ -1640,26 +1435,26 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+    <row r="21" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="n">
         <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="7">
+        <v>53</v>
+      </c>
+      <c r="E21" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="7" t="n">
         <v>40</v>
       </c>
       <c r="H21" s="5"/>
@@ -1667,21 +1462,21 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="n">
         <v>19</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="7">
+      <c r="E22" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="7" t="n">
         <v>3</v>
       </c>
       <c r="G22" s="7"/>
@@ -1690,21 +1485,21 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="n">
         <v>20</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="7"/>
-      <c r="E23" s="7">
+      <c r="E23" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="7" t="n">
         <v>2</v>
       </c>
       <c r="G23" s="7"/>
@@ -1713,21 +1508,21 @@
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="n">
         <v>21</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="7">
+      <c r="E24" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="7" t="n">
         <v>3</v>
       </c>
       <c r="G24" s="7"/>
@@ -1736,21 +1531,21 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
         <v>22</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="7"/>
-      <c r="E25" s="7">
+      <c r="E25" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="7" t="n">
         <v>5</v>
       </c>
       <c r="G25" s="7"/>
@@ -1759,26 +1554,26 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+    <row r="26" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="n">
         <v>23</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="7">
+        <v>59</v>
+      </c>
+      <c r="E26" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H26" s="5"/>
@@ -1786,26 +1581,26 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="n">
         <v>24</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="7">
+        <v>61</v>
+      </c>
+      <c r="E27" s="7" t="n">
         <v>70</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="7" t="n">
         <v>40</v>
       </c>
       <c r="H27" s="5"/>
@@ -1813,8 +1608,8 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="n">
         <v>25</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -1824,10 +1619,10 @@
         <v>22</v>
       </c>
       <c r="D28" s="7"/>
-      <c r="E28" s="7">
+      <c r="E28" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="7" t="n">
         <v>1</v>
       </c>
       <c r="G28" s="7"/>
@@ -1836,8 +1631,8 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1849,8 +1644,8 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1862,8 +1657,8 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1875,8 +1670,8 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1888,8 +1683,8 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1901,8 +1696,8 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1914,10 +1709,10 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+    <row r="35" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1"/>
       <c r="B35" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>3</v>
@@ -1929,7 +1724,7 @@
         <v>5</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>7</v>
@@ -1939,24 +1734,24 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
+    <row r="36" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1"/>
       <c r="B36" s="8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="7">
+        <v>65</v>
+      </c>
+      <c r="E36" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="7" t="n">
         <v>30</v>
       </c>
       <c r="H36" s="5"/>
@@ -1964,16 +1759,16 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1"/>
       <c r="B37" s="14" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="7">
+      <c r="E37" s="7" t="n">
         <v>30</v>
       </c>
       <c r="F37" s="7"/>
@@ -1983,16 +1778,16 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1"/>
       <c r="B38" s="14" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D38" s="7"/>
-      <c r="E38" s="7">
+      <c r="E38" s="7" t="n">
         <v>30</v>
       </c>
       <c r="F38" s="7"/>
@@ -2002,16 +1797,16 @@
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1"/>
       <c r="B39" s="14" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="7">
+      <c r="E39" s="7" t="n">
         <v>30</v>
       </c>
       <c r="F39" s="7"/>
@@ -2021,16 +1816,16 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
     </row>
-    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
+    <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1"/>
       <c r="B40" s="8" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D40" s="7"/>
-      <c r="E40" s="7">
+      <c r="E40" s="7" t="n">
         <v>100</v>
       </c>
       <c r="F40" s="7"/>
@@ -2040,24 +1835,24 @@
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
     </row>
-    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
+    <row r="41" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1"/>
       <c r="B41" s="8" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" s="7">
+        <v>71</v>
+      </c>
+      <c r="E41" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G41" s="7">
+      <c r="G41" s="7" t="n">
         <v>45</v>
       </c>
       <c r="H41" s="5"/>
@@ -2065,16 +1860,16 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
+    <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1"/>
       <c r="B42" s="8" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D42" s="7"/>
-      <c r="E42" s="7">
+      <c r="E42" s="7" t="n">
         <v>90</v>
       </c>
       <c r="F42" s="7"/>
@@ -2084,16 +1879,16 @@
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1"/>
       <c r="B43" s="14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D43" s="7"/>
-      <c r="E43" s="7">
+      <c r="E43" s="7" t="n">
         <v>30</v>
       </c>
       <c r="F43" s="7"/>
@@ -2103,16 +1898,16 @@
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1"/>
       <c r="B44" s="14" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D44" s="7"/>
-      <c r="E44" s="7">
+      <c r="E44" s="7" t="n">
         <v>30</v>
       </c>
       <c r="F44" s="7"/>
@@ -2122,16 +1917,16 @@
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1"/>
       <c r="B45" s="14" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="7">
+      <c r="E45" s="7" t="n">
         <v>30</v>
       </c>
       <c r="F45" s="7"/>
@@ -2141,16 +1936,16 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1"/>
       <c r="B46" s="8" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D46" s="7"/>
-      <c r="E46" s="7">
+      <c r="E46" s="7" t="n">
         <v>90</v>
       </c>
       <c r="F46" s="7"/>
@@ -2160,16 +1955,16 @@
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1"/>
       <c r="B47" s="8" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D47" s="7"/>
-      <c r="E47" s="7">
+      <c r="E47" s="7" t="n">
         <v>90</v>
       </c>
       <c r="F47" s="7"/>
@@ -2179,16 +1974,16 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1"/>
       <c r="B48" s="8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D48" s="7"/>
-      <c r="E48" s="7">
+      <c r="E48" s="7" t="n">
         <v>90</v>
       </c>
       <c r="F48" s="7"/>
@@ -2198,16 +1993,16 @@
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1"/>
       <c r="B49" s="8" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D49" s="7"/>
-      <c r="E49" s="7">
+      <c r="E49" s="7" t="n">
         <v>90</v>
       </c>
       <c r="F49" s="7"/>
@@ -2217,16 +2012,16 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
     </row>
-    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
+    <row r="50" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1"/>
       <c r="B50" s="8" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D50" s="7"/>
-      <c r="E50" s="7">
+      <c r="E50" s="7" t="n">
         <v>120</v>
       </c>
       <c r="F50" s="7"/>
@@ -2236,14 +2031,14 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="18" t="s">
-        <v>47</v>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="7" t="n">
         <v>30</v>
       </c>
     </row>
@@ -2252,101 +2047,114 @@
     <mergeCell ref="B1:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F28">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:J8">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36:F42">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C28 C36:C51">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C28 C36:C51" type="list">
       <formula1>Estados</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625"/>
-    <col min="2" max="1025" width="10.42578125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel modificado sin poder poner el estado corregido.
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
   <si>
     <t>Semana 1(Del 20/10/2017 hasta 26/10/2017)</t>
   </si>
@@ -171,7 +171,7 @@
     <t>Revisión de la tarea 8</t>
   </si>
   <si>
-    <t>En la correción en la línea 28 se cambio idgrupo por grupo porque estaba mal puesto,en lalínea 41 se cambio USUARIOS_GRUPO_ADD por USUARIOS_ADD y en la línea 61 USUARIOS_DELETE por USUARIOS_GRUPO_DELETE. En la línea 60 se cambió USUARIOS_GRUPO por USUARIOS_GRUPO_Model</t>
+    <t>En la correción en la línea 28 se cambio idgrupo por grupo porque estaba mal puesto,en lalínea 41 se cambio USUARIOS_GRUPO_ADD por USUARIOS_ADD y en la línea 61 USUARIOS_DELETE por USUARIOS_GRUPO_DELETE. En la línea 60 se cambió USUARIOS_GRUPO por USUARIOS_GRUPO_Model.  A mayores se añadieron comentarios para entender lo que se hacía</t>
   </si>
   <si>
     <t>Revisión de la tarea 9</t>
@@ -289,7 +289,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -333,12 +333,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -460,7 +454,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -531,10 +525,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -706,22 +696,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="89.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="88.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1016,7 +1006,7 @@
       </c>
       <c r="L7" s="5" t="n">
         <f aca="false">SUMIF(F4:F42,4,G4:G42)</f>
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M7" s="5" t="n">
         <f aca="false">K7/60*15</f>
@@ -1032,15 +1022,15 @@
       </c>
       <c r="P7" s="5" t="n">
         <f aca="false">L7/60*15</f>
-        <v>16.25</v>
+        <v>24.5</v>
       </c>
       <c r="Q7" s="5" t="n">
         <f aca="false">L7/60*25</f>
-        <v>27.0833333333333</v>
+        <v>40.8333333333333</v>
       </c>
       <c r="R7" s="5" t="n">
         <f aca="false">Q7-P7</f>
-        <v>10.8333333333333</v>
+        <v>16.3333333333333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,7 +1122,7 @@
       </c>
       <c r="L9" s="5" t="n">
         <f aca="false">SUM(L4:L8)</f>
-        <v>425</v>
+        <v>458</v>
       </c>
       <c r="M9" s="5" t="n">
         <f aca="false">SUM(M4:M8)</f>
@@ -1148,15 +1138,15 @@
       </c>
       <c r="P9" s="17" t="n">
         <f aca="false">SUM(P4:P8)</f>
-        <v>106.25</v>
+        <v>114.5</v>
       </c>
       <c r="Q9" s="17" t="str">
         <f aca="false">FIXED(SUM(Q5:Q8))</f>
-        <v>93,75</v>
+        <v>107,50</v>
       </c>
       <c r="R9" s="17" t="str">
         <f aca="false">FIXED(SUM(R5:R8))</f>
-        <v>37,50</v>
+        <v>43,00</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>36</v>
@@ -1341,17 +1331,15 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="202.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="n">
         <v>14</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="18" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="7" t="n">
@@ -1360,7 +1348,9 @@
       <c r="F17" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="7" t="n">
+        <v>33</v>
+      </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -2032,7 +2022,7 @@
       <c r="K50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="18" t="s">
         <v>81</v>
       </c>
       <c r="C51" s="9" t="s">
@@ -2114,8 +2104,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Modificado excel después de revisar varias tareas. Pendiente de sincronización de nombres entre modelos, vistas y controladores.
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -904,8 +904,8 @@
   </sheetPr>
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B31" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -920,7 +920,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="16.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="19.31"/>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="L8" s="16" t="n">
         <f aca="false">SUMIF(F4:F42,5,G4:G42)</f>
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="M8" s="16" t="n">
         <f aca="false">K8/60*15</f>
@@ -1298,15 +1298,15 @@
       </c>
       <c r="P8" s="5" t="n">
         <f aca="false">L8/60*15</f>
-        <v>36.25</v>
+        <v>38.75</v>
       </c>
       <c r="Q8" s="5" t="n">
         <f aca="false">L8/60*25</f>
-        <v>60.4166666666667</v>
+        <v>64.5833333333333</v>
       </c>
       <c r="R8" s="5" t="n">
         <f aca="false">Q8-P8</f>
-        <v>24.1666666666667</v>
+        <v>25.8333333333333</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="L9" s="5" t="n">
         <f aca="false">SUM(L4:L8)</f>
-        <v>697</v>
+        <v>707</v>
       </c>
       <c r="M9" s="5" t="n">
         <f aca="false">SUM(M4:M8)</f>
@@ -1356,15 +1356,15 @@
       </c>
       <c r="P9" s="17" t="n">
         <f aca="false">SUM(P4:P8)</f>
-        <v>174.25</v>
+        <v>176.75</v>
       </c>
       <c r="Q9" s="17" t="str">
         <f aca="false">FIXED(SUM(Q5:Q8))</f>
-        <v>207,08</v>
+        <v>211,25</v>
       </c>
       <c r="R9" s="17" t="str">
         <f aca="false">FIXED(SUM(R5:R8))</f>
-        <v>82,83</v>
+        <v>84,50</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>37</v>
@@ -1526,7 +1526,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="n">
         <v>13</v>
       </c>
@@ -1543,7 +1543,9 @@
       <c r="F16" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7" t="n">
+        <v>5</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -1576,7 +1578,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="n">
         <v>15</v>
       </c>
@@ -1593,7 +1595,9 @@
       <c r="F18" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G18" s="7"/>
+      <c r="G18" s="7" t="n">
+        <v>5</v>
+      </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -2344,7 +2348,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.37"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Modificado excel por un error.
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -171,10 +171,10 @@
     <t xml:space="preserve">Revisión de la tarea 7</t>
   </si>
   <si>
+    <t xml:space="preserve">Finalizada/Corregida</t>
+  </si>
+  <si>
     <t xml:space="preserve">Revisión de la tarea 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finalizada/Corregida</t>
   </si>
   <si>
     <t xml:space="preserve">En la correción en la línea 28 se cambio idgrupo por grupo porque estaba mal puesto,en lalínea 41 se cambio USUARIOS_GRUPO_ADD por USUARIOS_ADD y en la línea 61 USUARIOS_DELETE por USUARIOS_GRUPO_DELETE. En la línea 60 se cambió USUARIOS_GRUPO por USUARIOS_GRUPO_Model.  A mayores se añadieron comentarios para entender lo que se hacía</t>
@@ -904,8 +904,8 @@
   </sheetPr>
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1534,7 +1534,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="n">
@@ -1556,10 +1556,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>50</v>
@@ -1586,7 +1586,7 @@
         <v>51</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="n">
@@ -1983,7 +1983,7 @@
         <v>69</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7" t="n">
@@ -2354,7 +2354,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Actualizado excel revisada dos tareas
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ET3_GIT\EXCEL TAREAS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Estados">Hoja2!$A$1:$A$6</definedName>
-    <definedName name="EstadosVálidos">Hoja2!$A$1:$A$5</definedName>
+    <definedName function="false" hidden="false" name="Estados" vbProcedure="false">Hoja2!$A$1:$A$6</definedName>
+    <definedName function="false" hidden="false" name="EstadosVálidos" vbProcedure="false">Hoja2!$A$1:$A$5</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
   <si>
     <t>Semana 1(Del 20/10/2017 hasta 26/10/2017)</t>
   </si>
@@ -154,7 +150,7 @@
     <t>Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de los USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Creado el controladro: USUARIOS_GRUPO_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de USUARIO_GRUPO no se puede editar al ser claves.                              </t>
+    <t>Creado el controladro: USUARIOS_GRUPO_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de USUARIO_GRUPO no se puede editar al ser claves.                              </t>
   </si>
   <si>
     <t>Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
@@ -190,6 +186,9 @@
     <t>Revisión de la tarea 10</t>
   </si>
   <si>
+    <t>Se pusieron comillas en el value de los campos hidden de USUARIOS:GRUPO_DELETE.</t>
+  </si>
+  <si>
     <t>Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
   </si>
   <si>
@@ -208,6 +207,9 @@
     <t>Revisión de la tarea 17</t>
   </si>
   <si>
+    <t>Pendiente estandarización de nombres</t>
+  </si>
+  <si>
     <t>Revisión de la tarea 18</t>
   </si>
   <si>
@@ -244,6 +246,9 @@
     <t>Revisión de la tarea 24</t>
   </si>
   <si>
+    <t>Faltaron las comillas en el value de los campos hidden de ACCIONES_DELETE_view</t>
+  </si>
+  <si>
     <t>Revisión de la tarea 36</t>
   </si>
   <si>
@@ -296,22 +301,37 @@
   </si>
   <si>
     <t>Aplazada</t>
-  </si>
-  <si>
-    <t>Pendiente estandarización de nombres</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="22"/>
@@ -328,7 +348,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -346,7 +366,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDAE3F3"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFDBDBDB"/>
       </patternFill>
     </fill>
     <fill>
@@ -358,7 +378,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4C7E7"/>
-        <bgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF9DC3E6"/>
       </patternFill>
     </fill>
     <fill>
@@ -370,7 +390,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFFE699"/>
       </patternFill>
     </fill>
     <fill>
@@ -381,26 +401,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39994506668294322"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF9DC3E6"/>
+        <bgColor rgb="FFB4C7E7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="5">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
         <color rgb="FF2F5597"/>
       </left>
@@ -415,7 +435,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -424,99 +444,163 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyProtection="0">
-      <alignment wrapText="1"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
+  <cellStyles count="7">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFE699"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -530,7 +614,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBDBDB"/>
         </patternFill>
       </fill>
     </dxf>
@@ -544,21 +642,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
+          <bgColor rgb="FFC5E0B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -572,40 +656,25 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFFFE699"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C7E7"/>
@@ -627,12 +696,12 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFC5E0B4"/>
       <rgbColor rgb="FFFFE699"/>
-      <rgbColor rgb="FFC5E0B4"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FF9DC3E6"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF8CBAD"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -650,338 +719,64 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF2F5597"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="85.5546875" customWidth="1"/>
-    <col min="3" max="4" width="21.77734375" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" customWidth="1"/>
-    <col min="12" max="12" width="27.109375" customWidth="1"/>
-    <col min="13" max="15" width="16.109375" customWidth="1"/>
-    <col min="16" max="16" width="17.77734375" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" customWidth="1"/>
-    <col min="18" max="18" width="13" customWidth="1"/>
-    <col min="19" max="1025" width="8.33203125" customWidth="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="84.6377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1035,8 +830,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1046,57 +841,57 @@
         <v>19</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="7">
+      <c r="E4" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="7" t="n">
         <v>50</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="K4" s="5">
-        <f>SUMIF(F4:F28,1,E4:E28)</f>
+      <c r="K4" s="5" t="n">
+        <f aca="false">SUMIF(F4:F28,1,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L4" s="5">
-        <f>SUMIF(F4:F42,1,G4:G42)</f>
+      <c r="L4" s="5" t="n">
+        <f aca="false">SUMIF(F4:F42,1,G4:G42)</f>
         <v>200</v>
       </c>
-      <c r="M4" s="5">
-        <f>K4/60*15</f>
+      <c r="M4" s="5" t="n">
+        <f aca="false">K4/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N4" s="5">
-        <f>K4/60*25</f>
+      <c r="N4" s="5" t="n">
+        <f aca="false">K4/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O4" s="5">
-        <f>N4-M4</f>
+      <c r="O4" s="5" t="n">
+        <f aca="false">N4-M4</f>
         <v>45</v>
       </c>
-      <c r="P4" s="5">
-        <f>L4/60*15</f>
+      <c r="P4" s="5" t="n">
+        <f aca="false">L4/60*15</f>
         <v>50</v>
       </c>
-      <c r="Q4" s="5">
-        <f>L4/60*25</f>
-        <v>83.333333333333343</v>
-      </c>
-      <c r="R4" s="5">
-        <f>Q4-P4</f>
-        <v>33.333333333333343</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="Q4" s="5" t="n">
+        <f aca="false">L4/60*25</f>
+        <v>83.3333333333333</v>
+      </c>
+      <c r="R4" s="5" t="n">
+        <f aca="false">Q4-P4</f>
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1106,57 +901,57 @@
         <v>22</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="7">
+      <c r="E5" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K5" s="5">
-        <f>SUMIF(F4:F28,2,E4:E28)</f>
+      <c r="K5" s="5" t="n">
+        <f aca="false">SUMIF(F4:F28,2,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L5" s="5">
-        <f>SUMIF(F4:F42,2,G4:G42)</f>
+      <c r="L5" s="5" t="n">
+        <f aca="false">SUMIF(F4:F42,2,G4:G42)</f>
         <v>145</v>
       </c>
-      <c r="M5" s="5">
-        <f>K5/60*15</f>
+      <c r="M5" s="5" t="n">
+        <f aca="false">K5/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N5" s="5">
-        <f>K5/60*25</f>
+      <c r="N5" s="5" t="n">
+        <f aca="false">K5/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O5" s="5">
-        <f>N5-M5</f>
+      <c r="O5" s="5" t="n">
+        <f aca="false">N5-M5</f>
         <v>45</v>
       </c>
-      <c r="P5" s="5">
-        <f>L5/60*15</f>
+      <c r="P5" s="5" t="n">
+        <f aca="false">L5/60*15</f>
         <v>36.25</v>
       </c>
-      <c r="Q5" s="5">
-        <f>L5/60*25</f>
-        <v>60.416666666666664</v>
-      </c>
-      <c r="R5" s="5">
-        <f>Q5-P5</f>
-        <v>24.166666666666664</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="Q5" s="5" t="n">
+        <f aca="false">L5/60*25</f>
+        <v>60.4166666666667</v>
+      </c>
+      <c r="R5" s="5" t="n">
+        <f aca="false">Q5-P5</f>
+        <v>24.1666666666667</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1168,57 +963,57 @@
       <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="7" t="n">
         <v>22</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="K6" s="5">
-        <f>SUMIF(F4:F28,3,E4:E28)</f>
+      <c r="K6" s="5" t="n">
+        <f aca="false">SUMIF(F4:F28,3,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L6" s="5">
-        <f>SUMIF(F4:F42,3,G4:G42)</f>
+      <c r="L6" s="5" t="n">
+        <f aca="false">SUMIF(F4:F42,3,G4:G42)</f>
         <v>40</v>
       </c>
-      <c r="M6" s="5">
-        <f>K6/60*15</f>
+      <c r="M6" s="5" t="n">
+        <f aca="false">K6/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N6" s="5">
-        <f>K6/60*25</f>
+      <c r="N6" s="5" t="n">
+        <f aca="false">K6/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O6" s="5">
-        <f>N6-M6</f>
+      <c r="O6" s="5" t="n">
+        <f aca="false">N6-M6</f>
         <v>45</v>
       </c>
-      <c r="P6" s="5">
-        <f>L6/60*15</f>
+      <c r="P6" s="5" t="n">
+        <f aca="false">L6/60*15</f>
         <v>10</v>
       </c>
-      <c r="Q6" s="5">
-        <f>L6/60*25</f>
-        <v>16.666666666666664</v>
-      </c>
-      <c r="R6" s="5">
-        <f>Q6-P6</f>
-        <v>6.6666666666666643</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="Q6" s="5" t="n">
+        <f aca="false">L6/60*25</f>
+        <v>16.6666666666667</v>
+      </c>
+      <c r="R6" s="5" t="n">
+        <f aca="false">Q6-P6</f>
+        <v>6.66666666666666</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1230,57 +1025,57 @@
       <c r="D7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="7" t="n">
         <v>15</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="K7" s="5">
-        <f>SUMIF(F4:F28,4,E4:E28)</f>
+      <c r="K7" s="5" t="n">
+        <f aca="false">SUMIF(F4:F28,4,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="5">
-        <f>SUMIF(F4:F42,4,G4:G42)</f>
-        <v>192</v>
-      </c>
-      <c r="M7" s="5">
-        <f>K7/60*15</f>
+      <c r="L7" s="5" t="n">
+        <f aca="false">SUMIF(F4:F42,4,G4:G42)</f>
+        <v>212</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <f aca="false">K7/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N7" s="5">
-        <f>K7/60*25</f>
+      <c r="N7" s="5" t="n">
+        <f aca="false">K7/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O7" s="5">
-        <f>N7-M7</f>
+      <c r="O7" s="5" t="n">
+        <f aca="false">N7-M7</f>
         <v>45</v>
       </c>
-      <c r="P7" s="5">
-        <f>L7/60*15</f>
-        <v>48</v>
-      </c>
-      <c r="Q7" s="5">
-        <f>L7/60*25</f>
-        <v>80</v>
-      </c>
-      <c r="R7" s="5">
-        <f>Q7-P7</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="P7" s="5" t="n">
+        <f aca="false">L7/60*15</f>
+        <v>53</v>
+      </c>
+      <c r="Q7" s="5" t="n">
+        <f aca="false">L7/60*25</f>
+        <v>88.3333333333333</v>
+      </c>
+      <c r="R7" s="5" t="n">
+        <f aca="false">Q7-P7</f>
+        <v>35.3333333333333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
@@ -1292,57 +1087,57 @@
       <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="7" t="n">
         <v>30</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="K8" s="16">
-        <f>SUMIF(F4:F28,5,E4:E28)</f>
+      <c r="K8" s="16" t="n">
+        <f aca="false">SUMIF(F4:F28,5,E4:E28)</f>
         <v>270</v>
       </c>
-      <c r="L8" s="16">
-        <f>SUMIF(F4:F42,5,G4:G42)</f>
+      <c r="L8" s="16" t="n">
+        <f aca="false">SUMIF(F4:F42,5,G4:G42)</f>
         <v>155</v>
       </c>
-      <c r="M8" s="16">
-        <f>K8/60*15</f>
+      <c r="M8" s="16" t="n">
+        <f aca="false">K8/60*15</f>
         <v>67.5</v>
       </c>
-      <c r="N8" s="5">
-        <f>K8/60*25</f>
+      <c r="N8" s="5" t="n">
+        <f aca="false">K8/60*25</f>
         <v>112.5</v>
       </c>
-      <c r="O8" s="5">
-        <f>N8-M8</f>
+      <c r="O8" s="5" t="n">
+        <f aca="false">N8-M8</f>
         <v>45</v>
       </c>
-      <c r="P8" s="5">
-        <f>L8/60*15</f>
+      <c r="P8" s="5" t="n">
+        <f aca="false">L8/60*15</f>
         <v>38.75</v>
       </c>
-      <c r="Q8" s="5">
-        <f>L8/60*25</f>
-        <v>64.583333333333343</v>
-      </c>
-      <c r="R8" s="5">
-        <f>Q8-P8</f>
-        <v>25.833333333333343</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="Q8" s="5" t="n">
+        <f aca="false">L8/60*25</f>
+        <v>64.5833333333333</v>
+      </c>
+      <c r="R8" s="5" t="n">
+        <f aca="false">Q8-P8</f>
+        <v>25.8333333333333</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1354,56 +1149,56 @@
       <c r="D9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="5">
-        <f t="shared" ref="K9:P9" si="0">SUM(K4:K8)</f>
+      <c r="K9" s="5" t="n">
+        <f aca="false">SUM(K4:K8)</f>
         <v>1350</v>
       </c>
-      <c r="L9" s="5">
-        <f t="shared" si="0"/>
-        <v>732</v>
-      </c>
-      <c r="M9" s="5">
-        <f t="shared" si="0"/>
+      <c r="L9" s="5" t="n">
+        <f aca="false">SUM(L4:L8)</f>
+        <v>752</v>
+      </c>
+      <c r="M9" s="5" t="n">
+        <f aca="false">SUM(M4:M8)</f>
         <v>337.5</v>
       </c>
-      <c r="N9" s="17">
-        <f t="shared" si="0"/>
+      <c r="N9" s="17" t="n">
+        <f aca="false">SUM(N4:N8)</f>
         <v>562.5</v>
       </c>
-      <c r="O9" s="17">
-        <f t="shared" si="0"/>
+      <c r="O9" s="17" t="n">
+        <f aca="false">SUM(O4:O8)</f>
         <v>225</v>
       </c>
-      <c r="P9" s="17">
-        <f t="shared" si="0"/>
-        <v>183</v>
+      <c r="P9" s="17" t="n">
+        <f aca="false">SUM(P4:P8)</f>
+        <v>188</v>
       </c>
       <c r="Q9" s="17" t="str">
-        <f>FIXED(SUM(Q5:Q8))</f>
-        <v>221,67</v>
+        <f aca="false">FIXED(SUM(Q5:Q8))</f>
+        <v>230,00</v>
       </c>
       <c r="R9" s="17" t="str">
-        <f>FIXED(SUM(R5:R8))</f>
-        <v>88,67</v>
+        <f aca="false">FIXED(SUM(R5:R8))</f>
+        <v>92,00</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+    <row r="10" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1415,13 +1210,13 @@
       <c r="D10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="7" t="n">
         <v>26</v>
       </c>
       <c r="H10" s="5"/>
@@ -1429,8 +1224,8 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+    <row r="11" customFormat="false" ht="129.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1442,13 +1237,13 @@
       <c r="D11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="7" t="n">
         <v>35</v>
       </c>
       <c r="H11" s="5"/>
@@ -1456,8 +1251,8 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
+    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1467,13 +1262,13 @@
         <v>22</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="7">
+      <c r="E12" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H12" s="5"/>
@@ -1481,8 +1276,8 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+    <row r="13" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1494,13 +1289,13 @@
       <c r="D13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H13" s="5"/>
@@ -1508,8 +1303,8 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+    <row r="14" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
         <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1521,13 +1316,13 @@
       <c r="D14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="7" t="n">
         <v>15</v>
       </c>
       <c r="H14" s="5"/>
@@ -1535,8 +1330,8 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="n">
         <v>12</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -1546,10 +1341,10 @@
         <v>22</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="7">
+      <c r="E15" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="7" t="n">
         <v>3</v>
       </c>
       <c r="G15" s="7"/>
@@ -1558,8 +1353,8 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="n">
         <v>13</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -1569,13 +1364,13 @@
         <v>48</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="7">
+      <c r="E16" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="7" t="n">
         <v>5</v>
       </c>
       <c r="H16" s="5"/>
@@ -1583,8 +1378,8 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+    <row r="17" customFormat="false" ht="273.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="n">
         <v>14</v>
       </c>
       <c r="B17" s="14" t="s">
@@ -1596,13 +1391,13 @@
       <c r="D17" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="7" t="n">
         <v>33</v>
       </c>
       <c r="H17" s="5"/>
@@ -1610,8 +1405,8 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
+    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="n">
         <v>15</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -1621,13 +1416,13 @@
         <v>48</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="7">
+      <c r="E18" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="7" t="n">
         <v>5</v>
       </c>
       <c r="H18" s="5"/>
@@ -1635,49 +1430,53 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
+    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="n">
         <v>16</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7">
+        <v>48</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G19" s="7"/>
+      <c r="G19" s="7" t="n">
+        <v>10</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
+    <row r="20" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="n">
         <v>17</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="7">
+        <v>55</v>
+      </c>
+      <c r="E20" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="7" t="n">
         <v>25</v>
       </c>
       <c r="H20" s="5"/>
@@ -1685,26 +1484,26 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
+    <row r="21" customFormat="false" ht="115.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="n">
         <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="7">
+        <v>57</v>
+      </c>
+      <c r="E21" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="7" t="n">
         <v>40</v>
       </c>
       <c r="H21" s="5"/>
@@ -1712,21 +1511,21 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
+    <row r="22" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="n">
         <v>19</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="7">
+      <c r="E22" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="7" t="n">
         <v>3</v>
       </c>
       <c r="G22" s="7"/>
@@ -1735,26 +1534,26 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+    <row r="23" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="n">
         <v>20</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="7">
+        <v>60</v>
+      </c>
+      <c r="E23" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="7" t="n">
         <v>25</v>
       </c>
       <c r="H23" s="5"/>
@@ -1762,21 +1561,21 @@
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
+    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="n">
         <v>21</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="7">
+      <c r="E24" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="7" t="n">
         <v>3</v>
       </c>
       <c r="G24" s="7"/>
@@ -1785,21 +1584,21 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
+    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
         <v>22</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="7"/>
-      <c r="E25" s="7">
+      <c r="E25" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="7" t="n">
         <v>5</v>
       </c>
       <c r="G25" s="7"/>
@@ -1808,26 +1607,26 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
+    <row r="26" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="n">
         <v>23</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="7">
+        <v>64</v>
+      </c>
+      <c r="E26" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="7" t="n">
         <v>21</v>
       </c>
       <c r="H26" s="5"/>
@@ -1835,26 +1634,26 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
+    <row r="27" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="n">
         <v>24</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="7">
+        <v>66</v>
+      </c>
+      <c r="E27" s="7" t="n">
         <v>70</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="7" t="n">
         <v>40</v>
       </c>
       <c r="H27" s="5"/>
@@ -1862,8 +1661,8 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
+    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="n">
         <v>25</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -1873,10 +1672,10 @@
         <v>22</v>
       </c>
       <c r="D28" s="7"/>
-      <c r="E28" s="7">
+      <c r="E28" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="7" t="n">
         <v>1</v>
       </c>
       <c r="G28" s="7"/>
@@ -1885,8 +1684,8 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
+    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1898,8 +1697,8 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
+    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1911,8 +1710,8 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
+    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1924,8 +1723,8 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
+    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1937,8 +1736,8 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
+    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1950,8 +1749,8 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
+    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1963,10 +1762,10 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
+    <row r="35" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1"/>
       <c r="B35" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>3</v>
@@ -1978,7 +1777,7 @@
         <v>5</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>7</v>
@@ -1988,24 +1787,24 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
+    <row r="36" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1"/>
       <c r="B36" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="7">
+        <v>70</v>
+      </c>
+      <c r="E36" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="7" t="n">
         <v>30</v>
       </c>
       <c r="H36" s="5"/>
@@ -2013,22 +1812,22 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
+    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1"/>
       <c r="B37" s="14" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="7">
+      <c r="E37" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H37" s="5"/>
@@ -2036,35 +1835,41 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
+    <row r="38" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1"/>
       <c r="B38" s="14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7">
+        <v>48</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
+      <c r="F38" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="G38" s="7" t="n">
+        <v>10</v>
+      </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
+    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1"/>
       <c r="B39" s="14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="7">
+      <c r="E39" s="7" t="n">
         <v>30</v>
       </c>
       <c r="F39" s="7"/>
@@ -2074,24 +1879,24 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
     </row>
-    <row r="40" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
+    <row r="40" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1"/>
       <c r="B40" s="8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E40" s="7">
+        <v>76</v>
+      </c>
+      <c r="E40" s="7" t="n">
         <v>100</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40" s="7" t="n">
         <v>90</v>
       </c>
       <c r="H40" s="5"/>
@@ -2099,24 +1904,24 @@
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
     </row>
-    <row r="41" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
+    <row r="41" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1"/>
       <c r="B41" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E41" s="7">
+        <v>78</v>
+      </c>
+      <c r="E41" s="7" t="n">
         <v>120</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G41" s="7">
+      <c r="G41" s="7" t="n">
         <v>45</v>
       </c>
       <c r="H41" s="5"/>
@@ -2124,24 +1929,24 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="2"/>
+    <row r="42" customFormat="false" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1"/>
       <c r="B42" s="8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E42" s="7">
+        <v>80</v>
+      </c>
+      <c r="E42" s="7" t="n">
         <v>90</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G42" s="7" t="n">
         <v>80</v>
       </c>
       <c r="H42" s="5"/>
@@ -2149,24 +1954,24 @@
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
     </row>
-    <row r="43" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
+    <row r="43" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1"/>
       <c r="B43" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="7">
+        <v>60</v>
+      </c>
+      <c r="E43" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F43" s="19">
+      <c r="F43" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G43" s="7">
+      <c r="G43" s="7" t="n">
         <v>20</v>
       </c>
       <c r="H43" s="5"/>
@@ -2174,35 +1979,35 @@
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
+    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1"/>
       <c r="B44" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D44" s="7"/>
-      <c r="E44" s="7">
+      <c r="E44" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F44" s="20"/>
+      <c r="F44" s="19"/>
       <c r="G44" s="7"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
+    <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1"/>
       <c r="B45" s="14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="7">
+      <c r="E45" s="7" t="n">
         <v>30</v>
       </c>
       <c r="F45" s="7"/>
@@ -2212,16 +2017,16 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="2"/>
+    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1"/>
       <c r="B46" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D46" s="7"/>
-      <c r="E46" s="7">
+      <c r="E46" s="7" t="n">
         <v>90</v>
       </c>
       <c r="F46" s="7"/>
@@ -2231,16 +2036,16 @@
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
+    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1"/>
       <c r="B47" s="8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D47" s="7"/>
-      <c r="E47" s="7">
+      <c r="E47" s="7" t="n">
         <v>90</v>
       </c>
       <c r="F47" s="7"/>
@@ -2250,16 +2055,16 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="2"/>
+    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1"/>
       <c r="B48" s="8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D48" s="7"/>
-      <c r="E48" s="7">
+      <c r="E48" s="7" t="n">
         <v>90</v>
       </c>
       <c r="F48" s="7"/>
@@ -2269,16 +2074,16 @@
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
+    <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1"/>
       <c r="B49" s="8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D49" s="7"/>
-      <c r="E49" s="7">
+      <c r="E49" s="7" t="n">
         <v>90</v>
       </c>
       <c r="F49" s="7"/>
@@ -2288,16 +2093,16 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
     </row>
-    <row r="50" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
+    <row r="50" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1"/>
       <c r="B50" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D50" s="7"/>
-      <c r="E50" s="7">
+      <c r="E50" s="7" t="n">
         <v>120</v>
       </c>
       <c r="F50" s="7"/>
@@ -2307,14 +2112,14 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B51" s="18" t="s">
-        <v>86</v>
+    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="7" t="n">
         <v>30</v>
       </c>
     </row>
@@ -2323,101 +2128,114 @@
     <mergeCell ref="B1:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F28">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:J8">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36:F42">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C28 C36:C51">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C28 C36:C51" type="list">
       <formula1>Estados</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="1025" width="8.33203125" customWidth="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambio de estado de las tareas corregidas por el recurso 5 a finalizado/corregido.
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,280 +27,280 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
   <si>
-    <t>Semana 1(Del 20/10/2017 hasta 26/10/2017)</t>
-  </si>
-  <si>
-    <t>nº Tarea</t>
-  </si>
-  <si>
-    <t>Tareas principales</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Observaciones</t>
-  </si>
-  <si>
-    <t>Tiempo planificado (min)</t>
-  </si>
-  <si>
-    <t>Recurso asociado</t>
-  </si>
-  <si>
-    <t>Tiempo empleado (min)</t>
-  </si>
-  <si>
-    <t>Recursos</t>
-  </si>
-  <si>
-    <t>Código asociado</t>
-  </si>
-  <si>
-    <t>Tiempo planificado total (min)</t>
-  </si>
-  <si>
-    <t>Tiempo empleado total (min)</t>
-  </si>
-  <si>
-    <t>Coste por hora planificado</t>
-  </si>
-  <si>
-    <t>Ingresos planificados</t>
-  </si>
-  <si>
-    <t>Beneficio planificado</t>
-  </si>
-  <si>
-    <t>Coste por hora planificado utilizado</t>
-  </si>
-  <si>
-    <t>Ingresos reales</t>
-  </si>
-  <si>
-    <t>Beneficio real</t>
-  </si>
-  <si>
-    <t>Organizar y asignar tareas: Semana 1</t>
-  </si>
-  <si>
-    <t>Finalizada</t>
-  </si>
-  <si>
-    <t>Miguel Ferreiro Díaz</t>
-  </si>
-  <si>
-    <t>Gestión de usuarios:  Modificar controladores para adaptarlo al nuevo modelo de datos</t>
-  </si>
-  <si>
-    <t>Sin empezar</t>
-  </si>
-  <si>
-    <t>Alejandro Vila Cid</t>
-  </si>
-  <si>
-    <t>Gestión de usuarios:  Modificar modelos para adaptarlo al nuevo modelo de datos</t>
-  </si>
-  <si>
-    <t>Pendiente de correción</t>
-  </si>
-  <si>
-    <t>Nombre del modelo:USUARIOS_MODEL</t>
-  </si>
-  <si>
-    <t>Jonatan Couto Riádigos</t>
-  </si>
-  <si>
-    <t>Gestión de usuarios:  Modificar vistas para adapartalo al nuevo modelo de datos</t>
-  </si>
-  <si>
-    <t>Paralizada</t>
-  </si>
-  <si>
-    <t>Modificados valores para asegurar la concordancia con el modelo</t>
-  </si>
-  <si>
-    <t>Brais Santos Negreira</t>
-  </si>
-  <si>
-    <t>Planteamiento incicial de modelos de secuencia para la gestión de grupos de usuario, permisos de usuario y gestión de acciones</t>
-  </si>
-  <si>
-    <t>Creado modelo de secuencia empleando visual paradigm</t>
-  </si>
-  <si>
-    <t>Brais Rodríguez Martínez</t>
-  </si>
-  <si>
-    <t>Gestion de grupos de usuario: Crear modelo de datos para  la tabla USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Creados el modelo de USUARIO_GRUPO</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Gestion de grupos de usuario: Crear modelo de datos para  la tabla GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Nombre del modelo:GRUPO_MODEL</t>
-  </si>
-  <si>
-    <t>Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de los USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Creado el controladro: USUARIOS_GRUPO_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de USUARIO_GRUPO no se puede editar al ser claves.                              </t>
-  </si>
-  <si>
-    <t>Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Gestión de grupos de usuario: Crear vistas  las posibles acciones sobre la tabla USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Creadas las vistas de acuerdo a los atributos actuales</t>
-  </si>
-  <si>
-    <t>Gestión de grupos de usuario: Crear vistas para las posibles acciones sobre la tabla GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 6</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 7</t>
-  </si>
-  <si>
-    <t>Finalizada/Corregida</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 8</t>
-  </si>
-  <si>
-    <t>En la correción en la línea 28 se cambio idgrupo por grupo porque estaba mal puesto,en lalínea 41 se cambio USUARIOS_GRUPO_ADD por USUARIOS_ADD y en la línea 61 USUARIOS_DELETE por USUARIOS_GRUPO_DELETE. En la línea 60 se cambió USUARIOS_GRUPO por USUARIOS_GRUPO_Model.  A mayores se añadieron comentarios para entender lo que se hacía</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 9</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 10</t>
-  </si>
-  <si>
-    <t>Se pusieron comillas en el value de los campos hidden de USUARIOS:GRUPO_DELETE.</t>
-  </si>
-  <si>
-    <t>Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Creado el model de permisos</t>
-  </si>
-  <si>
-    <t>Gestion de permisos de usuario:  Crear controlador de datos para la tabla PERMISOS.  (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Creado el controladro: PERMISOS_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de  PERMISOS no se puede editar al ser claves.</t>
-  </si>
-  <si>
-    <t>Gestion de permisos de usuario:  Crear vistas para las posibles acciones sobre la tabla PERMISOS.   (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 17</t>
-  </si>
-  <si>
-    <t>Pendiente estandarización de nombres</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 18</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 19</t>
-  </si>
-  <si>
-    <t>Gestión de acciones:  Crear modelo de datos para ACCIONES</t>
-  </si>
-  <si>
-    <t>Nombre del modelo:ACCIONES_MODEL</t>
-  </si>
-  <si>
-    <t>Gestión de acciones: Crear vistas para ACCIONES</t>
-  </si>
-  <si>
-    <t>Estructura provisional de las vistas para acciones</t>
-  </si>
-  <si>
-    <t>Tareas extra</t>
-  </si>
-  <si>
-    <t>Recursos asociado</t>
-  </si>
-  <si>
-    <t>Gestión de acciones: Crear controlador de datos para ACCIONES</t>
-  </si>
-  <si>
-    <t>Falta solucionar como se trataría el borrado de un acción</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 23</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 24</t>
-  </si>
-  <si>
-    <t>Faltaron las comillas en el value de los campos hidden de ACCIONES_DELETE_view</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 36</t>
-  </si>
-  <si>
-    <t>Gestion de funcionalidades: Crear modelo de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t>Nombres de modelo:FUNCIONALIDAD_MODEL y FUNC_ACCION_MODEL</t>
-  </si>
-  <si>
-    <t>Gestion de funcionalidades: Crear controlador de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t>Falta solucionar como se trataría el borrado de una funcionalidad y de funcionalidad_accion</t>
-  </si>
-  <si>
-    <t>Gestion de funcionalidades: Crear vistas para las posibles acciones sobre las tablas FUNCIONALIDADES Y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t>Creadas las vistas correspondientes excepto  edit en funcionalidad_accion ya que los atributos son todos claves</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 40</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 41</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 42</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: USUARIO, USUARIO_GRUPO y GRUPO.</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: PERMISO y GRUPO.</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION.</t>
-  </si>
-  <si>
-    <t>Implementar el control sobre los usuarios que pertenecen a uno o varios grupos y tienen unos ciertos permisos.</t>
-  </si>
-  <si>
-    <t>Revisión de la tarea 11</t>
-  </si>
-  <si>
-    <t>En proceso</t>
-  </si>
-  <si>
-    <t>Aplazada</t>
+    <t xml:space="preserve">Semana 1(Del 20/10/2017 hasta 26/10/2017)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nº Tarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tareas principales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiempo planificado (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurso asociado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiempo empleado (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recursos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código asociado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiempo planificado total (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiempo empleado total (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coste por hora planificado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresos planificados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beneficio planificado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coste por hora planificado utilizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresos reales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beneficio real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organizar y asignar tareas: Semana 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalizada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miguel Ferreiro Díaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de usuarios:  Modificar controladores para adaptarlo al nuevo modelo de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin empezar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alejandro Vila Cid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de usuarios:  Modificar modelos para adaptarlo al nuevo modelo de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pendiente de correción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre del modelo:USUARIOS_MODEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonatan Couto Riádigos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de usuarios:  Modificar vistas para adapartalo al nuevo modelo de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paralizada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificados valores para asegurar la concordancia con el modelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brais Santos Negreira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planteamiento incicial de modelos de secuencia para la gestión de grupos de usuario, permisos de usuario y gestión de acciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creado modelo de secuencia empleando visual paradigm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brais Rodríguez Martínez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de grupos de usuario: Crear modelo de datos para  la tabla USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creados el modelo de USUARIO_GRUPO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de grupos de usuario: Crear modelo de datos para  la tabla GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalizada/Corregida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre del modelo:GRUPO_MODEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de los USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creado el controladro: USUARIOS_GRUPO_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de USUARIO_GRUPO no se puede editar al ser claves.                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de grupos de usuario: Crear vistas  las posibles acciones sobre la tabla USUARIO_GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creadas las vistas de acuerdo a los atributos actuales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de grupos de usuario: Crear vistas para las posibles acciones sobre la tabla GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En la correción en la línea 28 se cambio idgrupo por grupo porque estaba mal puesto,en lalínea 41 se cambio USUARIOS_GRUPO_ADD por USUARIOS_ADD y en la línea 61 USUARIOS_DELETE por USUARIOS_GRUPO_DELETE. En la línea 60 se cambió USUARIOS_GRUPO por USUARIOS_GRUPO_Model.  A mayores se añadieron comentarios para entender lo que se hacía</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se pusieron comillas en el value de los campos hidden de USUARIOS:GRUPO_DELETE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creado el model de permisos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de permisos de usuario:  Crear controlador de datos para la tabla PERMISOS.  (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creado el controladro: PERMISOS_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de  PERMISOS no se puede editar al ser claves.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de permisos de usuario:  Crear vistas para las posibles acciones sobre la tabla PERMISOS.   (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pendiente estandarización de nombres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de acciones:  Crear modelo de datos para ACCIONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre del modelo:ACCIONES_MODEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de acciones: Crear vistas para ACCIONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estructura provisional de las vistas para acciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tareas extra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recursos asociado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de acciones: Crear controlador de datos para ACCIONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta solucionar como se trataría el borrado de un acción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faltaron las comillas en el value de los campos hidden de ACCIONES_DELETE_view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de funcionalidades: Crear modelo de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombres de modelo:FUNCIONALIDAD_MODEL y FUNC_ACCION_MODEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de funcionalidades: Crear controlador de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta solucionar como se trataría el borrado de una funcionalidad y de funcionalidad_accion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de funcionalidades: Crear vistas para las posibles acciones sobre las tablas FUNCIONALIDADES Y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creadas las vistas correspondientes excepto  edit en funcionalidad_accion ya que los atributos son todos claves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tratamiento del borrado entre las tablas: USUARIO, USUARIO_GRUPO y GRUPO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tratamiento del borrado entre las tablas: PERMISO y GRUPO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar el control sobre los usuarios que pertenecen a uno o varios grupos y tienen unos ciertos permisos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisión de la tarea 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En proceso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplazada</t>
   </si>
 </sst>
 </file>
@@ -308,9 +308,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -332,6 +332,87 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="22"/>
@@ -356,7 +437,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,8 +446,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFC5E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFF8CBAD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFDBDBDB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDAE3F3"/>
-        <bgColor rgb="FFDBDBDB"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -390,7 +513,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
-        <bgColor rgb="FFFFE699"/>
+        <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -412,12 +535,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -459,7 +597,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -483,7 +621,55 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -496,15 +682,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,7 +698,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -528,59 +714,75 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -665,16 +867,16 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C7E7"/>
@@ -696,12 +898,12 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFDBDBDB"/>
-      <rgbColor rgb="FFC5E0B4"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFE699"/>
       <rgbColor rgb="FF9DC3E6"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFDBDBDB"/>
       <rgbColor rgb="FFF8CBAD"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -710,7 +912,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFC5E0B4"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -731,28 +933,28 @@
   </sheetPr>
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="84.6377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.10204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="84.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="21.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="15.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1197,7 +1399,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="n">
         <v>7</v>
       </c>
@@ -1205,10 +1407,10 @@
         <v>38</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E10" s="7" t="n">
         <v>90</v>
@@ -1229,13 +1431,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="7" t="n">
         <v>90</v>
@@ -1251,15 +1453,15 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="n">
@@ -1281,13 +1483,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" s="7" t="n">
         <v>60</v>
@@ -1308,13 +1510,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E14" s="7" t="n">
         <v>60</v>
@@ -1335,7 +1537,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>22</v>
@@ -1358,10 +1560,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="n">
@@ -1386,7 +1588,7 @@
         <v>49</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>50</v>
@@ -1413,7 +1615,7 @@
         <v>51</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="n">
@@ -1438,7 +1640,7 @@
         <v>52</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>53</v>
@@ -1542,7 +1744,7 @@
         <v>59</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>60</v>
@@ -1818,7 +2020,7 @@
         <v>71</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7" t="n">
@@ -1841,7 +2043,7 @@
         <v>72</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>73</v>
@@ -1960,7 +2162,7 @@
         <v>81</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>60</v>
@@ -2174,7 +2376,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2189,19 +2391,19 @@
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,7 +2434,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Modificado el excel con las revisiones del recurso 5. FIN DE PRIMERA SEMANA.
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="93">
   <si>
     <t xml:space="preserve">Semana 1(Del 20/10/2017 hasta 26/10/2017)</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t xml:space="preserve">Revisión de la tarea 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corregidas algunas referencias a controladores y clases. Eliminado edit porque los atributos son clave.</t>
   </si>
   <si>
     <t xml:space="preserve">Gestión de acciones:  Crear modelo de datos para ACCIONES</t>
@@ -933,8 +936,8 @@
   </sheetPr>
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -944,14 +947,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="21.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="15.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.1"/>
@@ -1311,7 +1314,7 @@
       </c>
       <c r="L8" s="16" t="n">
         <f aca="false">SUMIF(F4:F42,5,G4:G42)</f>
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="M8" s="16" t="n">
         <f aca="false">K8/60*15</f>
@@ -1327,15 +1330,15 @@
       </c>
       <c r="P8" s="5" t="n">
         <f aca="false">L8/60*15</f>
-        <v>38.75</v>
+        <v>43.75</v>
       </c>
       <c r="Q8" s="5" t="n">
         <f aca="false">L8/60*25</f>
-        <v>64.5833333333333</v>
+        <v>72.9166666666667</v>
       </c>
       <c r="R8" s="5" t="n">
         <f aca="false">Q8-P8</f>
-        <v>25.8333333333333</v>
+        <v>29.1666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1369,7 +1372,7 @@
       </c>
       <c r="L9" s="5" t="n">
         <f aca="false">SUM(L4:L8)</f>
-        <v>752</v>
+        <v>772</v>
       </c>
       <c r="M9" s="5" t="n">
         <f aca="false">SUM(M4:M8)</f>
@@ -1385,15 +1388,15 @@
       </c>
       <c r="P9" s="17" t="n">
         <f aca="false">SUM(P4:P8)</f>
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="Q9" s="17" t="str">
         <f aca="false">FIXED(SUM(Q5:Q8))</f>
-        <v>230,00</v>
+        <v>238,33</v>
       </c>
       <c r="R9" s="17" t="str">
         <f aca="false">FIXED(SUM(R5:R8))</f>
-        <v>92,00</v>
+        <v>95,33</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>37</v>
@@ -1713,7 +1716,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="n">
         <v>19</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>58</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="n">
@@ -1786,7 +1789,7 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="52.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="n">
         <v>22</v>
       </c>
@@ -1794,33 +1797,37 @@
         <v>62</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="E25" s="7" t="n">
         <v>20</v>
       </c>
       <c r="F25" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G25" s="7"/>
+      <c r="G25" s="7" t="n">
+        <v>20</v>
+      </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="31.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="n">
         <v>23</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E26" s="7" t="n">
         <v>100</v>
@@ -1841,13 +1848,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E27" s="7" t="n">
         <v>70</v>
@@ -1967,7 +1974,7 @@
     <row r="35" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
       <c r="B35" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>3</v>
@@ -1979,7 +1986,7 @@
         <v>5</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>7</v>
@@ -1992,13 +1999,13 @@
     <row r="36" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
       <c r="B36" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E36" s="7" t="n">
         <v>120</v>
@@ -2017,7 +2024,7 @@
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1"/>
       <c r="B37" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>39</v>
@@ -2040,13 +2047,13 @@
     <row r="38" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1"/>
       <c r="B38" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E38" s="7" t="n">
         <v>30</v>
@@ -2065,7 +2072,7 @@
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
       <c r="B39" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>22</v>
@@ -2084,13 +2091,13 @@
     <row r="40" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>
       <c r="B40" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E40" s="7" t="n">
         <v>100</v>
@@ -2109,13 +2116,13 @@
     <row r="41" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
       <c r="B41" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E41" s="7" t="n">
         <v>120</v>
@@ -2134,13 +2141,13 @@
     <row r="42" customFormat="false" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
       <c r="B42" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E42" s="7" t="n">
         <v>90</v>
@@ -2159,7 +2166,7 @@
     <row r="43" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
       <c r="B43" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>39</v>
@@ -2184,7 +2191,7 @@
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1"/>
       <c r="B44" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>22</v>
@@ -2203,7 +2210,7 @@
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
       <c r="B45" s="14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>22</v>
@@ -2222,7 +2229,7 @@
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1"/>
       <c r="B46" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>22</v>
@@ -2241,7 +2248,7 @@
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1"/>
       <c r="B47" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>22</v>
@@ -2260,7 +2267,7 @@
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1"/>
       <c r="B48" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>22</v>
@@ -2279,7 +2286,7 @@
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1"/>
       <c r="B49" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>22</v>
@@ -2298,7 +2305,7 @@
     <row r="50" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
       <c r="B50" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>22</v>
@@ -2316,7 +2323,7 @@
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>22</v>
@@ -2397,7 +2404,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.1"/>
   </cols>
   <sheetData>
@@ -2408,7 +2415,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2423,7 +2430,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Añadidas las vistas, controlador y modelo de la tabla TRABAJO. Modificado el excel.
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="216">
   <si>
     <t xml:space="preserve">Semana 1(Del 20/11/2017 hasta 26/11/2017)</t>
   </si>
@@ -1191,6 +1191,12 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Pendiente de correción</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creados los elementos correspondientes según la guía de nombres</t>
+  </si>
+  <si>
     <t xml:space="preserve">Revisión y corrección de las tarea 34.</t>
   </si>
   <si>
@@ -2199,9 +2205,6 @@
   </si>
   <si>
     <t xml:space="preserve">Aplazada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendiente de correción</t>
   </si>
 </sst>
 </file>
@@ -2584,7 +2587,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2757,14 +2760,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2791,7 +2786,7 @@
     <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="37">
     <dxf>
       <fill>
         <patternFill>
@@ -2900,20 +2895,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFE699"/>
         </patternFill>
       </fill>
@@ -2943,6 +2924,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB4C7E7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3057,275 +3052,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3413,13 +3139,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="8.14"/>
@@ -4959,8 +4685,8 @@
   </sheetPr>
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5149,11 +4875,11 @@
       </c>
       <c r="AA4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Sin empezar")</f>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Pendiente de correción")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Aplazada")</f>
@@ -5246,11 +4972,11 @@
       </c>
       <c r="AA5" s="0" t="n">
         <f aca="false">AA4/AD4 *100</f>
-        <v>78.5714285714286</v>
+        <v>76.1904761904762</v>
       </c>
       <c r="AB5" s="0" t="n">
         <f aca="false">AB4/AD4*100</f>
-        <v>0</v>
+        <v>2.38095238095238</v>
       </c>
       <c r="AC5" s="0" t="n">
         <f aca="false">AC4/AD4 *100</f>
@@ -5421,11 +5147,11 @@
       </c>
       <c r="L8" s="8" t="n">
         <f aca="false">SUMIF(F4:F121,5,G4:G121)</f>
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="M8" s="8" t="n">
         <f aca="false">K8-L8</f>
-        <v>450</v>
+        <v>390</v>
       </c>
       <c r="N8" s="28" t="n">
         <f aca="false">K8/60*15</f>
@@ -5441,15 +5167,15 @@
       </c>
       <c r="Q8" s="8" t="n">
         <f aca="false">L8/60*15</f>
-        <v>42.5</v>
+        <v>57.5</v>
       </c>
       <c r="R8" s="8" t="n">
         <f aca="false">L8/60*25</f>
-        <v>70.8333333333333</v>
+        <v>95.8333333333333</v>
       </c>
       <c r="S8" s="8" t="n">
         <f aca="false">R8-Q8</f>
-        <v>28.3333333333333</v>
+        <v>38.3333333333333</v>
       </c>
       <c r="T8" s="2"/>
     </row>
@@ -5479,11 +5205,11 @@
       </c>
       <c r="L9" s="29" t="n">
         <f aca="false">SUM(L4:L8)</f>
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="M9" s="29" t="n">
         <f aca="false">SUM(M4:M8)</f>
-        <v>1845</v>
+        <v>1785</v>
       </c>
       <c r="N9" s="8" t="n">
         <f aca="false">SUM(N4:N8)</f>
@@ -5499,15 +5225,15 @@
       </c>
       <c r="Q9" s="29" t="n">
         <f aca="false">SUM(Q4:Q8)</f>
-        <v>42.5</v>
+        <v>57.5</v>
       </c>
       <c r="R9" s="29" t="str">
         <f aca="false">FIXED(SUM(R5:R8))</f>
-        <v>70,83</v>
+        <v>95,83</v>
       </c>
       <c r="S9" s="29" t="str">
         <f aca="false">FIXED(SUM(S5:S8))</f>
-        <v>28,33</v>
+        <v>38,33</v>
       </c>
       <c r="T9" s="5" t="s">
         <v>45</v>
@@ -5988,7 +5714,7 @@
       </c>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="31.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="n">
         <v>34</v>
       </c>
@@ -5996,23 +5722,27 @@
         <v>123</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="11"/>
+        <v>124</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="E35" s="8" t="n">
         <v>120</v>
       </c>
       <c r="F35" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="G35" s="8"/>
+      <c r="G35" s="8" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>94</v>
@@ -6031,7 +5761,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>94</v>
@@ -6050,7 +5780,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>94</v>
@@ -6067,7 +5797,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>94</v>
@@ -6084,7 +5814,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>94</v>
@@ -6101,7 +5831,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>94</v>
@@ -6118,7 +5848,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>94</v>
@@ -6135,7 +5865,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>94</v>
@@ -6152,7 +5882,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>94</v>
@@ -6169,7 +5899,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>94</v>
@@ -6229,52 +5959,24 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C:C">
-    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
-      <formula>"Sin empezar"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
-      <formula>"Finalizada/Corregida"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>"Paralizada"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F:F">
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+  <conditionalFormatting sqref="F15:F19">
+    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F19">
-    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6301,7 +6003,7 @@
   </sheetPr>
   <dimension ref="A1:T111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G105" activeCellId="0" sqref="G105"/>
     </sheetView>
   </sheetViews>
@@ -6338,10 +6040,10 @@
       <c r="G2" s="33"/>
       <c r="H2" s="33"/>
       <c r="I2" s="33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>19</v>
@@ -6362,7 +6064,7 @@
         <v>24</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6370,7 +6072,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>27</v>
@@ -6423,7 +6125,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>27</v>
@@ -6544,7 +6246,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>27</v>
@@ -6562,7 +6264,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>27</v>
@@ -6580,7 +6282,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>27</v>
@@ -6598,7 +6300,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>37</v>
@@ -6616,7 +6318,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>37</v>
@@ -6634,7 +6336,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>27</v>
@@ -6652,7 +6354,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>27</v>
@@ -6670,7 +6372,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>27</v>
@@ -6688,7 +6390,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>27</v>
@@ -6706,7 +6408,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>27</v>
@@ -6724,7 +6426,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>94</v>
@@ -6742,7 +6444,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>27</v>
@@ -6760,7 +6462,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>27</v>
@@ -6778,7 +6480,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>37</v>
@@ -6796,7 +6498,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>27</v>
@@ -6814,7 +6516,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>27</v>
@@ -6832,7 +6534,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>27</v>
@@ -6850,7 +6552,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>27</v>
@@ -6868,7 +6570,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>37</v>
@@ -6886,7 +6588,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>27</v>
@@ -6902,7 +6604,7 @@
       <c r="G28" s="33"/>
       <c r="H28" s="33"/>
       <c r="I28" s="33" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6930,7 +6632,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>27</v>
@@ -6950,7 +6652,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>27</v>
@@ -6970,7 +6672,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>94</v>
@@ -7045,7 +6747,7 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="J35" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7053,7 +6755,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>27</v>
@@ -7069,7 +6771,7 @@
       <c r="G36" s="36"/>
       <c r="H36" s="33"/>
       <c r="I36" s="37" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J36" s="0" t="n">
         <f aca="false">SUM(E37:E76)</f>
@@ -7138,7 +6840,7 @@
         <v>99</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D40" s="6" t="str">
         <f aca="false">IF(C40 = "Finalizada/Corregida","100%","")</f>
@@ -7207,7 +6909,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>37</v>
@@ -7279,7 +6981,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>94</v>
@@ -7297,7 +6999,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>94</v>
@@ -7315,7 +7017,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>94</v>
@@ -7423,7 +7125,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>94</v>
@@ -7441,7 +7143,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>94</v>
@@ -7459,7 +7161,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>94</v>
@@ -7477,7 +7179,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>94</v>
@@ -7495,7 +7197,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>94</v>
@@ -7621,7 +7323,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>94</v>
@@ -7639,7 +7341,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>94</v>
@@ -7657,7 +7359,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>94</v>
@@ -7675,7 +7377,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>94</v>
@@ -7693,7 +7395,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>94</v>
@@ -7711,7 +7413,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>94</v>
@@ -7729,7 +7431,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>94</v>
@@ -7747,7 +7449,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>94</v>
@@ -7765,7 +7467,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>94</v>
@@ -7783,7 +7485,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="38" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C76" s="28" t="s">
         <v>94</v>
@@ -7799,10 +7501,10 @@
       <c r="G76" s="33"/>
       <c r="H76" s="33"/>
       <c r="I76" s="33" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7810,7 +7512,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>94</v>
@@ -7836,7 +7538,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="42" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>94</v>
@@ -7858,7 +7560,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>94</v>
@@ -7880,7 +7582,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>94</v>
@@ -7900,7 +7602,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>94</v>
@@ -7918,7 +7620,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="31" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>94</v>
@@ -7936,7 +7638,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>94</v>
@@ -7954,7 +7656,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>94</v>
@@ -7972,7 +7674,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="31" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>94</v>
@@ -7990,7 +7692,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>94</v>
@@ -8008,7 +7710,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>94</v>
@@ -8026,7 +7728,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="38" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C88" s="28" t="s">
         <v>94</v>
@@ -8042,10 +7744,10 @@
       <c r="G88" s="33"/>
       <c r="H88" s="33"/>
       <c r="I88" s="33" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8053,7 +7755,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>94</v>
@@ -8075,7 +7777,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="42" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>94</v>
@@ -8093,7 +7795,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="31" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>94</v>
@@ -8102,7 +7804,7 @@
         <f aca="false">IF(C91 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E91" s="43" t="n">
+      <c r="E91" s="40" t="n">
         <v>120</v>
       </c>
     </row>
@@ -8111,7 +7813,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>94</v>
@@ -8120,7 +7822,7 @@
         <f aca="false">IF(C92 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E92" s="43" t="n">
+      <c r="E92" s="40" t="n">
         <v>120</v>
       </c>
     </row>
@@ -8129,7 +7831,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="31" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>94</v>
@@ -8138,7 +7840,7 @@
         <f aca="false">IF(C93 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E93" s="43" t="n">
+      <c r="E93" s="40" t="n">
         <v>120</v>
       </c>
     </row>
@@ -8147,7 +7849,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="31" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>94</v>
@@ -8156,7 +7858,7 @@
         <f aca="false">IF(C94 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E94" s="43" t="n">
+      <c r="E94" s="40" t="n">
         <v>120</v>
       </c>
     </row>
@@ -8165,7 +7867,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="31" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>94</v>
@@ -8174,7 +7876,7 @@
         <f aca="false">IF(C95 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E95" s="43" t="n">
+      <c r="E95" s="40" t="n">
         <v>120</v>
       </c>
     </row>
@@ -8183,7 +7885,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="31" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>94</v>
@@ -8192,7 +7894,7 @@
         <f aca="false">IF(C96 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E96" s="43" t="n">
+      <c r="E96" s="40" t="n">
         <v>120</v>
       </c>
     </row>
@@ -8201,7 +7903,7 @@
         <v>49</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>94</v>
@@ -8237,7 +7939,7 @@
         <v>95</v>
       </c>
       <c r="B99" s="38" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C99" s="28" t="s">
         <v>94</v>
@@ -8246,17 +7948,17 @@
         <f aca="false">IF(C99 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E99" s="44" t="n">
+      <c r="E99" s="36" t="n">
         <v>60</v>
       </c>
       <c r="F99" s="33"/>
       <c r="G99" s="33"/>
       <c r="H99" s="33"/>
       <c r="I99" s="33" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="J99" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8264,7 +7966,7 @@
         <v>96</v>
       </c>
       <c r="B100" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>94</v>
@@ -8286,7 +7988,7 @@
         <v>97</v>
       </c>
       <c r="B101" s="42" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>94</v>
@@ -8304,7 +8006,7 @@
         <v>98</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C102" s="10" t="s">
         <v>94</v>
@@ -8313,7 +8015,7 @@
         <f aca="false">IF(C102 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E102" s="43" t="n">
+      <c r="E102" s="40" t="n">
         <v>60</v>
       </c>
     </row>
@@ -8322,7 +8024,7 @@
         <v>99</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>94</v>
@@ -8331,7 +8033,7 @@
         <f aca="false">IF(C103 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E103" s="43" t="n">
+      <c r="E103" s="40" t="n">
         <v>60</v>
       </c>
     </row>
@@ -8340,7 +8042,7 @@
         <v>100</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>94</v>
@@ -8349,7 +8051,7 @@
         <f aca="false">IF(C104 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E104" s="43" t="n">
+      <c r="E104" s="40" t="n">
         <v>150</v>
       </c>
     </row>
@@ -8358,7 +8060,7 @@
         <v>101</v>
       </c>
       <c r="B105" s="31" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>94</v>
@@ -8367,7 +8069,7 @@
         <f aca="false">IF(C105 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E105" s="43" t="n">
+      <c r="E105" s="40" t="n">
         <v>90</v>
       </c>
     </row>
@@ -8376,7 +8078,7 @@
         <v>102</v>
       </c>
       <c r="B106" s="31" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>94</v>
@@ -8385,7 +8087,7 @@
         <f aca="false">IF(C106 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E106" s="43" t="n">
+      <c r="E106" s="40" t="n">
         <v>120</v>
       </c>
     </row>
@@ -8394,7 +8096,7 @@
         <v>103</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>94</v>
@@ -8403,7 +8105,7 @@
         <f aca="false">IF(C107 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E107" s="43" t="n">
+      <c r="E107" s="40" t="n">
         <v>90</v>
       </c>
     </row>
@@ -8412,7 +8114,7 @@
         <v>104</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>94</v>
@@ -8421,7 +8123,7 @@
         <f aca="false">IF(C108 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E108" s="43" t="n">
+      <c r="E108" s="40" t="n">
         <v>90</v>
       </c>
     </row>
@@ -8430,7 +8132,7 @@
         <v>105</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C109" s="10" t="s">
         <v>94</v>
@@ -8439,7 +8141,7 @@
         <f aca="false">IF(C109 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E109" s="43" t="n">
+      <c r="E109" s="40" t="n">
         <v>100</v>
       </c>
     </row>
@@ -8448,7 +8150,7 @@
         <v>106</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>94</v>
@@ -8466,7 +8168,7 @@
         <v>107</v>
       </c>
       <c r="B111" s="31" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C111" s="10" t="s">
         <v>94</v>
@@ -8475,7 +8177,7 @@
         <f aca="false">IF(C111 = "Finalizada/Corregida","100%","")</f>
         <v/>
       </c>
-      <c r="E111" s="43" t="n">
+      <c r="E111" s="40" t="n">
         <v>90</v>
       </c>
     </row>
@@ -8532,80 +8234,80 @@
     <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>"Sin empezar"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Paralizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C89">
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>"Sin empezar"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>"Paralizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"Sin empezar"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"Paralizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100">
-    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"Sin empezar"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"Paralizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:C111">
-    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
+    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
+    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"Sin empezar"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>"Paralizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
+    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97:C98">
-    <cfRule type="cellIs" priority="35" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+    <cfRule type="cellIs" priority="35" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="36" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="cellIs" priority="36" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>"Sin empezar"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>"Paralizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8638,7 +8340,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.14"/>
   </cols>
   <sheetData>
@@ -8649,7 +8351,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8664,12 +8366,12 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>214</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizado EXCEL y revisada vistas de FUNC_ACCION y FUNCIONALIDAD, mas sus controladores
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,309 +27,308 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="210">
-  <si>
-    <t xml:space="preserve">Semana 1(Del 20/11/2017 hasta 26/11/2017)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nº Tarea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tareas principales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porcentaje de consecución de la tarea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Observaciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiempo planificado (min)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recurso asociado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiempo empleado (min)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recursos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código asociado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiempo planificado total (min)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiempo empleado total (min)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiempo no utilizado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coste por hora planificado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingresos planificados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beneficio planificado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coste por hora planificado utilizado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beneficio real</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tareas paralizadas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tareas Finalizadas /Corregidas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tareas en proceso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tareas sin empezar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tareas Pendientes de correción</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tareas Aplazadas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nº Tareas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organizar y asignar tareas: Semana 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finalizada/Corregida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miguel Ferreiro Díaz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nº</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de usuarios:  Modificar controladores para adaptarlo al nuevo modelo de datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alejandro Vila Cid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de usuarios:  Modificar modelos para adaptarlo al nuevo modelo de datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del modelo:USUARIOS_MODEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jonatan Couto Riádigos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de usuarios:  Modificar vistas para adapartalo al nuevo modelo de datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paralizada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificados valores para asegurar la concordancia con el modelo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brais Santos Negreira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planteamiento incicial de modelos de secuencia para la gestión de grupos de usuario, permisos de usuario y gestión de acciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creado modelo de secuencia empleando visual paradigm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brais Rodríguez Martínez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de grupos de usuario: Crear modelo de datos para  la tabla USUARIO_GRUPO. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creados el modelo de USUARIO_GRUPO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de grupos de usuario: Crear modelo de datos para  la tabla GRUPO. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del modelo:GRUPO_MODEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de los USUARIO_GRUPO. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creado el controlador: USUARIOS_GRUPO_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de USUARIO_GRUPO no se puede editar al ser claves.                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de grupos de usuario: Crear vistas  las posibles acciones sobre la tabla </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creadas las vistas de acuerdo a los atributos actuales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de grupos de usuario: Crear vistas para las posibles acciones sobre la tabla GRUPO. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión   y correción de la tarea 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión  y correción de la tarea 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión  y correción de la tarea 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En la correción en la línea 28 se cambio idgrupo por grupo porque estaba mal puesto,en lalínea 41 se cambio USUARIOS_GRUPO_ADD por USUARIOS_ADD y en la línea 61 USUARIOS_DELETE por USUARIOS_GRUPO_DELETE. En la línea 60 se cambió USUARIOS_GRUPO por USUARIOS_GRUPO_Model.  A mayores se añadieron comentarios para entender lo que se hacía</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión  y correción de la tarea 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión de la tarea 10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se pusieron comillas en el value de los campos hidden de USUARIOS:GRUPO_DELETE.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creado el model de permisos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de permisos de usuario:  Crear controlador de datos para la tabla PERMISOS.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creado el controlador: PERMISOS_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de  PERMISOS no se puede editar al ser claves.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de permisos de usuario:  Crear vistas para las posibles acciones sobre la tabla PERMISOS.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión  y correción de la tarea 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendiente estandarización de nombres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión  y correción de la tarea 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión  y correciónde la tarea 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corregidas algunas referencias a controladores y clases. Eliminado edit porque los atributos son clave.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de acciones:  Crear modelo de datos para ACCIONES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del modelo:ACCIONES_MODEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de acciones: Crear vistas para ACCIONES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estructura provisional de las vistas para acciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organizar y asignar tareas: Semana 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tareas extra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recursos asociado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de acciones: Crear controlador de datos para ACCIONES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Falta solucionar como se trataría el borrado de un acción</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión  y correción de la tarea 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión  y correciónde la tarea 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faltaron las comillas en el value de los campos hidden de ACCIONES_DELETE_view</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de funcionalidades: Crear modelo de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombres de modelo: FUNCIONALIDAD_MODEL y FUNC_ACCION_MODEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de funcionalidades: Crear controlador de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Falta solucionar como se trataría el borrado de una funcionalidad y de funcionalidad_accion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de funcionalidades: Crear vistas para las posibles acciones sobre las tablas FUNCIONALIDADES Y FUNCIONALIDAD_ACCION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creadas las vistas correspondientes excepto  edit en funcionalidad_accion ya que los atributos son todos claves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión  y correción de la tarea 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semana 2(Del 20/11/2017 hasta 3/12/2017)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiempo restante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingresos reales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seguimiento en la organización y asignación de tareas de la Semana 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin empezar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creación de una guía para llamar a los diferentes archivos, atributos, clases, funciones, etc para crear una unicidad en la elaboración de las tareas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECHADLE UN VISTAZO</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="211">
+  <si>
+    <t>Semana 1(Del 20/11/2017 hasta 26/11/2017)</t>
+  </si>
+  <si>
+    <t>nº Tarea</t>
+  </si>
+  <si>
+    <t>Tareas principales</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Porcentaje de consecución de la tarea</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Tiempo planificado (min)</t>
+  </si>
+  <si>
+    <t>Recurso asociado</t>
+  </si>
+  <si>
+    <t>Tiempo empleado (min)</t>
+  </si>
+  <si>
+    <t>Recursos</t>
+  </si>
+  <si>
+    <t>Código asociado</t>
+  </si>
+  <si>
+    <t>Tiempo planificado total (min)</t>
+  </si>
+  <si>
+    <t>Tiempo empleado total (min)</t>
+  </si>
+  <si>
+    <t>Tiempo no utilizado</t>
+  </si>
+  <si>
+    <t>Coste por hora planificado</t>
+  </si>
+  <si>
+    <t>Ingresos planificados</t>
+  </si>
+  <si>
+    <t>Beneficio planificado</t>
+  </si>
+  <si>
+    <t>Coste por hora planificado utilizado</t>
+  </si>
+  <si>
+    <t>Beneficio real</t>
+  </si>
+  <si>
+    <t>Tareas paralizadas</t>
+  </si>
+  <si>
+    <t> Tareas Finalizadas /Corregidas</t>
+  </si>
+  <si>
+    <t> Tareas en proceso</t>
+  </si>
+  <si>
+    <t>Tareas sin empezar</t>
+  </si>
+  <si>
+    <t>Tareas Pendientes de correción</t>
+  </si>
+  <si>
+    <t>Tareas Aplazadas</t>
+  </si>
+  <si>
+    <t>nº Tareas</t>
+  </si>
+  <si>
+    <t>Organizar y asignar tareas: Semana 1</t>
+  </si>
+  <si>
+    <t>Finalizada/Corregida</t>
+  </si>
+  <si>
+    <t>Miguel Ferreiro Díaz</t>
+  </si>
+  <si>
+    <t>nº</t>
+  </si>
+  <si>
+    <t>Gestión de usuarios:  Modificar controladores para adaptarlo al nuevo modelo de datos</t>
+  </si>
+  <si>
+    <t>Alejandro Vila Cid</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Gestión de usuarios:  Modificar modelos para adaptarlo al nuevo modelo de datos</t>
+  </si>
+  <si>
+    <t>Nombre del modelo:USUARIOS_MODEL</t>
+  </si>
+  <si>
+    <t>Jonatan Couto Riádigos</t>
+  </si>
+  <si>
+    <t>Gestión de usuarios:  Modificar vistas para adapartalo al nuevo modelo de datos</t>
+  </si>
+  <si>
+    <t>Paralizada</t>
+  </si>
+  <si>
+    <t>Modificados valores para asegurar la concordancia con el modelo</t>
+  </si>
+  <si>
+    <t>Brais Santos Negreira</t>
+  </si>
+  <si>
+    <t>Planteamiento incicial de modelos de secuencia para la gestión de grupos de usuario, permisos de usuario y gestión de acciones</t>
+  </si>
+  <si>
+    <t>Creado modelo de secuencia empleando visual paradigm</t>
+  </si>
+  <si>
+    <t>Brais Rodríguez Martínez</t>
+  </si>
+  <si>
+    <t>Gestion de grupos de usuario: Crear modelo de datos para  la tabla USUARIO_GRUPO. </t>
+  </si>
+  <si>
+    <t>Creados el modelo de USUARIO_GRUPO</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Gestion de grupos de usuario: Crear modelo de datos para  la tabla GRUPO. </t>
+  </si>
+  <si>
+    <t>Nombre del modelo:GRUPO_MODEL</t>
+  </si>
+  <si>
+    <t>Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de los USUARIO_GRUPO. </t>
+  </si>
+  <si>
+    <t>Creado el controlador: USUARIOS_GRUPO_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de USUARIO_GRUPO no se puede editar al ser claves.                              </t>
+  </si>
+  <si>
+    <t>Gestión de grupos de usuario: Crear controlador para manejar las acciones asociadas a la gestión de GRUPO. (ADD,SEARCH, EDIT,DELETE, SHOWCURRENT,SHOWALL)</t>
+  </si>
+  <si>
+    <t>Gestión de grupos de usuario: Crear vistas  las posibles acciones sobre la tabla </t>
+  </si>
+  <si>
+    <t>Creadas las vistas de acuerdo a los atributos actuales</t>
+  </si>
+  <si>
+    <t>Gestión de grupos de usuario: Crear vistas para las posibles acciones sobre la tabla GRUPO. </t>
+  </si>
+  <si>
+    <t>Revisión   y correción de la tarea 6</t>
+  </si>
+  <si>
+    <t>Revisión  y correción de la tarea 7</t>
+  </si>
+  <si>
+    <t>Revisión  y correción de la tarea 8</t>
+  </si>
+  <si>
+    <t>En la correción en la línea 28 se cambio idgrupo por grupo porque estaba mal puesto,en lalínea 41 se cambio USUARIOS_GRUPO_ADD por USUARIOS_ADD y en la línea 61 USUARIOS_DELETE por USUARIOS_GRUPO_DELETE. En la línea 60 se cambió USUARIOS_GRUPO por USUARIOS_GRUPO_Model.  A mayores se añadieron comentarios para entender lo que se hacía</t>
+  </si>
+  <si>
+    <t>Revisión  y correción de la tarea 9</t>
+  </si>
+  <si>
+    <t>Revisión de la tarea 10 </t>
+  </si>
+  <si>
+    <t>Se pusieron comillas en el value de los campos hidden de USUARIOS:GRUPO_DELETE.</t>
+  </si>
+  <si>
+    <t>Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS. </t>
+  </si>
+  <si>
+    <t>Creado el model de permisos</t>
+  </si>
+  <si>
+    <t>Gestion de permisos de usuario:  Crear controlador de datos para la tabla PERMISOS.  </t>
+  </si>
+  <si>
+    <t>Creado el controlador: PERMISOS_CONTROLLER.php. La acción edit no se ha incluido al no ser necesaria debido a que los atributos de  PERMISOS no se puede editar al ser claves.</t>
+  </si>
+  <si>
+    <t>Gestion de permisos de usuario:  Crear vistas para las posibles acciones sobre la tabla PERMISOS.  </t>
+  </si>
+  <si>
+    <t>Revisión  y correción de la tarea 17</t>
+  </si>
+  <si>
+    <t>Pendiente estandarización de nombres</t>
+  </si>
+  <si>
+    <t>Revisión  y correción de la tarea 18</t>
+  </si>
+  <si>
+    <t>Revisión  y correciónde la tarea 19</t>
+  </si>
+  <si>
+    <t>Corregidas algunas referencias a controladores y clases. Eliminado edit porque los atributos son clave.</t>
+  </si>
+  <si>
+    <t>Gestión de acciones:  Crear modelo de datos para ACCIONES</t>
+  </si>
+  <si>
+    <t>Nombre del modelo:ACCIONES_MODEL</t>
+  </si>
+  <si>
+    <t>Gestión de acciones: Crear vistas para ACCIONES</t>
+  </si>
+  <si>
+    <t>Estructura provisional de las vistas para acciones</t>
+  </si>
+  <si>
+    <t>Organizar y asignar tareas: Semana 2</t>
+  </si>
+  <si>
+    <t>Tareas extra</t>
+  </si>
+  <si>
+    <t>Recursos asociado</t>
+  </si>
+  <si>
+    <t>Gestión de acciones: Crear controlador de datos para ACCIONES</t>
+  </si>
+  <si>
+    <t>Falta solucionar como se trataría el borrado de un acción</t>
+  </si>
+  <si>
+    <t>Revisión  y correción de la tarea 23</t>
+  </si>
+  <si>
+    <t>Revisión  y correciónde la tarea 24</t>
+  </si>
+  <si>
+    <t>Faltaron las comillas en el value de los campos hidden de ACCIONES_DELETE_view</t>
+  </si>
+  <si>
+    <t>Gestion de funcionalidades: Crear modelo de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t>Nombres de modelo: FUNCIONALIDAD_MODEL y FUNC_ACCION_MODEL</t>
+  </si>
+  <si>
+    <t>Gestion de funcionalidades: Crear controlador de datos para FUNCIONALIDADES y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t>Falta solucionar como se trataría el borrado de una funcionalidad y de funcionalidad_accion</t>
+  </si>
+  <si>
+    <t>Gestion de funcionalidades: Crear vistas para las posibles acciones sobre las tablas FUNCIONALIDADES Y FUNCIONALIDAD_ACCION</t>
+  </si>
+  <si>
+    <t>Creadas las vistas correspondientes excepto  edit en funcionalidad_accion ya que los atributos son todos claves</t>
+  </si>
+  <si>
+    <t>Revisión  y correción de la tarea 40</t>
+  </si>
+  <si>
+    <t>Semana 2(Del 20/11/2017 hasta 3/12/2017)</t>
+  </si>
+  <si>
+    <t>Tiempo restante</t>
+  </si>
+  <si>
+    <t>Ingresos reales</t>
+  </si>
+  <si>
+    <t>Seguimiento en la organización y asignación de tareas de la Semana 2</t>
+  </si>
+  <si>
+    <t>Sin empezar</t>
+  </si>
+  <si>
+    <t>Creación de una guía para llamar a los diferentes archivos, atributos, clases, funciones, etc para crear una unicidad en la elaboración de las tareas.</t>
+  </si>
+  <si>
+    <t>ECHADLE UN VISTAZO</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Realizar el </t>
+      <t>Realizar el </t>
     </r>
     <r>
       <rPr>
@@ -339,344 +338,347 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">cambio de nombre de archivos, atributos, etc según lo establecido en la tarea 2</t>
+      <t>cambio de nombre de archivos, atributos, etc según lo establecido en la tarea 2</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Tiempo excedido por fallo de comunicación.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organizar en directorios con el nombre indicado en la tarea 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de usuarios: Modificar vistas para adapartalo al nuevo modelo de datos.  (Tarea paralizada en la Semana 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de grupos de usuario: Crear vistas  las posibles acciones sobre la tabla USUARIO_GRUPO. (Tarea paralizada en la Semana 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de grupos de usuario: Crear vistas para las posibles acciones sobre la tabla GRUPO. (Tarea paralizada en la Semana 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de permisos de usuario:  Crear vistas para las posibles acciones sobre la tabla PERMISOS.  (Tarea paralizada en la Semana 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de acciones: Crear vistas para ACCIONES (Tarea paralizada en la Semana 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de funcionalidades: Crear vistas para las posibles acciones sobre las tablas FUNCIONALIDADES Y FUNCIONALIDAD_ACCION (Tarea paralizada en la Semana 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de las tareas paralizadas:  Tarea 5, 6,7,8,9,10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se hizo paralelo a una revisión del recurso 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reunión para tratar mejoras en la organización, unificar el tratamiento del borrado en las tablas y la confirmación del documento a seguir para nombrar a los diferentes elementos. Además se tratarán aspectos como el de mejorar el ACL y como abordar de manera correcta  la gestión de trabajos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratamiento del borrado entre las tablas: USUARIO, USUARIO_GRUPO y GRUPO.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendiente de correción</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratamiento del borrado entre las tablas: PERMISO y GRUPO. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción del tratamiento del borrado de las tareas 17,18,18 y 20.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 36 de la Semana 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 41 de la Semana 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 42 de la Semana 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión  y correción de la tarea 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teniendo la BD: adaptar los modelos y controladores a la nueva base de datos. (Las vistas deben adaptarse a través de las tareas paralizadas ya que implican un mayor esfuerzo al tener que controlar las validaciones)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se probará la aplicación para observar el comportamiento de las vistas y se solucionarán problemas en las vistas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se probará la aplicación para observar el compartamiento de los controladores y se solucionarán sus problemas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas:  se probará la aplicación para observar el compartamiento de los modelos y se solucionarán sus problemas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de un esquema de como sería  y como interacionaría los diferentes elementos de la interfaz tanto para el usuario.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de un esquema de como sería  y como interacionaría los diferentes elementos de la interfaz tanto para el administrador.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de trabajos: realizar las vistas, controladores y  modelos de la tabla TRABAJO.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creados los elementos correspondientes según la guía de nombres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y corrección de las tarea 34.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de historias: realizar las vistas, controladores y  modelos de la tabla HISTORIA.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y corrección de la tarea 36.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión evaluación: realizar las vistas, controladores y  modelos de la tabla EVALUACIÓN.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y corrección de la tarea 38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de la asignación automática de QAs: realizar una primera versión con los archivos necesarios para su tratamiento (vistas, controladores, modelos).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y corrección de la tarea 41 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de la entregas: realizar una primera versión con los archivos necesarios para su tratamiento (vistas, controladores, modelos).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del modelo:ENTREGA_MODEL,Nombre del controlador ENTREGA_CONTROLLER y nombre de las vistas empiezan por ENTREGA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y corrección de la tarea 43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organización y planificación de Semana 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inicio de la Semana 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiempo planificado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tareas Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de grupos: Crear modelo de datos para  la tabla GRUPO. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de grupos: Crear controlador para manejar las acciones asociadas a la gestión de GRUPO. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de grupos de usuario: Crear vistas  las posibles acciones sobre la tabla USUARIO_GRUPO. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de grupos : Crear vistas para las posibles acciones sobre la tabla GRUPO. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion de permisos de usuario:  Crear controlador de datos para la tabla PERMISOS. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fin de lo planeado en la Semana 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inicio de lo planeado en la Semana 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En proceso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de grupos: Crear vistas para las posibles acciones sobre la tabla GRUPO. (Tarea paralizada en la Semana 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de las tareas paralizadas cuando finalicen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 32 de la Semana 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 33 de la Semana 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratamiento del borrado entre las tablas: USUARIO, USUARIO_GRUPO y GRUPO.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratamiento del borrado entre las tablas: PERMISO y GRUPO. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción del tratamiento del borrado.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de las tarea 64.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 66.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de la asignación de QAs: realizar las vistas, controladores y  modelos de la tabla ASIGNAC_QA.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión de la entregas: realizar las vistas, controladores y  modelos de la tabla ENTREGA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inicio de la Semana 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actualización del powerpoint </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comprobación/Correción de todos los elementos para asegurar de que siguen el estándar establecido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tratamiento del borrado entre las tablas: Realizar los cambios pertinentes para asegurar el borrado correcto de los nuevos modelos de datos creados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisión y correción de la tarea 78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se probará la aplicación para observar el comportamiento de la gestión de trabajos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementación de la regulación de los usuarios para usar las funcionalidades dependiendo de las acciones y permisos asociados. Implementar esta tarea en la parte correspondiente al ACL.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se probará la aplicación para observar el comportamiento de la regulación de  los usuarios para usar las funcionalidades dependiendo de las acciones y permisos permitidos. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementación de la regulación de los usuarios para usar las funcionalidades dependiendo de las acciones y permisos permitidos. Implementar esta tarea en la parte correspondiente a la parte de gestión de trabajos. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organización y planificación de Semana 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inicio de la Semana 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comprobar/Corregir el funcionamiento de la generación automática de QAS  usuarios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comprobar/Corregir el funcionamiento de las historias a evaluar en EVALUACIÓN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comprobar/Corregir el funcionamiento de la generación de notas entregas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comprobar/Corregir el funcionamiento de las notas de Qas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comprobar/Corregir el funcionamiento de la consulta de correción de entrega propia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comprobar/Corregir el funcionamiento de la consulta de correción de QA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reunión para tratar los aspectos de la aplicación más críticos en ese momento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organización y planificación de Semana 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inicio de la Semana 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se realizará pruebas sobre el funcionamiento  de gestión de usuarios.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se realizará pruebas sobre el funcionamiento  de gestión de grupos de usuarios.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se realizará pruebas sobre el funcionamiento  de gestión de permisos en toda la aplicación. Incluye la aplicación correcta de acciones para posibles las funcionalidades.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se realizará pruebas sobre el funcionamiento  de gestión de nota de trabajos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se realizará pruebas sobre el funcionamiento  correcto de los trabajos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se realizará pruebas sobre el funcionamiento  correcto de las historias.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se realizará pruebas sobre el funcionamiento  correcto de las asignación de Qas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se realizará pruebas sobre el funcionamiento  correcto de la evaluación de historias y asignación de Qas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización de pruebas: se realizará pruebas sobre el funcionamiento  correcto de la gestión de entregas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realización del manual de usuario:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aplazada</t>
+    <t>Tiempo excedido por fallo de comunicación.</t>
+  </si>
+  <si>
+    <t>Organizar en directorios con el nombre indicado en la tarea 2</t>
+  </si>
+  <si>
+    <t>Gestión de usuarios: Modificar vistas para adapartalo al nuevo modelo de datos.  (Tarea paralizada en la Semana 1)</t>
+  </si>
+  <si>
+    <t>Gestión de grupos de usuario: Crear vistas  las posibles acciones sobre la tabla USUARIO_GRUPO. (Tarea paralizada en la Semana 1)</t>
+  </si>
+  <si>
+    <t>Gestión de grupos de usuario: Crear vistas para las posibles acciones sobre la tabla GRUPO. (Tarea paralizada en la Semana 1)</t>
+  </si>
+  <si>
+    <t>Gestion de permisos de usuario:  Crear vistas para las posibles acciones sobre la tabla PERMISOS.  (Tarea paralizada en la Semana 1)</t>
+  </si>
+  <si>
+    <t>Gestión de acciones: Crear vistas para ACCIONES (Tarea paralizada en la Semana 1)</t>
+  </si>
+  <si>
+    <t>Gestion de funcionalidades: Crear vistas para las posibles acciones sobre las tablas FUNCIONALIDADES Y FUNCIONALIDAD_ACCION (Tarea paralizada en la Semana 1)</t>
+  </si>
+  <si>
+    <t>Revisión y correción de las tareas paralizadas:  Tarea 5, 6,7,8,9,10</t>
+  </si>
+  <si>
+    <t>Se hizo paralelo a una revisión del recurso 2</t>
+  </si>
+  <si>
+    <t>Reunión para tratar mejoras en la organización, unificar el tratamiento del borrado en las tablas y la confirmación del documento a seguir para nombrar a los diferentes elementos. Además se tratarán aspectos como el de mejorar el ACL y como abordar de manera correcta  la gestión de trabajos.</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: USUARIO, USUARIO_GRUPO y GRUPO.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
+  </si>
+  <si>
+    <t>Pendiente de correción</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: PERMISO y GRUPO. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
+  </si>
+  <si>
+    <t>Revisión y correción del tratamiento del borrado de las tareas 17,18,18 y 20.</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 36 de la Semana 1</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 41 de la Semana 1</t>
+  </si>
+  <si>
+    <t>se cambiaron los size debido a que  no tenían el tamaño que está en la BD</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 42 de la Semana 1</t>
+  </si>
+  <si>
+    <t>Revisión  y correción de la tarea 25</t>
+  </si>
+  <si>
+    <t>Teniendo la BD: adaptar los modelos y controladores a la nueva base de datos. (Las vistas deben adaptarse a través de las tareas paralizadas ya que implican un mayor esfuerzo al tener que controlar las validaciones)</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se probará la aplicación para observar el comportamiento de las vistas y se solucionarán problemas en las vistas.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se probará la aplicación para observar el compartamiento de los controladores y se solucionarán sus problemas </t>
+  </si>
+  <si>
+    <t>Realización de pruebas:  se probará la aplicación para observar el compartamiento de los modelos y se solucionarán sus problemas.</t>
+  </si>
+  <si>
+    <t>Realización de un esquema de como sería  y como interacionaría los diferentes elementos de la interfaz tanto para el usuario.</t>
+  </si>
+  <si>
+    <t>Realización de un esquema de como sería  y como interacionaría los diferentes elementos de la interfaz tanto para el administrador.</t>
+  </si>
+  <si>
+    <t>Gestión de trabajos: realizar las vistas, controladores y  modelos de la tabla TRABAJO.</t>
+  </si>
+  <si>
+    <t>Creados los elementos correspondientes según la guía de nombres</t>
+  </si>
+  <si>
+    <t>Revisión y corrección de las tarea 34.</t>
+  </si>
+  <si>
+    <t>Gestión de historias: realizar las vistas, controladores y  modelos de la tabla HISTORIA.</t>
+  </si>
+  <si>
+    <t>Revisión y corrección de la tarea 36.</t>
+  </si>
+  <si>
+    <t>Gestión evaluación: realizar las vistas, controladores y  modelos de la tabla EVALUACIÓN.</t>
+  </si>
+  <si>
+    <t>Revisión y corrección de la tarea 38</t>
+  </si>
+  <si>
+    <t>Gestión de la asignación automática de QAs: realizar una primera versión con los archivos necesarios para su tratamiento (vistas, controladores, modelos).</t>
+  </si>
+  <si>
+    <t>Revisión y corrección de la tarea 41 </t>
+  </si>
+  <si>
+    <t>Gestión de la entregas: realizar una primera versión con los archivos necesarios para su tratamiento (vistas, controladores, modelos).</t>
+  </si>
+  <si>
+    <t>Nombre del modelo:ENTREGA_MODEL,Nombre del controlador ENTREGA_CONTROLLER y nombre de las vistas empiezan por ENTREGA</t>
+  </si>
+  <si>
+    <t>Revisión y corrección de la tarea 43</t>
+  </si>
+  <si>
+    <t>Organización y planificación de Semana 3</t>
+  </si>
+  <si>
+    <t>Inicio de la Semana 1</t>
+  </si>
+  <si>
+    <t>Tiempo planificado</t>
+  </si>
+  <si>
+    <t>Tareas Total</t>
+  </si>
+  <si>
+    <t>Gestion de grupos: Crear modelo de datos para  la tabla GRUPO. </t>
+  </si>
+  <si>
+    <t>Gestión de grupos: Crear controlador para manejar las acciones asociadas a la gestión de GRUPO. </t>
+  </si>
+  <si>
+    <t>Gestión de grupos de usuario: Crear vistas  las posibles acciones sobre la tabla USUARIO_GRUPO. </t>
+  </si>
+  <si>
+    <t>Gestión de grupos : Crear vistas para las posibles acciones sobre la tabla GRUPO. </t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 6</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 7</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 8</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 9</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 10</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 11</t>
+  </si>
+  <si>
+    <t>Gestion de permisos de usuario: Crear modelo de datos para la tabla PERMISOS.</t>
+  </si>
+  <si>
+    <t>Gestion de permisos de usuario:  Crear controlador de datos para la tabla PERMISOS. </t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 18</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 19</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 20</t>
+  </si>
+  <si>
+    <t>Fin de lo planeado en la Semana 1</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 24</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 25</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 26</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 31</t>
+  </si>
+  <si>
+    <t>Inicio de lo planeado en la Semana 2</t>
+  </si>
+  <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>Gestión de grupos: Crear vistas para las posibles acciones sobre la tabla GRUPO. (Tarea paralizada en la Semana 1)</t>
+  </si>
+  <si>
+    <t>Revisión y correción de las tareas paralizadas cuando finalicen.</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 32 de la Semana 1</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 33 de la Semana 1</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: USUARIO, USUARIO_GRUPO y GRUPO.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado.</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: PERMISO y GRUPO. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado.</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado.</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado.</t>
+  </si>
+  <si>
+    <t>Revisión y correción del tratamiento del borrado.</t>
+  </si>
+  <si>
+    <t>Revisión y correción de las tarea 64.</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 66.</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 68</t>
+  </si>
+  <si>
+    <t>Gestión de la asignación de QAs: realizar las vistas, controladores y  modelos de la tabla ASIGNAC_QA.</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 70</t>
+  </si>
+  <si>
+    <t>Gestión de la entregas: realizar las vistas, controladores y  modelos de la tabla ENTREGA</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 73</t>
+  </si>
+  <si>
+    <t>Inicio de la Semana 3</t>
+  </si>
+  <si>
+    <t>Actualización del powerpoint </t>
+  </si>
+  <si>
+    <t>Comprobación/Correción de todos los elementos para asegurar de que siguen el estándar establecido</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: Realizar los cambios pertinentes para asegurar el borrado correcto de los nuevos modelos de datos creados</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 78</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se probará la aplicación para observar el comportamiento de la gestión de trabajos.</t>
+  </si>
+  <si>
+    <t>Implementación de la regulación de los usuarios para usar las funcionalidades dependiendo de las acciones y permisos asociados. Implementar esta tarea en la parte correspondiente al ACL.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se probará la aplicación para observar el comportamiento de la regulación de  los usuarios para usar las funcionalidades dependiendo de las acciones y permisos permitidos. </t>
+  </si>
+  <si>
+    <t>Implementación de la regulación de los usuarios para usar las funcionalidades dependiendo de las acciones y permisos permitidos. Implementar esta tarea en la parte correspondiente a la parte de gestión de trabajos. </t>
+  </si>
+  <si>
+    <t>Organización y planificación de Semana 4</t>
+  </si>
+  <si>
+    <t>Inicio de la Semana 4</t>
+  </si>
+  <si>
+    <t>Comprobar/Corregir el funcionamiento de la generación automática de QAS  usuarios</t>
+  </si>
+  <si>
+    <t>Comprobar/Corregir el funcionamiento de las historias a evaluar en EVALUACIÓN </t>
+  </si>
+  <si>
+    <t>Comprobar/Corregir el funcionamiento de la generación de notas entregas</t>
+  </si>
+  <si>
+    <t>Comprobar/Corregir el funcionamiento de las notas de Qas</t>
+  </si>
+  <si>
+    <t>Comprobar/Corregir el funcionamiento de la consulta de correción de entrega propia</t>
+  </si>
+  <si>
+    <t>Comprobar/Corregir el funcionamiento de la consulta de correción de QA</t>
+  </si>
+  <si>
+    <t>Reunión para tratar los aspectos de la aplicación más críticos en ese momento</t>
+  </si>
+  <si>
+    <t>Organización y planificación de Semana 5</t>
+  </si>
+  <si>
+    <t>inicio de la Semana 5</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se realizará pruebas sobre el funcionamiento  de gestión de usuarios.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se realizará pruebas sobre el funcionamiento  de gestión de grupos de usuarios.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se realizará pruebas sobre el funcionamiento  de gestión de permisos en toda la aplicación. Incluye la aplicación correcta de acciones para posibles las funcionalidades.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se realizará pruebas sobre el funcionamiento  de gestión de nota de trabajos.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se realizará pruebas sobre el funcionamiento  correcto de los trabajos.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se realizará pruebas sobre el funcionamiento  correcto de las historias.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se realizará pruebas sobre el funcionamiento  correcto de las asignación de Qas.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se realizará pruebas sobre el funcionamiento  correcto de la evaluación de historias y asignación de Qas.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se realizará pruebas sobre el funcionamiento  correcto de la gestión de entregas.</t>
+  </si>
+  <si>
+    <t>Realización del manual de usuario:</t>
+  </si>
+  <si>
+    <t>Aplazada</t>
   </si>
 </sst>
 </file>
@@ -684,10 +686,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0\ %"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -709,87 +711,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="22"/>
@@ -814,7 +735,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -823,50 +744,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFC5E0B4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFF8CBAD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
+        <fgColor rgb="FFDAE3F3"/>
         <bgColor rgb="FFDBDBDB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDAE3F3"/>
-        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -890,7 +769,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFFE699"/>
       </patternFill>
     </fill>
     <fill>
@@ -912,27 +791,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -983,7 +847,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1007,55 +871,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -1072,15 +888,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1088,7 +904,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1108,15 +924,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1124,63 +940,63 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1192,39 +1008,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1236,39 +1052,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="36" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
@@ -1367,16 +1167,16 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C7E7"/>
@@ -1398,12 +1198,12 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00B0F0"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFC5E0B4"/>
       <rgbColor rgb="FFFFE699"/>
       <rgbColor rgb="FF9DC3E6"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF8CBAD"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -1412,7 +1212,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FFC5E0B4"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -1433,38 +1233,38 @@
   </sheetPr>
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="83.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="26.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="18.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="13.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="8.54"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.75"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2847,7 +2647,7 @@
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
       <c r="B41" s="9" t="s">
         <v>87</v>
@@ -2969,7 +2769,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2984,18 +2784,18 @@
   </sheetPr>
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q21" activeCellId="0" sqref="Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="20.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.39"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.0969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3166,7 +2966,7 @@
       </c>
       <c r="Y4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Finalizada/Corregida")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Z4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "En proceso")</f>
@@ -3174,7 +2974,7 @@
       </c>
       <c r="AA4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Sin empezar")</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AB4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Pendiente de correción")</f>
@@ -3263,7 +3063,7 @@
       </c>
       <c r="Y5" s="0" t="n">
         <f aca="false">Y4/AD4 *100</f>
-        <v>11.9047619047619</v>
+        <v>16.6666666666667</v>
       </c>
       <c r="Z5" s="0" t="n">
         <f aca="false">Z4/AD4 *100</f>
@@ -3271,7 +3071,7 @@
       </c>
       <c r="AA5" s="0" t="n">
         <f aca="false">AA4/AD4 *100</f>
-        <v>57.1428571428571</v>
+        <v>52.3809523809524</v>
       </c>
       <c r="AB5" s="0" t="n">
         <f aca="false">AB4/AD4*100</f>
@@ -3694,7 +3494,7 @@
       </c>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="n">
         <v>15</v>
       </c>
@@ -3711,7 +3511,9 @@
       <c r="F18" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="8" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="52.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="n">
@@ -3856,7 +3658,7 @@
       </c>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="n">
         <v>23</v>
       </c>
@@ -3864,26 +3666,30 @@
         <v>116</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>117</v>
+      </c>
       <c r="E26" s="8" t="n">
         <v>30</v>
       </c>
       <c r="F26" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="8" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="n">
         <v>24</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="8" t="n">
@@ -3892,14 +3698,16 @@
       <c r="F27" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="G27" s="8"/>
+      <c r="G27" s="8" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="n">
         <v>26</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>94</v>
@@ -3918,7 +3726,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>94</v>
@@ -3937,7 +3745,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>94</v>
@@ -3956,7 +3764,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>94</v>
@@ -3975,7 +3783,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>94</v>
@@ -3994,7 +3802,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>94</v>
@@ -4013,7 +3821,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>94</v>
@@ -4032,13 +3840,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>110</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E35" s="8" t="n">
         <v>120</v>
@@ -4055,7 +3863,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>94</v>
@@ -4074,7 +3882,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>94</v>
@@ -4093,7 +3901,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>94</v>
@@ -4110,7 +3918,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>110</v>
@@ -4130,7 +3938,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>94</v>
@@ -4147,7 +3955,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>94</v>
@@ -4164,7 +3972,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>94</v>
@@ -4181,13 +3989,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>110</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E43" s="8" t="n">
         <v>90</v>
@@ -4204,7 +4012,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>94</v>
@@ -4221,7 +4029,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>94</v>
@@ -4260,7 +4068,7 @@
     <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4293,7 +4101,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4308,20 +4116,20 @@
   </sheetPr>
   <dimension ref="A1:T111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G105" activeCellId="0" sqref="G105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="62.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="32" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.39"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="61.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="20.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4350,10 +4158,10 @@
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
       <c r="I2" s="34" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>19</v>
@@ -4374,7 +4182,7 @@
         <v>24</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4556,7 +4364,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>27</v>
@@ -4592,7 +4400,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>27</v>
@@ -4610,7 +4418,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>37</v>
@@ -4628,7 +4436,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>37</v>
@@ -4646,7 +4454,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>27</v>
@@ -4664,7 +4472,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>27</v>
@@ -4682,7 +4490,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>27</v>
@@ -4700,7 +4508,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>27</v>
@@ -4718,7 +4526,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>27</v>
@@ -4736,7 +4544,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>94</v>
@@ -4754,7 +4562,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>27</v>
@@ -4772,7 +4580,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>27</v>
@@ -4808,7 +4616,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>27</v>
@@ -4826,7 +4634,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>27</v>
@@ -4844,7 +4652,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>27</v>
@@ -4914,7 +4722,7 @@
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4942,7 +4750,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>27</v>
@@ -4962,7 +4770,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>27</v>
@@ -4982,7 +4790,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>94</v>
@@ -5057,7 +4865,7 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="J35" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5065,7 +4873,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>27</v>
@@ -5081,7 +4889,7 @@
       <c r="G36" s="37"/>
       <c r="H36" s="34"/>
       <c r="I36" s="39" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J36" s="0" t="n">
         <f aca="false">SUM(E37:E76)</f>
@@ -5150,7 +4958,7 @@
         <v>99</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D40" s="6" t="str">
         <f aca="false">IF(C40 = "Finalizada/Corregida","100%","")</f>
@@ -5165,7 +4973,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>94</v>
@@ -5219,7 +5027,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>37</v>
@@ -5291,7 +5099,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>94</v>
@@ -5309,7 +5117,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>94</v>
@@ -5327,7 +5135,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>94</v>
@@ -5435,7 +5243,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>94</v>
@@ -5453,7 +5261,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>94</v>
@@ -5471,7 +5279,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>94</v>
@@ -5489,7 +5297,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>94</v>
@@ -5507,7 +5315,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>94</v>
@@ -5525,7 +5333,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>94</v>
@@ -5543,7 +5351,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>94</v>
@@ -5561,7 +5369,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>94</v>
@@ -5579,7 +5387,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>94</v>
@@ -5597,7 +5405,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>94</v>
@@ -5615,7 +5423,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>94</v>
@@ -5633,7 +5441,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>94</v>
@@ -5651,7 +5459,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>94</v>
@@ -5669,7 +5477,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>94</v>
@@ -5687,7 +5495,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>94</v>
@@ -5705,7 +5513,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>94</v>
@@ -5723,7 +5531,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>94</v>
@@ -5741,7 +5549,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>94</v>
@@ -5759,7 +5567,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>94</v>
@@ -5777,7 +5585,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>94</v>
@@ -5795,7 +5603,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="40" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C76" s="28" t="s">
         <v>94</v>
@@ -5811,10 +5619,10 @@
       <c r="G76" s="34"/>
       <c r="H76" s="34"/>
       <c r="I76" s="34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5822,7 +5630,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>94</v>
@@ -5848,7 +5656,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="44" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>94</v>
@@ -5870,7 +5678,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>94</v>
@@ -5892,7 +5700,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>94</v>
@@ -5912,7 +5720,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>94</v>
@@ -5930,7 +5738,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="31" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>94</v>
@@ -5948,7 +5756,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>94</v>
@@ -5966,7 +5774,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>94</v>
@@ -5984,7 +5792,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>94</v>
@@ -6002,7 +5810,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>94</v>
@@ -6020,7 +5828,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>94</v>
@@ -6038,7 +5846,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="40" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C88" s="28" t="s">
         <v>94</v>
@@ -6054,10 +5862,10 @@
       <c r="G88" s="34"/>
       <c r="H88" s="34"/>
       <c r="I88" s="34" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6065,7 +5873,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>94</v>
@@ -6087,7 +5895,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="44" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>94</v>
@@ -6105,7 +5913,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="45" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>94</v>
@@ -6123,7 +5931,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="45" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>94</v>
@@ -6141,7 +5949,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="45" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>94</v>
@@ -6159,7 +5967,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="45" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>94</v>
@@ -6177,7 +5985,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="45" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>94</v>
@@ -6195,7 +6003,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="45" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>94</v>
@@ -6213,7 +6021,7 @@
         <v>49</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>94</v>
@@ -6249,7 +6057,7 @@
         <v>95</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C99" s="28" t="s">
         <v>94</v>
@@ -6265,10 +6073,10 @@
       <c r="G99" s="34"/>
       <c r="H99" s="34"/>
       <c r="I99" s="34" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J99" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6276,7 +6084,7 @@
         <v>96</v>
       </c>
       <c r="B100" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>94</v>
@@ -6298,7 +6106,7 @@
         <v>97</v>
       </c>
       <c r="B101" s="44" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>94</v>
@@ -6316,7 +6124,7 @@
         <v>98</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C102" s="10" t="s">
         <v>94</v>
@@ -6334,7 +6142,7 @@
         <v>99</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>94</v>
@@ -6352,7 +6160,7 @@
         <v>100</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>94</v>
@@ -6370,7 +6178,7 @@
         <v>101</v>
       </c>
       <c r="B105" s="31" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>94</v>
@@ -6388,7 +6196,7 @@
         <v>102</v>
       </c>
       <c r="B106" s="31" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>94</v>
@@ -6406,7 +6214,7 @@
         <v>103</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>94</v>
@@ -6424,7 +6232,7 @@
         <v>104</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>94</v>
@@ -6442,7 +6250,7 @@
         <v>105</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C109" s="10" t="s">
         <v>94</v>
@@ -6460,7 +6268,7 @@
         <v>106</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>94</v>
@@ -6478,7 +6286,7 @@
         <v>107</v>
       </c>
       <c r="B111" s="45" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C111" s="10" t="s">
         <v>94</v>
@@ -6516,10 +6324,10 @@
     <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>"Sin empezar"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Paralizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6603,7 +6411,7 @@
     <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>"Paralizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Finalizada/Corregida"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6615,7 +6423,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6630,14 +6438,14 @@
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.54"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6647,7 +6455,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6662,7 +6470,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6673,7 +6481,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
EXCEL actualizado de correcion de tratamiento de borrado
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -320,26 +320,7 @@
     <t>ECHADLE UN VISTAZO</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Realizar el </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>cambio de nombre de archivos, atributos, etc según lo establecido en la tarea 2</t>
-    </r>
+    <t>Realizar el cambio de nombre de archivos, atributos, etc según lo establecido en la tarea 2</t>
   </si>
   <si>
     <t>Tiempo excedido por fallo de comunicación.</t>
@@ -378,55 +359,55 @@
     <t>Tratamiento del borrado entre las tablas: USUARIO, USUARIO_GRUPO y GRUPO.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
   </si>
   <si>
+    <t>Tratamiento del borrado entre las tablas: PERMISO y GRUPO. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
+  </si>
+  <si>
+    <t>Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
+  </si>
+  <si>
+    <t>Revisión y correción del tratamiento del borrado de las tareas 17,18,18 y 20.</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 36 de la Semana 1</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 41 de la Semana 1</t>
+  </si>
+  <si>
+    <t>se cambiaron los size debido a que  no tenían el tamaño que está en la BD</t>
+  </si>
+  <si>
+    <t>Revisión y correción de la tarea 42 de la Semana 1</t>
+  </si>
+  <si>
+    <t>Revisión  y correción de la tarea 25</t>
+  </si>
+  <si>
+    <t>Teniendo la BD: adaptar los modelos y controladores a la nueva base de datos. (Las vistas deben adaptarse a través de las tareas paralizadas ya que implican un mayor esfuerzo al tener que controlar las validaciones)</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se probará la aplicación para observar el comportamiento de las vistas y se solucionarán problemas en las vistas.</t>
+  </si>
+  <si>
+    <t>Realización de pruebas: se probará la aplicación para observar el compartamiento de los controladores y se solucionarán sus problemas </t>
+  </si>
+  <si>
+    <t>Realización de pruebas:  se probará la aplicación para observar el compartamiento de los modelos y se solucionarán sus problemas.</t>
+  </si>
+  <si>
+    <t>Realización de un esquema de como sería  y como interacionaría los diferentes elementos de la interfaz tanto para el usuario.</t>
+  </si>
+  <si>
+    <t>Realización de un esquema de como sería  y como interacionaría los diferentes elementos de la interfaz tanto para el administrador.</t>
+  </si>
+  <si>
+    <t>Gestión de trabajos: realizar las vistas, controladores y  modelos de la tabla TRABAJO.</t>
+  </si>
+  <si>
     <t>Pendiente de correción</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: PERMISO y GRUPO. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: PERMISO y FUNCIONALIDAD_ACCION.Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
-  </si>
-  <si>
-    <t>Tratamiento del borrado entre las tablas: FUNCIONALIDAD_ACCION, FUNCIONALIDAD y ACCION. Realizar los cambios pertinentes en el código para conseguir una coherencia en el borrado</t>
-  </si>
-  <si>
-    <t>Revisión y correción del tratamiento del borrado de las tareas 17,18,18 y 20.</t>
-  </si>
-  <si>
-    <t>Revisión y correción de la tarea 36 de la Semana 1</t>
-  </si>
-  <si>
-    <t>Revisión y correción de la tarea 41 de la Semana 1</t>
-  </si>
-  <si>
-    <t>se cambiaron los size debido a que  no tenían el tamaño que está en la BD</t>
-  </si>
-  <si>
-    <t>Revisión y correción de la tarea 42 de la Semana 1</t>
-  </si>
-  <si>
-    <t>Revisión  y correción de la tarea 25</t>
-  </si>
-  <si>
-    <t>Teniendo la BD: adaptar los modelos y controladores a la nueva base de datos. (Las vistas deben adaptarse a través de las tareas paralizadas ya que implican un mayor esfuerzo al tener que controlar las validaciones)</t>
-  </si>
-  <si>
-    <t>Realización de pruebas: se probará la aplicación para observar el comportamiento de las vistas y se solucionarán problemas en las vistas.</t>
-  </si>
-  <si>
-    <t>Realización de pruebas: se probará la aplicación para observar el compartamiento de los controladores y se solucionarán sus problemas </t>
-  </si>
-  <si>
-    <t>Realización de pruebas:  se probará la aplicación para observar el compartamiento de los modelos y se solucionarán sus problemas.</t>
-  </si>
-  <si>
-    <t>Realización de un esquema de como sería  y como interacionaría los diferentes elementos de la interfaz tanto para el usuario.</t>
-  </si>
-  <si>
-    <t>Realización de un esquema de como sería  y como interacionaría los diferentes elementos de la interfaz tanto para el administrador.</t>
-  </si>
-  <si>
-    <t>Gestión de trabajos: realizar las vistas, controladores y  modelos de la tabla TRABAJO.</t>
   </si>
   <si>
     <t>Creados los elementos correspondientes según la guía de nombres</t>
@@ -1070,7 +1051,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -1148,20 +1129,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF33"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -1197,7 +1164,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00B0F0"/>
+      <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFDBDBDB"/>
       <rgbColor rgb="FFC5E0B4"/>
       <rgbColor rgb="FFFFE699"/>
@@ -1207,7 +1174,7 @@
       <rgbColor rgb="FFF8CBAD"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99FF33"/>
+      <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -1239,32 +1206,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.75"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="81.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2784,18 +2751,18 @@
   </sheetPr>
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q21" activeCellId="0" sqref="Q21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.0969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.4234693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2966,7 +2933,7 @@
       </c>
       <c r="Y4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Finalizada/Corregida")</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="Z4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "En proceso")</f>
@@ -2974,11 +2941,11 @@
       </c>
       <c r="AA4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Sin empezar")</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AB4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Pendiente de correción")</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AC4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Aplazada")</f>
@@ -3063,7 +3030,7 @@
       </c>
       <c r="Y5" s="0" t="n">
         <f aca="false">Y4/AD4 *100</f>
-        <v>16.6666666666667</v>
+        <v>28.5714285714286</v>
       </c>
       <c r="Z5" s="0" t="n">
         <f aca="false">Z4/AD4 *100</f>
@@ -3071,11 +3038,11 @@
       </c>
       <c r="AA5" s="0" t="n">
         <f aca="false">AA4/AD4 *100</f>
-        <v>52.3809523809524</v>
+        <v>50</v>
       </c>
       <c r="AB5" s="0" t="n">
         <f aca="false">AB4/AD4*100</f>
-        <v>16.6666666666667</v>
+        <v>7.14285714285714</v>
       </c>
       <c r="AC5" s="0" t="n">
         <f aca="false">AC4/AD4 *100</f>
@@ -3090,7 +3057,7 @@
       <c r="A6" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -3536,7 +3503,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="31.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="n">
         <v>17</v>
       </c>
@@ -3544,7 +3511,7 @@
         <v>109</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="8" t="n">
@@ -3557,15 +3524,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="n">
         <v>18</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="8" t="n">
@@ -3578,15 +3545,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="31.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="n">
         <v>19</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="8" t="n">
@@ -3599,15 +3566,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="31.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="n">
         <v>20</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="8" t="n">
@@ -3620,15 +3587,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="n">
         <v>21</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="8" t="n">
@@ -3637,14 +3604,16 @@
       <c r="F24" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="G24" s="8"/>
+      <c r="G24" s="8" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="n">
         <v>22</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>94</v>
@@ -3663,13 +3632,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>116</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="E26" s="8" t="n">
         <v>30</v>
@@ -3686,7 +3655,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>27</v>
@@ -3707,7 +3676,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>94</v>
@@ -3726,7 +3695,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>94</v>
@@ -3745,7 +3714,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>94</v>
@@ -3764,7 +3733,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>94</v>
@@ -3783,7 +3752,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>94</v>
@@ -3802,7 +3771,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>94</v>
@@ -3821,7 +3790,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>94</v>
@@ -3840,10 +3809,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>127</v>
@@ -3921,7 +3890,7 @@
         <v>131</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="E39" s="8" t="n">
         <v>120</v>
@@ -3992,7 +3961,7 @@
         <v>135</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>136</v>
@@ -4122,14 +4091,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="61.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="20.25"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="61.1530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4936,7 +4905,7 @@
       <c r="A39" s="6" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C39" s="10" t="s">
@@ -4973,7 +4942,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>94</v>
@@ -5333,7 +5302,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>94</v>
@@ -5351,7 +5320,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>94</v>
@@ -5369,7 +5338,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>94</v>
@@ -5387,7 +5356,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>94</v>
@@ -5405,7 +5374,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>94</v>
@@ -5423,7 +5392,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>94</v>
@@ -6444,8 +6413,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6475,7 +6444,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizado EXCEL, se tuvo que añadir el atributo PorcentajeNota de TRABAJO en vistas,controaldores y modelos
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="212">
   <si>
     <t>Semana 1(Del 20/11/2017 hasta 26/11/2017)</t>
   </si>
@@ -407,22 +407,25 @@
     <t>Gestión de trabajos: realizar las vistas, controladores y  modelos de la tabla TRABAJO.</t>
   </si>
   <si>
+    <t>Creados los elementos correspondientes según la guía de nombres</t>
+  </si>
+  <si>
+    <t>Revisión y corrección de las tarea 34.</t>
+  </si>
+  <si>
+    <t>Inserte el aributo PorcentajeNota en todo ya que falta en las vistas,controlador y modelo.</t>
+  </si>
+  <si>
+    <t>Gestión de historias: realizar las vistas, controladores y  modelos de la tabla HISTORIA.</t>
+  </si>
+  <si>
+    <t>Revisión y corrección de la tarea 36.</t>
+  </si>
+  <si>
+    <t>Gestión evaluación: realizar las vistas, controladores y  modelos de la tabla EVALUACIÓN.</t>
+  </si>
+  <si>
     <t>Pendiente de correción</t>
-  </si>
-  <si>
-    <t>Creados los elementos correspondientes según la guía de nombres</t>
-  </si>
-  <si>
-    <t>Revisión y corrección de las tarea 34.</t>
-  </si>
-  <si>
-    <t>Gestión de historias: realizar las vistas, controladores y  modelos de la tabla HISTORIA.</t>
-  </si>
-  <si>
-    <t>Revisión y corrección de la tarea 36.</t>
-  </si>
-  <si>
-    <t>Gestión evaluación: realizar las vistas, controladores y  modelos de la tabla EVALUACIÓN.</t>
   </si>
   <si>
     <t>Revisión y corrección de la tarea 38</t>
@@ -1206,32 +1209,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="81.8061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.6632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.2602040816326"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2751,18 +2754,16 @@
   </sheetPr>
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.4234693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.7448979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2933,7 +2934,7 @@
       </c>
       <c r="Y4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Finalizada/Corregida")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Z4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "En proceso")</f>
@@ -2941,11 +2942,11 @@
       </c>
       <c r="AA4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Sin empezar")</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AB4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Pendiente de correción")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Aplazada")</f>
@@ -3030,7 +3031,7 @@
       </c>
       <c r="Y5" s="0" t="n">
         <f aca="false">Y4/AD4 *100</f>
-        <v>28.5714285714286</v>
+        <v>33.3333333333333</v>
       </c>
       <c r="Z5" s="0" t="n">
         <f aca="false">Z4/AD4 *100</f>
@@ -3038,11 +3039,11 @@
       </c>
       <c r="AA5" s="0" t="n">
         <f aca="false">AA4/AD4 *100</f>
-        <v>50</v>
+        <v>47.6190476190476</v>
       </c>
       <c r="AB5" s="0" t="n">
         <f aca="false">AB4/AD4*100</f>
-        <v>7.14285714285714</v>
+        <v>4.76190476190476</v>
       </c>
       <c r="AC5" s="0" t="n">
         <f aca="false">AC4/AD4 *100</f>
@@ -3804,7 +3805,7 @@
       </c>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="31.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="n">
         <v>34</v>
       </c>
@@ -3812,10 +3813,10 @@
         <v>125</v>
       </c>
       <c r="C35" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>126</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="E35" s="8" t="n">
         <v>120</v>
@@ -3827,24 +3828,28 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" s="11"/>
       <c r="E36" s="8" t="n">
         <v>30</v>
       </c>
       <c r="F36" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="G36" s="8"/>
+      <c r="G36" s="8" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="n">
@@ -3890,7 +3895,7 @@
         <v>131</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E39" s="8" t="n">
         <v>120</v>
@@ -3907,7 +3912,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>94</v>
@@ -3924,7 +3929,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>94</v>
@@ -3941,7 +3946,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>94</v>
@@ -3958,13 +3963,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E43" s="8" t="n">
         <v>90</v>
@@ -3981,7 +3986,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>94</v>
@@ -3998,7 +4003,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>94</v>
@@ -4091,14 +4096,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="61.1530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="60.4744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.6377551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4127,10 +4130,10 @@
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
       <c r="I2" s="34" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>19</v>
@@ -4151,7 +4154,7 @@
         <v>24</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4333,7 +4336,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>27</v>
@@ -4369,7 +4372,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>27</v>
@@ -4387,7 +4390,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>37</v>
@@ -4405,7 +4408,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>37</v>
@@ -4423,7 +4426,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>27</v>
@@ -4441,7 +4444,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>27</v>
@@ -4459,7 +4462,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>27</v>
@@ -4477,7 +4480,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>27</v>
@@ -4495,7 +4498,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>27</v>
@@ -4513,7 +4516,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>94</v>
@@ -4531,7 +4534,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>27</v>
@@ -4549,7 +4552,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>27</v>
@@ -4585,7 +4588,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>27</v>
@@ -4603,7 +4606,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>27</v>
@@ -4621,7 +4624,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>27</v>
@@ -4691,7 +4694,7 @@
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4719,7 +4722,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>27</v>
@@ -4739,7 +4742,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>27</v>
@@ -4759,7 +4762,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>94</v>
@@ -4834,7 +4837,7 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="J35" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4842,7 +4845,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>27</v>
@@ -4858,7 +4861,7 @@
       <c r="G36" s="37"/>
       <c r="H36" s="34"/>
       <c r="I36" s="39" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J36" s="0" t="n">
         <f aca="false">SUM(E37:E76)</f>
@@ -4927,7 +4930,7 @@
         <v>99</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D40" s="6" t="str">
         <f aca="false">IF(C40 = "Finalizada/Corregida","100%","")</f>
@@ -4996,7 +4999,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>37</v>
@@ -5068,7 +5071,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>94</v>
@@ -5086,7 +5089,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>94</v>
@@ -5104,7 +5107,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>94</v>
@@ -5212,7 +5215,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>94</v>
@@ -5230,7 +5233,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>94</v>
@@ -5248,7 +5251,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>94</v>
@@ -5266,7 +5269,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>94</v>
@@ -5284,7 +5287,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>94</v>
@@ -5410,7 +5413,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>94</v>
@@ -5446,7 +5449,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>94</v>
@@ -5482,7 +5485,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>94</v>
@@ -5500,7 +5503,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>94</v>
@@ -5518,7 +5521,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>94</v>
@@ -5536,7 +5539,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>94</v>
@@ -5554,7 +5557,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>94</v>
@@ -5572,7 +5575,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="40" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C76" s="28" t="s">
         <v>94</v>
@@ -5588,10 +5591,10 @@
       <c r="G76" s="34"/>
       <c r="H76" s="34"/>
       <c r="I76" s="34" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5599,7 +5602,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="41" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>94</v>
@@ -5625,7 +5628,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="44" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>94</v>
@@ -5647,7 +5650,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>94</v>
@@ -5669,7 +5672,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>94</v>
@@ -5689,7 +5692,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>94</v>
@@ -5707,7 +5710,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="31" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>94</v>
@@ -5725,7 +5728,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>94</v>
@@ -5743,7 +5746,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>94</v>
@@ -5761,7 +5764,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="31" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>94</v>
@@ -5779,7 +5782,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>94</v>
@@ -5797,7 +5800,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>94</v>
@@ -5815,7 +5818,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="40" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C88" s="28" t="s">
         <v>94</v>
@@ -5831,10 +5834,10 @@
       <c r="G88" s="34"/>
       <c r="H88" s="34"/>
       <c r="I88" s="34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5842,7 +5845,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="41" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>94</v>
@@ -5864,7 +5867,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="44" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>94</v>
@@ -5882,7 +5885,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="45" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>94</v>
@@ -5900,7 +5903,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="45" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>94</v>
@@ -5918,7 +5921,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="45" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>94</v>
@@ -5936,7 +5939,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="45" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>94</v>
@@ -5954,7 +5957,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="45" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>94</v>
@@ -5972,7 +5975,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="45" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>94</v>
@@ -5990,7 +5993,7 @@
         <v>49</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>94</v>
@@ -6026,7 +6029,7 @@
         <v>95</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C99" s="28" t="s">
         <v>94</v>
@@ -6042,10 +6045,10 @@
       <c r="G99" s="34"/>
       <c r="H99" s="34"/>
       <c r="I99" s="34" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J99" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6053,7 +6056,7 @@
         <v>96</v>
       </c>
       <c r="B100" s="41" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>94</v>
@@ -6075,7 +6078,7 @@
         <v>97</v>
       </c>
       <c r="B101" s="44" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>94</v>
@@ -6093,7 +6096,7 @@
         <v>98</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C102" s="10" t="s">
         <v>94</v>
@@ -6111,7 +6114,7 @@
         <v>99</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>94</v>
@@ -6129,7 +6132,7 @@
         <v>100</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>94</v>
@@ -6147,7 +6150,7 @@
         <v>101</v>
       </c>
       <c r="B105" s="31" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>94</v>
@@ -6165,7 +6168,7 @@
         <v>102</v>
       </c>
       <c r="B106" s="31" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>94</v>
@@ -6183,7 +6186,7 @@
         <v>103</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>94</v>
@@ -6201,7 +6204,7 @@
         <v>104</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>94</v>
@@ -6219,7 +6222,7 @@
         <v>105</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C109" s="10" t="s">
         <v>94</v>
@@ -6237,7 +6240,7 @@
         <v>106</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>94</v>
@@ -6255,7 +6258,7 @@
         <v>107</v>
       </c>
       <c r="B111" s="45" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C111" s="10" t="s">
         <v>94</v>
@@ -6413,8 +6416,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6424,7 +6427,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6439,12 +6442,12 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel cambiado y revision de trabajo echo
</commit_message>
<xml_diff>
--- a/EXCEL TAREAS/Seguimiento et3.xlsx
+++ b/EXCEL TAREAS/Seguimiento et3.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="213">
   <si>
     <t>Semana 1(Del 20/11/2017 hasta 26/11/2017)</t>
   </si>
@@ -425,19 +425,22 @@
     <t>Gestión evaluación: realizar las vistas, controladores y  modelos de la tabla EVALUACIÓN.</t>
   </si>
   <si>
+    <t>Revisión y corrección de la tarea 38</t>
+  </si>
+  <si>
+    <t>Casi todo mal, los size y maxlenght mal puestos,ningun textarea,fallos en algun nombre…</t>
+  </si>
+  <si>
+    <t>Gestión de la asignación automática de QAs: realizar una primera versión con los archivos necesarios para su tratamiento (vistas, controladores, modelos).</t>
+  </si>
+  <si>
+    <t>Revisión y corrección de la tarea 41 </t>
+  </si>
+  <si>
+    <t>Gestión de la entregas: realizar una primera versión con los archivos necesarios para su tratamiento (vistas, controladores, modelos).</t>
+  </si>
+  <si>
     <t>Pendiente de correción</t>
-  </si>
-  <si>
-    <t>Revisión y corrección de la tarea 38</t>
-  </si>
-  <si>
-    <t>Gestión de la asignación automática de QAs: realizar una primera versión con los archivos necesarios para su tratamiento (vistas, controladores, modelos).</t>
-  </si>
-  <si>
-    <t>Revisión y corrección de la tarea 41 </t>
-  </si>
-  <si>
-    <t>Gestión de la entregas: realizar una primera versión con los archivos necesarios para su tratamiento (vistas, controladores, modelos).</t>
   </si>
   <si>
     <t>Nombre del modelo:ENTREGA_MODEL,Nombre del controlador ENTREGA_CONTROLLER y nombre de las vistas empiezan por ENTREGA</t>
@@ -1209,32 +1212,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.9132653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2754,16 +2753,18 @@
   </sheetPr>
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G37" activeCellId="0" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.7448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.9387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2934,7 +2935,7 @@
       </c>
       <c r="Y4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Finalizada/Corregida")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Z4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "En proceso")</f>
@@ -2942,11 +2943,11 @@
       </c>
       <c r="AA4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Sin empezar")</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AB4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Pendiente de correción")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC4" s="0" t="n">
         <f aca="false">COUNTIF(C:C, "Aplazada")</f>
@@ -3031,7 +3032,7 @@
       </c>
       <c r="Y5" s="0" t="n">
         <f aca="false">Y4/AD4 *100</f>
-        <v>33.3333333333333</v>
+        <v>38.0952380952381</v>
       </c>
       <c r="Z5" s="0" t="n">
         <f aca="false">Z4/AD4 *100</f>
@@ -3039,11 +3040,11 @@
       </c>
       <c r="AA5" s="0" t="n">
         <f aca="false">AA4/AD4 *100</f>
-        <v>47.6190476190476</v>
+        <v>45.2380952380952</v>
       </c>
       <c r="AB5" s="0" t="n">
         <f aca="false">AB4/AD4*100</f>
-        <v>4.76190476190476</v>
+        <v>2.38095238095238</v>
       </c>
       <c r="AC5" s="0" t="n">
         <f aca="false">AC4/AD4 *100</f>
@@ -3848,7 +3849,7 @@
         <v>4</v>
       </c>
       <c r="G36" s="8" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3887,7 +3888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="n">
         <v>38</v>
       </c>
@@ -3895,7 +3896,7 @@
         <v>131</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="E39" s="8" t="n">
         <v>120</v>
@@ -3907,21 +3908,27 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>133</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>94</v>
       </c>
       <c r="E40" s="8" t="n">
         <v>30</v>
       </c>
       <c r="F40" s="8" t="n">
         <v>4</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3966,10 +3973,10 @@
         <v>136</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E43" s="8" t="n">
         <v>90</v>
@@ -3978,7 +3985,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3986,7 +3993,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>94</v>
@@ -4003,7 +4010,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>94</v>
@@ -4096,12 +4103,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="60.4744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="59.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4130,10 +4139,10 @@
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
       <c r="I2" s="34" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>19</v>
@@ -4154,7 +4163,7 @@
         <v>24</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4336,7 +4345,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>27</v>
@@ -4372,7 +4381,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>27</v>
@@ -4390,7 +4399,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>37</v>
@@ -4408,7 +4417,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>37</v>
@@ -4426,7 +4435,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>27</v>
@@ -4444,7 +4453,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>27</v>
@@ -4462,7 +4471,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>27</v>
@@ -4480,7 +4489,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>27</v>
@@ -4498,7 +4507,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>27</v>
@@ -4516,7 +4525,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>94</v>
@@ -4534,7 +4543,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>27</v>
@@ -4552,7 +4561,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>27</v>
@@ -4588,7 +4597,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>27</v>
@@ -4606,7 +4615,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>27</v>
@@ -4624,7 +4633,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>27</v>
@@ -4694,7 +4703,7 @@
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4722,7 +4731,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>27</v>
@@ -4742,7 +4751,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>27</v>
@@ -4762,7 +4771,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>94</v>
@@ -4837,7 +4846,7 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="J35" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4845,7 +4854,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>27</v>
@@ -4861,7 +4870,7 @@
       <c r="G36" s="37"/>
       <c r="H36" s="34"/>
       <c r="I36" s="39" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J36" s="0" t="n">
         <f aca="false">SUM(E37:E76)</f>
@@ -4930,7 +4939,7 @@
         <v>99</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D40" s="6" t="str">
         <f aca="false">IF(C40 = "Finalizada/Corregida","100%","")</f>
@@ -4999,7 +5008,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>37</v>
@@ -5071,7 +5080,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>94</v>
@@ -5089,7 +5098,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>94</v>
@@ -5107,7 +5116,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>94</v>
@@ -5215,7 +5224,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>94</v>
@@ -5233,7 +5242,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>94</v>
@@ -5251,7 +5260,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>94</v>
@@ -5269,7 +5278,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>94</v>
@@ -5287,7 +5296,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>94</v>
@@ -5413,7 +5422,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>94</v>
@@ -5449,7 +5458,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>94</v>
@@ -5485,7 +5494,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>94</v>
@@ -5503,7 +5512,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>94</v>
@@ -5521,7 +5530,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>94</v>
@@ -5539,7 +5548,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>94</v>
@@ -5557,7 +5566,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>94</v>
@@ -5575,7 +5584,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="40" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C76" s="28" t="s">
         <v>94</v>
@@ -5591,10 +5600,10 @@
       <c r="G76" s="34"/>
       <c r="H76" s="34"/>
       <c r="I76" s="34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5602,7 +5611,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="41" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>94</v>
@@ -5628,7 +5637,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="44" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>94</v>
@@ -5650,7 +5659,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>94</v>
@@ -5672,7 +5681,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>94</v>
@@ -5692,7 +5701,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>94</v>
@@ -5710,7 +5719,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>94</v>
@@ -5728,7 +5737,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>94</v>
@@ -5746,7 +5755,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>94</v>
@@ -5764,7 +5773,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="31" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>94</v>
@@ -5782,7 +5791,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>94</v>
@@ -5800,7 +5809,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>94</v>
@@ -5818,7 +5827,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="40" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C88" s="28" t="s">
         <v>94</v>
@@ -5834,10 +5843,10 @@
       <c r="G88" s="34"/>
       <c r="H88" s="34"/>
       <c r="I88" s="34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5845,7 +5854,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="41" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>94</v>
@@ -5867,7 +5876,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="44" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>94</v>
@@ -5885,7 +5894,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="45" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>94</v>
@@ -5903,7 +5912,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="45" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>94</v>
@@ -5921,7 +5930,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="45" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>94</v>
@@ -5939,7 +5948,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="45" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>94</v>
@@ -5957,7 +5966,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="45" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>94</v>
@@ -5975,7 +5984,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="45" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>94</v>
@@ -5993,7 +6002,7 @@
         <v>49</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>94</v>
@@ -6029,7 +6038,7 @@
         <v>95</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C99" s="28" t="s">
         <v>94</v>
@@ -6045,10 +6054,10 @@
       <c r="G99" s="34"/>
       <c r="H99" s="34"/>
       <c r="I99" s="34" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J99" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6056,7 +6065,7 @@
         <v>96</v>
       </c>
       <c r="B100" s="41" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>94</v>
@@ -6078,7 +6087,7 @@
         <v>97</v>
       </c>
       <c r="B101" s="44" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>94</v>
@@ -6096,7 +6105,7 @@
         <v>98</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C102" s="10" t="s">
         <v>94</v>
@@ -6114,7 +6123,7 @@
         <v>99</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>94</v>
@@ -6132,7 +6141,7 @@
         <v>100</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>94</v>
@@ -6150,7 +6159,7 @@
         <v>101</v>
       </c>
       <c r="B105" s="31" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>94</v>
@@ -6168,7 +6177,7 @@
         <v>102</v>
       </c>
       <c r="B106" s="31" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>94</v>
@@ -6186,7 +6195,7 @@
         <v>103</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>94</v>
@@ -6204,7 +6213,7 @@
         <v>104</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>94</v>
@@ -6222,7 +6231,7 @@
         <v>105</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C109" s="10" t="s">
         <v>94</v>
@@ -6240,7 +6249,7 @@
         <v>106</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>94</v>
@@ -6258,7 +6267,7 @@
         <v>107</v>
       </c>
       <c r="B111" s="45" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C111" s="10" t="s">
         <v>94</v>
@@ -6416,8 +6425,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6427,7 +6435,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6442,12 +6450,12 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>